<commit_message>
linux changes to biol file mum 20180531 for base run
</commit_message>
<xml_diff>
--- a/R/C_and_Mum.xlsx
+++ b/R/C_and_Mum.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="7"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="C_v1" sheetId="1" state="visible" r:id="rId2"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1447" uniqueCount="336">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1475" uniqueCount="337">
   <si>
     <t xml:space="preserve">FPL</t>
   </si>
@@ -864,6 +864,9 @@
   </si>
   <si>
     <t xml:space="preserve">20180510a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">linux</t>
   </si>
   <si>
     <t xml:space="preserve">C_LSQ_T15</t>
@@ -1145,9 +1148,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="30.5102040816327"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="30.2397959183673"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3132,7 +3135,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6442,7 +6445,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9752,14 +9755,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="5.12755102040816"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="31.0459183673469"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.7091836734694"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="1.88775510204082"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="2.83673469387755"/>
-    <col collapsed="false" hidden="false" max="16" min="7" style="0" width="8.77551020408163"/>
-    <col collapsed="false" hidden="false" max="1025" min="17" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="4.99489795918367"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="30.6428571428571"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="1.75510204081633"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="2.69897959183673"/>
+    <col collapsed="false" hidden="false" max="16" min="7" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="17" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13074,14 +13077,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="5.12755102040816"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="31.0459183673469"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.7091836734694"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="1.88775510204082"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="2.83673469387755"/>
-    <col collapsed="false" hidden="false" max="16" min="7" style="0" width="11.7448979591837"/>
-    <col collapsed="false" hidden="false" max="1025" min="17" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="4.99489795918367"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="30.6428571428571"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="1.75510204081633"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="2.69897959183673"/>
+    <col collapsed="false" hidden="false" max="16" min="7" style="0" width="11.4744897959184"/>
+    <col collapsed="false" hidden="false" max="1025" min="17" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16396,9 +16399,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="30.5102040816327"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="30.2397959183673"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18405,15 +18408,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H28"/>
+  <dimension ref="A1:G56"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E27" activeCellId="0" sqref="E27"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G5" activeCellId="0" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18426,10 +18429,18 @@
       <c r="D1" s="0" t="s">
         <v>278</v>
       </c>
+      <c r="E1" s="0" t="n">
+        <v>20180531</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E2" s="0" t="s">
+        <v>279</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>0.001455</v>
@@ -18440,10 +18451,13 @@
       <c r="D3" s="0" t="n">
         <v>0.0001455</v>
       </c>
+      <c r="E3" s="0" t="n">
+        <v>0.001455</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>0.001</v>
@@ -18454,10 +18468,13 @@
       <c r="D4" s="0" t="n">
         <v>0.0001</v>
       </c>
+      <c r="E4" s="0" t="n">
+        <v>0.001</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>0.001455</v>
@@ -18468,10 +18485,13 @@
       <c r="D5" s="0" t="n">
         <v>0.0001455</v>
       </c>
+      <c r="E5" s="0" t="n">
+        <v>0.001455</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>0.001</v>
@@ -18482,10 +18502,13 @@
       <c r="D6" s="0" t="n">
         <v>0.0001</v>
       </c>
+      <c r="E6" s="0" t="n">
+        <v>0.001</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>0.02</v>
@@ -18496,10 +18519,13 @@
       <c r="D7" s="0" t="n">
         <v>0.0002</v>
       </c>
+      <c r="E7" s="0" t="n">
+        <v>0.002</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>0.02</v>
@@ -18510,10 +18536,13 @@
       <c r="D8" s="0" t="n">
         <v>0.0002</v>
       </c>
+      <c r="E8" s="0" t="n">
+        <v>0.002</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>0.02</v>
@@ -18524,11 +18553,14 @@
       <c r="D9" s="0" t="n">
         <v>0.0002</v>
       </c>
-      <c r="H9" s="1"/>
+      <c r="E9" s="0" t="n">
+        <v>0.002</v>
+      </c>
+      <c r="G9" s="1"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="B10" s="1" t="n">
         <v>7E-005</v>
@@ -18539,10 +18571,13 @@
       <c r="D10" s="1" t="n">
         <v>7E-005</v>
       </c>
+      <c r="E10" s="1" t="n">
+        <v>0.0007</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="B11" s="1" t="n">
         <v>5E-005</v>
@@ -18553,11 +18588,13 @@
       <c r="D11" s="1" t="n">
         <v>5E-006</v>
       </c>
-      <c r="E11" s="1"/>
+      <c r="E11" s="1" t="n">
+        <v>0.0005</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B12" s="1" t="n">
         <v>6.5E-005</v>
@@ -18568,11 +18605,14 @@
       <c r="D12" s="1" t="n">
         <v>6.5E-005</v>
       </c>
-      <c r="H12" s="1"/>
+      <c r="E12" s="1" t="n">
+        <v>0.00065</v>
+      </c>
+      <c r="G12" s="1"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="B13" s="1" t="n">
         <v>0.005</v>
@@ -18583,11 +18623,13 @@
       <c r="D13" s="1" t="n">
         <v>0.0005</v>
       </c>
-      <c r="F13" s="1"/>
+      <c r="E13" s="1" t="n">
+        <v>0.0005</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="B14" s="1" t="n">
         <v>5E-005</v>
@@ -18598,10 +18640,13 @@
       <c r="D14" s="1" t="n">
         <v>5E-006</v>
       </c>
+      <c r="E14" s="1" t="n">
+        <v>5E-006</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>0.0015</v>
@@ -18612,10 +18657,13 @@
       <c r="D15" s="0" t="n">
         <v>0.00015</v>
       </c>
+      <c r="E15" s="0" t="n">
+        <v>0.00015</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B16" s="0" t="n">
         <v>0.001</v>
@@ -18626,10 +18674,13 @@
       <c r="D16" s="0" t="n">
         <v>0.0001</v>
       </c>
+      <c r="E16" s="0" t="n">
+        <v>0.0001</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="B17" s="0" t="n">
         <v>0.0015</v>
@@ -18640,10 +18691,13 @@
       <c r="D17" s="0" t="n">
         <v>0.00015</v>
       </c>
+      <c r="E17" s="0" t="n">
+        <v>0.00015</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="B18" s="0" t="n">
         <v>0.001</v>
@@ -18654,10 +18708,13 @@
       <c r="D18" s="0" t="n">
         <v>0.0001</v>
       </c>
+      <c r="E18" s="0" t="n">
+        <v>0.0001</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="B19" s="0" t="n">
         <v>0.002</v>
@@ -18668,11 +18725,13 @@
       <c r="D19" s="0" t="n">
         <v>0.0002</v>
       </c>
-      <c r="F19" s="1"/>
+      <c r="E19" s="0" t="n">
+        <v>0.002</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="B20" s="1" t="n">
         <v>0.0005</v>
@@ -18683,10 +18742,13 @@
       <c r="D20" s="1" t="n">
         <v>5E-005</v>
       </c>
+      <c r="E20" s="1" t="n">
+        <v>0.0005</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="B21" s="0" t="n">
         <v>0.003</v>
@@ -18697,10 +18759,13 @@
       <c r="D21" s="0" t="n">
         <v>0.0003</v>
       </c>
+      <c r="E21" s="0" t="n">
+        <v>0.0003</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="B22" s="0" t="n">
         <v>0.01</v>
@@ -18711,10 +18776,13 @@
       <c r="D22" s="0" t="n">
         <v>0.0001</v>
       </c>
+      <c r="E22" s="0" t="n">
+        <v>0.0001</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="B23" s="0" t="n">
         <v>0.008</v>
@@ -18725,10 +18793,13 @@
       <c r="D23" s="0" t="n">
         <v>0.0008</v>
       </c>
+      <c r="E23" s="0" t="n">
+        <v>0.008</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="B24" s="0" t="n">
         <v>0.15</v>
@@ -18739,10 +18810,13 @@
       <c r="D24" s="0" t="n">
         <v>0.0015</v>
       </c>
+      <c r="E24" s="0" t="n">
+        <v>0.0015</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="B25" s="0" t="n">
         <v>0</v>
@@ -18753,10 +18827,13 @@
       <c r="D25" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="E25" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="B26" s="0" t="n">
         <v>0</v>
@@ -18767,10 +18844,13 @@
       <c r="D26" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="E26" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="B27" s="0" t="n">
         <v>0.0001</v>
@@ -18781,10 +18861,13 @@
       <c r="D27" s="0" t="n">
         <v>1E-005</v>
       </c>
+      <c r="E27" s="0" t="n">
+        <v>0.0001</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="B28" s="0" t="n">
         <v>0.006</v>
@@ -18793,6 +18876,217 @@
         <v>0.0006</v>
       </c>
       <c r="D28" s="0" t="n">
+        <v>0.0006</v>
+      </c>
+      <c r="E28" s="0" t="n">
+        <v>0.0006</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="s">
+        <v>280</v>
+      </c>
+      <c r="B31" s="0" t="n">
+        <v>0.001455</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="s">
+        <v>281</v>
+      </c>
+      <c r="B32" s="0" t="n">
+        <v>0.001</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
+        <v>282</v>
+      </c>
+      <c r="B33" s="0" t="n">
+        <v>0.001455</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
+        <v>283</v>
+      </c>
+      <c r="B34" s="0" t="n">
+        <v>0.001</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="s">
+        <v>284</v>
+      </c>
+      <c r="B35" s="0" t="n">
+        <v>0.002</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="s">
+        <v>285</v>
+      </c>
+      <c r="B36" s="0" t="n">
+        <v>0.002</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="s">
+        <v>286</v>
+      </c>
+      <c r="B37" s="0" t="n">
+        <v>0.002</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="s">
+        <v>287</v>
+      </c>
+      <c r="B38" s="1" t="n">
+        <v>0.0007</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="s">
+        <v>288</v>
+      </c>
+      <c r="B39" s="1" t="n">
+        <v>0.0005</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0" t="s">
+        <v>289</v>
+      </c>
+      <c r="B40" s="1" t="n">
+        <v>0.00065</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0" t="s">
+        <v>290</v>
+      </c>
+      <c r="B41" s="1" t="n">
+        <v>0.0005</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="s">
+        <v>291</v>
+      </c>
+      <c r="B42" s="1" t="n">
+        <v>5E-006</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0" t="s">
+        <v>292</v>
+      </c>
+      <c r="B43" s="0" t="n">
+        <v>0.00015</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="0" t="s">
+        <v>293</v>
+      </c>
+      <c r="B44" s="0" t="n">
+        <v>0.0001</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0" t="s">
+        <v>294</v>
+      </c>
+      <c r="B45" s="0" t="n">
+        <v>0.00015</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="0" t="s">
+        <v>295</v>
+      </c>
+      <c r="B46" s="0" t="n">
+        <v>0.0001</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="0" t="s">
+        <v>296</v>
+      </c>
+      <c r="B47" s="0" t="n">
+        <v>0.002</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="0" t="s">
+        <v>297</v>
+      </c>
+      <c r="B48" s="1" t="n">
+        <v>0.0005</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="0" t="s">
+        <v>298</v>
+      </c>
+      <c r="B49" s="0" t="n">
+        <v>0.0003</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="0" t="s">
+        <v>299</v>
+      </c>
+      <c r="B50" s="0" t="n">
+        <v>0.0001</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="0" t="s">
+        <v>300</v>
+      </c>
+      <c r="B51" s="0" t="n">
+        <v>0.008</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="0" t="s">
+        <v>301</v>
+      </c>
+      <c r="B52" s="0" t="n">
+        <v>0.0015</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="0" t="s">
+        <v>302</v>
+      </c>
+      <c r="B53" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="0" t="s">
+        <v>303</v>
+      </c>
+      <c r="B54" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="0" t="s">
+        <v>304</v>
+      </c>
+      <c r="B55" s="0" t="n">
+        <v>0.0001</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="0" t="s">
+        <v>305</v>
+      </c>
+      <c r="B56" s="0" t="n">
         <v>0.0006</v>
       </c>
     </row>
@@ -18806,7 +19100,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{485BCDED-369D-4FE7-AB63-83726573E2B5}</x14:id>
+          <x14:id>{27B61ABC-2AD7-4758-AB4E-C3B7BB64A6C3}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -18822,7 +19116,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{485BCDED-369D-4FE7-AB63-83726573E2B5}">
+          <x14:cfRule type="dataBar" id="{27B61ABC-2AD7-4758-AB4E-C3B7BB64A6C3}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="true">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -18843,16 +19137,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D33"/>
+  <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F8" activeCellId="0" sqref="F8"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F5" activeCellId="0" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.0459183673469"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.7142857142857"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18865,10 +19159,18 @@
       <c r="D1" s="0" t="s">
         <v>278</v>
       </c>
+      <c r="E1" s="0" t="n">
+        <v>20180531</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E2" s="0" t="s">
+        <v>279</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>0.0044</v>
@@ -18879,10 +19181,13 @@
       <c r="D3" s="0" t="n">
         <v>0.0044</v>
       </c>
+      <c r="E3" s="0" t="n">
+        <v>0.044</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>0.004</v>
@@ -18893,10 +19198,13 @@
       <c r="D4" s="0" t="n">
         <v>0.004</v>
       </c>
+      <c r="E4" s="0" t="n">
+        <v>0.04</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>0.00444</v>
@@ -18907,10 +19215,13 @@
       <c r="D5" s="0" t="n">
         <v>0.00444</v>
       </c>
+      <c r="E5" s="0" t="n">
+        <v>0.0444</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>0.004</v>
@@ -18921,10 +19232,13 @@
       <c r="D6" s="0" t="n">
         <v>0.004</v>
       </c>
+      <c r="E6" s="0" t="n">
+        <v>0.04</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>0.05</v>
@@ -18935,10 +19249,13 @@
       <c r="D7" s="0" t="n">
         <v>0.005</v>
       </c>
+      <c r="E7" s="0" t="n">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>0.05</v>
@@ -18949,10 +19266,13 @@
       <c r="D8" s="0" t="n">
         <v>0.005</v>
       </c>
+      <c r="E8" s="0" t="n">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>0.05</v>
@@ -18963,10 +19283,13 @@
       <c r="D9" s="0" t="n">
         <v>0.005</v>
       </c>
+      <c r="E9" s="0" t="n">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>0.0035</v>
@@ -18977,10 +19300,13 @@
       <c r="D10" s="0" t="n">
         <v>0.0035</v>
       </c>
+      <c r="E10" s="0" t="n">
+        <v>0.0035</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>0.0002</v>
@@ -18991,10 +19317,13 @@
       <c r="D11" s="0" t="n">
         <v>0.0002</v>
       </c>
+      <c r="E11" s="0" t="n">
+        <v>0.0002</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>0.0012</v>
@@ -19005,10 +19334,13 @@
       <c r="D12" s="0" t="n">
         <v>0.0012</v>
       </c>
+      <c r="E12" s="0" t="n">
+        <v>0.012</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="B13" s="1" t="n">
         <v>0.001</v>
@@ -19019,10 +19351,13 @@
       <c r="D13" s="1" t="n">
         <v>0.001</v>
       </c>
+      <c r="E13" s="1" t="n">
+        <v>0.01</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="B14" s="1" t="n">
         <v>0.001</v>
@@ -19033,10 +19368,13 @@
       <c r="D14" s="1" t="n">
         <v>0.001</v>
       </c>
+      <c r="E14" s="1" t="n">
+        <v>0.001</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>0.003043</v>
@@ -19047,10 +19385,13 @@
       <c r="D15" s="0" t="n">
         <v>0.003043</v>
       </c>
+      <c r="E15" s="0" t="n">
+        <v>0.003043</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="B16" s="0" t="n">
         <v>0.003</v>
@@ -19061,10 +19402,13 @@
       <c r="D16" s="0" t="n">
         <v>0.003</v>
       </c>
+      <c r="E16" s="0" t="n">
+        <v>0.003</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="B17" s="0" t="n">
         <v>0.003043</v>
@@ -19075,10 +19419,13 @@
       <c r="D17" s="0" t="n">
         <v>0.003043</v>
       </c>
+      <c r="E17" s="0" t="n">
+        <v>0.003043</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="B18" s="0" t="n">
         <v>0.003</v>
@@ -19089,10 +19436,13 @@
       <c r="D18" s="0" t="n">
         <v>0.003</v>
       </c>
+      <c r="E18" s="0" t="n">
+        <v>0.003</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="B19" s="0" t="n">
         <v>0.005</v>
@@ -19103,10 +19453,13 @@
       <c r="D19" s="0" t="n">
         <v>0.005</v>
       </c>
+      <c r="E19" s="0" t="n">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="B20" s="0" t="n">
         <v>0.0014</v>
@@ -19117,10 +19470,13 @@
       <c r="D20" s="0" t="n">
         <v>0.0014</v>
       </c>
+      <c r="E20" s="0" t="n">
+        <v>0.0014</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="B21" s="0" t="n">
         <v>0.01</v>
@@ -19131,10 +19487,13 @@
       <c r="D21" s="0" t="n">
         <v>0.001</v>
       </c>
+      <c r="E21" s="0" t="n">
+        <v>0.001</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="B22" s="0" t="n">
         <v>0.018</v>
@@ -19145,10 +19504,13 @@
       <c r="D22" s="0" t="n">
         <v>0.018</v>
       </c>
+      <c r="E22" s="0" t="n">
+        <v>0.018</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="B23" s="0" t="n">
         <v>0.07</v>
@@ -19159,10 +19521,13 @@
       <c r="D23" s="0" t="n">
         <v>0.07</v>
       </c>
+      <c r="E23" s="0" t="n">
+        <v>0.07</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="B24" s="0" t="n">
         <v>0.08</v>
@@ -19173,10 +19538,13 @@
       <c r="D24" s="0" t="n">
         <v>0.008</v>
       </c>
+      <c r="E24" s="0" t="n">
+        <v>0.008</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="B25" s="0" t="n">
         <v>0.017</v>
@@ -19187,10 +19555,13 @@
       <c r="D25" s="0" t="n">
         <v>0.0017</v>
       </c>
+      <c r="E25" s="0" t="n">
+        <v>0.17</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="B26" s="0" t="n">
         <v>0.4</v>
@@ -19201,10 +19572,13 @@
       <c r="D26" s="0" t="n">
         <v>0.1</v>
       </c>
+      <c r="E26" s="0" t="n">
+        <v>0.4</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="B27" s="0" t="n">
         <v>0.01</v>
@@ -19215,10 +19589,13 @@
       <c r="D27" s="0" t="n">
         <v>0.001</v>
       </c>
+      <c r="E27" s="0" t="n">
+        <v>0.001</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="B28" s="0" t="n">
         <v>0.05</v>
@@ -19229,10 +19606,13 @@
       <c r="D28" s="0" t="n">
         <v>0.05</v>
       </c>
+      <c r="E28" s="0" t="n">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="B29" s="0" t="n">
         <v>0.18</v>
@@ -19243,10 +19623,13 @@
       <c r="D29" s="0" t="n">
         <v>0.0018</v>
       </c>
+      <c r="E29" s="0" t="n">
+        <v>0.018</v>
+      </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="B30" s="0" t="n">
         <v>0.55</v>
@@ -19257,10 +19640,13 @@
       <c r="D30" s="0" t="n">
         <v>0.0055</v>
       </c>
+      <c r="E30" s="0" t="n">
+        <v>0.055</v>
+      </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="B31" s="0" t="n">
         <v>0.05</v>
@@ -19271,10 +19657,13 @@
       <c r="D31" s="0" t="n">
         <v>0.0005</v>
       </c>
+      <c r="E31" s="0" t="n">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="B32" s="0" t="n">
         <v>0.02</v>
@@ -19285,10 +19674,13 @@
       <c r="D32" s="0" t="n">
         <v>0.0002</v>
       </c>
+      <c r="E32" s="0" t="n">
+        <v>0.02</v>
+      </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="B33" s="0" t="n">
         <v>0.001</v>
@@ -19297,6 +19689,9 @@
         <v>0.0001</v>
       </c>
       <c r="D33" s="0" t="n">
+        <v>0.0001</v>
+      </c>
+      <c r="E33" s="0" t="n">
         <v>0.0001</v>
       </c>
     </row>
@@ -19310,7 +19705,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{3083651F-D8CB-43B7-A11D-4E5A241D6634}</x14:id>
+          <x14:id>{65B143CF-CA16-4C43-B6F3-C68A543BC1C4}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -19326,7 +19721,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{3083651F-D8CB-43B7-A11D-4E5A241D6634}">
+          <x14:cfRule type="dataBar" id="{65B143CF-CA16-4C43-B6F3-C68A543BC1C4}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="true">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>

</xml_diff>

<commit_message>
updates to biol file for compatibility with new code
</commit_message>
<xml_diff>
--- a/R/C_and_Mum.xlsx
+++ b/R/C_and_Mum.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="6"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="988" firstSheet="0" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="C_v1" sheetId="1" state="visible" r:id="rId2"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1475" uniqueCount="337">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1508" uniqueCount="338">
   <si>
     <t xml:space="preserve">FPL</t>
   </si>
@@ -866,7 +866,10 @@
     <t xml:space="preserve">20180510a</t>
   </si>
   <si>
-    <t xml:space="preserve">linux</t>
+    <t xml:space="preserve">linux test 0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">desktop test 1</t>
   </si>
   <si>
     <t xml:space="preserve">C_LSQ_T15</t>
@@ -18410,8 +18413,8 @@
   </sheetPr>
   <dimension ref="A1:G56"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G5" activeCellId="0" sqref="G5"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A34" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -18432,15 +18435,21 @@
       <c r="E1" s="0" t="n">
         <v>20180531</v>
       </c>
+      <c r="F1" s="0" t="n">
+        <v>20180530</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E2" s="0" t="s">
         <v>279</v>
       </c>
+      <c r="F2" s="0" t="s">
+        <v>280</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>0.001455</v>
@@ -18454,10 +18463,13 @@
       <c r="E3" s="0" t="n">
         <v>0.001455</v>
       </c>
+      <c r="F3" s="0" t="n">
+        <v>0.001455</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>0.001</v>
@@ -18471,10 +18483,13 @@
       <c r="E4" s="0" t="n">
         <v>0.001</v>
       </c>
+      <c r="F4" s="0" t="n">
+        <v>0.001</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>0.001455</v>
@@ -18488,10 +18503,13 @@
       <c r="E5" s="0" t="n">
         <v>0.001455</v>
       </c>
+      <c r="F5" s="0" t="n">
+        <v>0.001455</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>0.001</v>
@@ -18505,10 +18523,13 @@
       <c r="E6" s="0" t="n">
         <v>0.001</v>
       </c>
+      <c r="F6" s="0" t="n">
+        <v>0.001</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>0.02</v>
@@ -18522,10 +18543,13 @@
       <c r="E7" s="0" t="n">
         <v>0.002</v>
       </c>
+      <c r="F7" s="0" t="n">
+        <v>0.002</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>0.02</v>
@@ -18539,10 +18563,13 @@
       <c r="E8" s="0" t="n">
         <v>0.002</v>
       </c>
+      <c r="F8" s="0" t="n">
+        <v>0.002</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>0.02</v>
@@ -18556,11 +18583,14 @@
       <c r="E9" s="0" t="n">
         <v>0.002</v>
       </c>
+      <c r="F9" s="0" t="n">
+        <v>0.002</v>
+      </c>
       <c r="G9" s="1"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="B10" s="1" t="n">
         <v>7E-005</v>
@@ -18574,10 +18604,13 @@
       <c r="E10" s="1" t="n">
         <v>0.0007</v>
       </c>
+      <c r="F10" s="1" t="n">
+        <v>0.0007</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B11" s="1" t="n">
         <v>5E-005</v>
@@ -18591,10 +18624,13 @@
       <c r="E11" s="1" t="n">
         <v>0.0005</v>
       </c>
+      <c r="F11" s="1" t="n">
+        <v>0.0005</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="B12" s="1" t="n">
         <v>6.5E-005</v>
@@ -18608,11 +18644,14 @@
       <c r="E12" s="1" t="n">
         <v>0.00065</v>
       </c>
+      <c r="F12" s="1" t="n">
+        <v>0.00065</v>
+      </c>
       <c r="G12" s="1"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="B13" s="1" t="n">
         <v>0.005</v>
@@ -18626,10 +18665,13 @@
       <c r="E13" s="1" t="n">
         <v>0.0005</v>
       </c>
+      <c r="F13" s="1" t="n">
+        <v>0.0005</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="B14" s="1" t="n">
         <v>5E-005</v>
@@ -18643,10 +18685,13 @@
       <c r="E14" s="1" t="n">
         <v>5E-006</v>
       </c>
+      <c r="F14" s="1" t="n">
+        <v>5E-006</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>0.0015</v>
@@ -18660,10 +18705,13 @@
       <c r="E15" s="0" t="n">
         <v>0.00015</v>
       </c>
+      <c r="F15" s="0" t="n">
+        <v>0.00015</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="B16" s="0" t="n">
         <v>0.001</v>
@@ -18677,10 +18725,13 @@
       <c r="E16" s="0" t="n">
         <v>0.0001</v>
       </c>
+      <c r="F16" s="0" t="n">
+        <v>0.0001</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="B17" s="0" t="n">
         <v>0.0015</v>
@@ -18694,10 +18745,13 @@
       <c r="E17" s="0" t="n">
         <v>0.00015</v>
       </c>
+      <c r="F17" s="0" t="n">
+        <v>0.00015</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="B18" s="0" t="n">
         <v>0.001</v>
@@ -18711,10 +18765,13 @@
       <c r="E18" s="0" t="n">
         <v>0.0001</v>
       </c>
+      <c r="F18" s="0" t="n">
+        <v>0.0001</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="B19" s="0" t="n">
         <v>0.002</v>
@@ -18728,10 +18785,13 @@
       <c r="E19" s="0" t="n">
         <v>0.002</v>
       </c>
+      <c r="F19" s="0" t="n">
+        <v>0.002</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="B20" s="1" t="n">
         <v>0.0005</v>
@@ -18745,10 +18805,13 @@
       <c r="E20" s="1" t="n">
         <v>0.0005</v>
       </c>
+      <c r="F20" s="1" t="n">
+        <v>0.0005</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="B21" s="0" t="n">
         <v>0.003</v>
@@ -18762,10 +18825,13 @@
       <c r="E21" s="0" t="n">
         <v>0.0003</v>
       </c>
+      <c r="F21" s="0" t="n">
+        <v>0.0003</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="B22" s="0" t="n">
         <v>0.01</v>
@@ -18779,10 +18845,13 @@
       <c r="E22" s="0" t="n">
         <v>0.0001</v>
       </c>
+      <c r="F22" s="0" t="n">
+        <v>0.0001</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="B23" s="0" t="n">
         <v>0.008</v>
@@ -18796,10 +18865,13 @@
       <c r="E23" s="0" t="n">
         <v>0.008</v>
       </c>
+      <c r="F23" s="0" t="n">
+        <v>0.008</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="B24" s="0" t="n">
         <v>0.15</v>
@@ -18813,10 +18885,13 @@
       <c r="E24" s="0" t="n">
         <v>0.0015</v>
       </c>
+      <c r="F24" s="0" t="n">
+        <v>0.0015</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="B25" s="0" t="n">
         <v>0</v>
@@ -18830,10 +18905,13 @@
       <c r="E25" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="F25" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="B26" s="0" t="n">
         <v>0</v>
@@ -18847,10 +18925,13 @@
       <c r="E26" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="F26" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="B27" s="0" t="n">
         <v>0.0001</v>
@@ -18864,10 +18945,13 @@
       <c r="E27" s="0" t="n">
         <v>0.0001</v>
       </c>
+      <c r="F27" s="0" t="n">
+        <v>0.0001</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="B28" s="0" t="n">
         <v>0.006</v>
@@ -18881,10 +18965,13 @@
       <c r="E28" s="0" t="n">
         <v>0.0006</v>
       </c>
+      <c r="F28" s="0" t="n">
+        <v>0.0006</v>
+      </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="B31" s="0" t="n">
         <v>0.001455</v>
@@ -18892,7 +18979,7 @@
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="B32" s="0" t="n">
         <v>0.001</v>
@@ -18900,7 +18987,7 @@
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="B33" s="0" t="n">
         <v>0.001455</v>
@@ -18908,7 +18995,7 @@
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="B34" s="0" t="n">
         <v>0.001</v>
@@ -18916,7 +19003,7 @@
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="B35" s="0" t="n">
         <v>0.002</v>
@@ -18924,7 +19011,7 @@
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="B36" s="0" t="n">
         <v>0.002</v>
@@ -18932,7 +19019,7 @@
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="B37" s="0" t="n">
         <v>0.002</v>
@@ -18940,7 +19027,7 @@
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="B38" s="1" t="n">
         <v>0.0007</v>
@@ -18948,7 +19035,7 @@
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B39" s="1" t="n">
         <v>0.0005</v>
@@ -18956,7 +19043,7 @@
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="B40" s="1" t="n">
         <v>0.00065</v>
@@ -18964,7 +19051,7 @@
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="B41" s="1" t="n">
         <v>0.0005</v>
@@ -18972,7 +19059,7 @@
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="B42" s="1" t="n">
         <v>5E-006</v>
@@ -18980,7 +19067,7 @@
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B43" s="0" t="n">
         <v>0.00015</v>
@@ -18988,7 +19075,7 @@
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="B44" s="0" t="n">
         <v>0.0001</v>
@@ -18996,7 +19083,7 @@
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="B45" s="0" t="n">
         <v>0.00015</v>
@@ -19004,7 +19091,7 @@
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="B46" s="0" t="n">
         <v>0.0001</v>
@@ -19012,7 +19099,7 @@
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="B47" s="0" t="n">
         <v>0.002</v>
@@ -19020,7 +19107,7 @@
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="B48" s="1" t="n">
         <v>0.0005</v>
@@ -19028,7 +19115,7 @@
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="B49" s="0" t="n">
         <v>0.0003</v>
@@ -19036,7 +19123,7 @@
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="B50" s="0" t="n">
         <v>0.0001</v>
@@ -19044,7 +19131,7 @@
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="B51" s="0" t="n">
         <v>0.008</v>
@@ -19052,7 +19139,7 @@
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="B52" s="0" t="n">
         <v>0.0015</v>
@@ -19060,7 +19147,7 @@
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="B53" s="0" t="n">
         <v>0</v>
@@ -19068,7 +19155,7 @@
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="B54" s="0" t="n">
         <v>0</v>
@@ -19076,7 +19163,7 @@
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="B55" s="0" t="n">
         <v>0.0001</v>
@@ -19084,7 +19171,7 @@
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="B56" s="0" t="n">
         <v>0.0006</v>
@@ -19100,7 +19187,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{27B61ABC-2AD7-4758-AB4E-C3B7BB64A6C3}</x14:id>
+          <x14:id>{6AEEEA61-8913-40F5-8A17-69E9D22C2B96}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -19116,7 +19203,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{27B61ABC-2AD7-4758-AB4E-C3B7BB64A6C3}">
+          <x14:cfRule type="dataBar" id="{6AEEEA61-8913-40F5-8A17-69E9D22C2B96}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="true">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -19137,10 +19224,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E33"/>
+  <dimension ref="A1:F65"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F5" activeCellId="0" sqref="F5"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -19162,15 +19249,21 @@
       <c r="E1" s="0" t="n">
         <v>20180531</v>
       </c>
+      <c r="F1" s="0" t="n">
+        <v>20180530</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E2" s="0" t="s">
         <v>279</v>
       </c>
+      <c r="F2" s="0" t="s">
+        <v>280</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>0.0044</v>
@@ -19184,10 +19277,13 @@
       <c r="E3" s="0" t="n">
         <v>0.044</v>
       </c>
+      <c r="F3" s="0" t="n">
+        <v>0.044</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>0.004</v>
@@ -19201,10 +19297,13 @@
       <c r="E4" s="0" t="n">
         <v>0.04</v>
       </c>
+      <c r="F4" s="0" t="n">
+        <v>0.04</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>0.00444</v>
@@ -19218,10 +19317,13 @@
       <c r="E5" s="0" t="n">
         <v>0.0444</v>
       </c>
+      <c r="F5" s="0" t="n">
+        <v>0.0444</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>0.004</v>
@@ -19235,10 +19337,13 @@
       <c r="E6" s="0" t="n">
         <v>0.04</v>
       </c>
+      <c r="F6" s="0" t="n">
+        <v>0.04</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>0.05</v>
@@ -19252,10 +19357,13 @@
       <c r="E7" s="0" t="n">
         <v>0.05</v>
       </c>
+      <c r="F7" s="0" t="n">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>0.05</v>
@@ -19269,10 +19377,13 @@
       <c r="E8" s="0" t="n">
         <v>0.05</v>
       </c>
+      <c r="F8" s="0" t="n">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>0.05</v>
@@ -19286,10 +19397,13 @@
       <c r="E9" s="0" t="n">
         <v>0.05</v>
       </c>
+      <c r="F9" s="0" t="n">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>0.0035</v>
@@ -19303,10 +19417,13 @@
       <c r="E10" s="0" t="n">
         <v>0.0035</v>
       </c>
+      <c r="F10" s="0" t="n">
+        <v>0.035</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>0.0002</v>
@@ -19320,10 +19437,13 @@
       <c r="E11" s="0" t="n">
         <v>0.0002</v>
       </c>
+      <c r="F11" s="0" t="n">
+        <v>0.002</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>0.0012</v>
@@ -19337,10 +19457,13 @@
       <c r="E12" s="0" t="n">
         <v>0.012</v>
       </c>
+      <c r="F12" s="0" t="n">
+        <v>0.012</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="B13" s="1" t="n">
         <v>0.001</v>
@@ -19354,10 +19477,13 @@
       <c r="E13" s="1" t="n">
         <v>0.01</v>
       </c>
+      <c r="F13" s="1" t="n">
+        <v>0.001</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="B14" s="1" t="n">
         <v>0.001</v>
@@ -19371,10 +19497,13 @@
       <c r="E14" s="1" t="n">
         <v>0.001</v>
       </c>
+      <c r="F14" s="1" t="n">
+        <v>0.001</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>0.003043</v>
@@ -19388,10 +19517,13 @@
       <c r="E15" s="0" t="n">
         <v>0.003043</v>
       </c>
+      <c r="F15" s="0" t="n">
+        <v>0.03043</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="B16" s="0" t="n">
         <v>0.003</v>
@@ -19405,10 +19537,13 @@
       <c r="E16" s="0" t="n">
         <v>0.003</v>
       </c>
+      <c r="F16" s="0" t="n">
+        <v>0.03</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="B17" s="0" t="n">
         <v>0.003043</v>
@@ -19422,10 +19557,13 @@
       <c r="E17" s="0" t="n">
         <v>0.003043</v>
       </c>
+      <c r="F17" s="0" t="n">
+        <v>0.03043</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="B18" s="0" t="n">
         <v>0.003</v>
@@ -19439,10 +19577,13 @@
       <c r="E18" s="0" t="n">
         <v>0.003</v>
       </c>
+      <c r="F18" s="0" t="n">
+        <v>0.03</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="B19" s="0" t="n">
         <v>0.005</v>
@@ -19456,10 +19597,13 @@
       <c r="E19" s="0" t="n">
         <v>0.05</v>
       </c>
+      <c r="F19" s="0" t="n">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="B20" s="0" t="n">
         <v>0.0014</v>
@@ -19473,10 +19617,13 @@
       <c r="E20" s="0" t="n">
         <v>0.0014</v>
       </c>
+      <c r="F20" s="0" t="n">
+        <v>0.014</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="B21" s="0" t="n">
         <v>0.01</v>
@@ -19490,10 +19637,13 @@
       <c r="E21" s="0" t="n">
         <v>0.001</v>
       </c>
+      <c r="F21" s="0" t="n">
+        <v>0.001</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="B22" s="0" t="n">
         <v>0.018</v>
@@ -19507,10 +19657,13 @@
       <c r="E22" s="0" t="n">
         <v>0.018</v>
       </c>
+      <c r="F22" s="0" t="n">
+        <v>0.018</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="B23" s="0" t="n">
         <v>0.07</v>
@@ -19524,10 +19677,13 @@
       <c r="E23" s="0" t="n">
         <v>0.07</v>
       </c>
+      <c r="F23" s="0" t="n">
+        <v>0.07</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="B24" s="0" t="n">
         <v>0.08</v>
@@ -19541,10 +19697,13 @@
       <c r="E24" s="0" t="n">
         <v>0.008</v>
       </c>
+      <c r="F24" s="0" t="n">
+        <v>0.08</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="B25" s="0" t="n">
         <v>0.017</v>
@@ -19558,10 +19717,13 @@
       <c r="E25" s="0" t="n">
         <v>0.17</v>
       </c>
+      <c r="F25" s="0" t="n">
+        <v>0.17</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="B26" s="0" t="n">
         <v>0.4</v>
@@ -19575,10 +19737,13 @@
       <c r="E26" s="0" t="n">
         <v>0.4</v>
       </c>
+      <c r="F26" s="0" t="n">
+        <v>0.2</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="B27" s="0" t="n">
         <v>0.01</v>
@@ -19592,10 +19757,13 @@
       <c r="E27" s="0" t="n">
         <v>0.001</v>
       </c>
+      <c r="F27" s="0" t="n">
+        <v>0.001</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="B28" s="0" t="n">
         <v>0.05</v>
@@ -19609,10 +19777,13 @@
       <c r="E28" s="0" t="n">
         <v>0.05</v>
       </c>
+      <c r="F28" s="0" t="n">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="B29" s="0" t="n">
         <v>0.18</v>
@@ -19626,10 +19797,13 @@
       <c r="E29" s="0" t="n">
         <v>0.018</v>
       </c>
+      <c r="F29" s="0" t="n">
+        <v>0.018</v>
+      </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="B30" s="0" t="n">
         <v>0.55</v>
@@ -19643,10 +19817,13 @@
       <c r="E30" s="0" t="n">
         <v>0.055</v>
       </c>
+      <c r="F30" s="0" t="n">
+        <v>0.055</v>
+      </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="B31" s="0" t="n">
         <v>0.05</v>
@@ -19660,10 +19837,13 @@
       <c r="E31" s="0" t="n">
         <v>0.05</v>
       </c>
+      <c r="F31" s="0" t="n">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="B32" s="0" t="n">
         <v>0.02</v>
@@ -19677,10 +19857,13 @@
       <c r="E32" s="0" t="n">
         <v>0.02</v>
       </c>
+      <c r="F32" s="0" t="n">
+        <v>0.02</v>
+      </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="B33" s="0" t="n">
         <v>0.001</v>
@@ -19693,6 +19876,257 @@
       </c>
       <c r="E33" s="0" t="n">
         <v>0.0001</v>
+      </c>
+      <c r="F33" s="0" t="n">
+        <v>0.001</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="s">
+        <v>307</v>
+      </c>
+      <c r="B35" s="0" t="n">
+        <v>0.044</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="s">
+        <v>308</v>
+      </c>
+      <c r="B36" s="0" t="n">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="s">
+        <v>309</v>
+      </c>
+      <c r="B37" s="0" t="n">
+        <v>0.0444</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="B38" s="0" t="n">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="s">
+        <v>311</v>
+      </c>
+      <c r="B39" s="0" t="n">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0" t="s">
+        <v>312</v>
+      </c>
+      <c r="B40" s="0" t="n">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0" t="s">
+        <v>313</v>
+      </c>
+      <c r="B41" s="0" t="n">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="s">
+        <v>314</v>
+      </c>
+      <c r="B42" s="0" t="n">
+        <v>0.035</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0" t="s">
+        <v>315</v>
+      </c>
+      <c r="B43" s="0" t="n">
+        <v>0.002</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="0" t="s">
+        <v>316</v>
+      </c>
+      <c r="B44" s="0" t="n">
+        <v>0.012</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0" t="s">
+        <v>317</v>
+      </c>
+      <c r="B45" s="1" t="n">
+        <v>0.001</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="0" t="s">
+        <v>318</v>
+      </c>
+      <c r="B46" s="1" t="n">
+        <v>0.001</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="0" t="s">
+        <v>319</v>
+      </c>
+      <c r="B47" s="0" t="n">
+        <v>0.03043</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="0" t="s">
+        <v>320</v>
+      </c>
+      <c r="B48" s="0" t="n">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="0" t="s">
+        <v>321</v>
+      </c>
+      <c r="B49" s="0" t="n">
+        <v>0.03043</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="0" t="s">
+        <v>322</v>
+      </c>
+      <c r="B50" s="0" t="n">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="0" t="s">
+        <v>323</v>
+      </c>
+      <c r="B51" s="0" t="n">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="0" t="s">
+        <v>324</v>
+      </c>
+      <c r="B52" s="0" t="n">
+        <v>0.014</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="0" t="s">
+        <v>325</v>
+      </c>
+      <c r="B53" s="0" t="n">
+        <v>0.001</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="0" t="s">
+        <v>326</v>
+      </c>
+      <c r="B54" s="0" t="n">
+        <v>0.018</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="0" t="s">
+        <v>327</v>
+      </c>
+      <c r="B55" s="0" t="n">
+        <v>0.07</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="0" t="s">
+        <v>328</v>
+      </c>
+      <c r="B56" s="0" t="n">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="0" t="s">
+        <v>329</v>
+      </c>
+      <c r="B57" s="0" t="n">
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="0" t="s">
+        <v>330</v>
+      </c>
+      <c r="B58" s="0" t="n">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="0" t="s">
+        <v>331</v>
+      </c>
+      <c r="B59" s="0" t="n">
+        <v>0.001</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="0" t="s">
+        <v>332</v>
+      </c>
+      <c r="B60" s="0" t="n">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="0" t="s">
+        <v>333</v>
+      </c>
+      <c r="B61" s="0" t="n">
+        <v>0.018</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="0" t="s">
+        <v>334</v>
+      </c>
+      <c r="B62" s="0" t="n">
+        <v>0.055</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="0" t="s">
+        <v>335</v>
+      </c>
+      <c r="B63" s="0" t="n">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="0" t="s">
+        <v>336</v>
+      </c>
+      <c r="B64" s="0" t="n">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="0" t="s">
+        <v>337</v>
+      </c>
+      <c r="B65" s="0" t="n">
+        <v>0.001</v>
       </c>
     </row>
   </sheetData>
@@ -19705,7 +20139,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{65B143CF-CA16-4C43-B6F3-C68A543BC1C4}</x14:id>
+          <x14:id>{BF613A9C-3A93-4CC1-BEE0-7B95E5A12ED3}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -19721,7 +20155,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{65B143CF-CA16-4C43-B6F3-C68A543BC1C4}">
+          <x14:cfRule type="dataBar" id="{BF613A9C-3A93-4CC1-BEE0-7B95E5A12ED3}">
             <x14:dataBar minLength="0" maxLength="100" axisPosition="automatic" gradient="true">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>

</xml_diff>

<commit_message>
final merge between v1 and v15 pPREY
</commit_message>
<xml_diff>
--- a/R/C_and_Mum.xlsx
+++ b/R/C_and_Mum.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="988" firstSheet="8" activeTab="8"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="988" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="C_v1" sheetId="1" r:id="rId1"/>
@@ -21,6 +21,7 @@
     <sheet name="2018_tuning_C" sheetId="7" r:id="rId7"/>
     <sheet name="2018_tuning_mum" sheetId="8" r:id="rId8"/>
     <sheet name="ageclass" sheetId="9" r:id="rId9"/>
+    <sheet name="gape" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1680" uniqueCount="509">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1852" uniqueCount="681">
   <si>
     <t>FPL</t>
   </si>
@@ -1559,6 +1560,522 @@
   </si>
   <si>
     <t>http://www.fishbase.org/Summary/SpeciesSummary.php?ID=118&amp;AT=atlantic+mackerel</t>
+  </si>
+  <si>
+    <t>KLP_MAK</t>
+  </si>
+  <si>
+    <t>KLP_HER</t>
+  </si>
+  <si>
+    <t>KLP_WHK</t>
+  </si>
+  <si>
+    <t>KLP_BLF</t>
+  </si>
+  <si>
+    <t>KLP_WPF</t>
+  </si>
+  <si>
+    <t>KLP_SUF</t>
+  </si>
+  <si>
+    <t>KLP_WIF</t>
+  </si>
+  <si>
+    <t>KLP_WTF</t>
+  </si>
+  <si>
+    <t>KLP_HAL</t>
+  </si>
+  <si>
+    <t>KLP_PLA</t>
+  </si>
+  <si>
+    <t>KLP_FOU</t>
+  </si>
+  <si>
+    <t>KLP_FLA</t>
+  </si>
+  <si>
+    <t>KLP_BFT</t>
+  </si>
+  <si>
+    <t>KLP_TUN</t>
+  </si>
+  <si>
+    <t>KLP_BIL</t>
+  </si>
+  <si>
+    <t>KLP_MPF</t>
+  </si>
+  <si>
+    <t>KLP_BUT</t>
+  </si>
+  <si>
+    <t>KLP_ANC</t>
+  </si>
+  <si>
+    <t>KLP_BPF</t>
+  </si>
+  <si>
+    <t>KLP_GOO</t>
+  </si>
+  <si>
+    <t>KLP_MEN</t>
+  </si>
+  <si>
+    <t>KLP_FDE</t>
+  </si>
+  <si>
+    <t>KLP_COD</t>
+  </si>
+  <si>
+    <t>KLP_SHK</t>
+  </si>
+  <si>
+    <t>KLP_OHK</t>
+  </si>
+  <si>
+    <t>KLP_POL</t>
+  </si>
+  <si>
+    <t>KLP_RHK</t>
+  </si>
+  <si>
+    <t>KLP_BSB</t>
+  </si>
+  <si>
+    <t>KLP_SCU</t>
+  </si>
+  <si>
+    <t>KLP_TYL</t>
+  </si>
+  <si>
+    <t>KLP_RED</t>
+  </si>
+  <si>
+    <t>KLP_OPT</t>
+  </si>
+  <si>
+    <t>KLP_SAL</t>
+  </si>
+  <si>
+    <t>KLP_DRM</t>
+  </si>
+  <si>
+    <t>KLP_STB</t>
+  </si>
+  <si>
+    <t>KLP_TAU</t>
+  </si>
+  <si>
+    <t>KLP_WOL</t>
+  </si>
+  <si>
+    <t>KLP_SDF</t>
+  </si>
+  <si>
+    <t>KLP_FDF</t>
+  </si>
+  <si>
+    <t>KLP_HAD</t>
+  </si>
+  <si>
+    <t>KLP_YTF</t>
+  </si>
+  <si>
+    <t>KLP_DOG</t>
+  </si>
+  <si>
+    <t>KLP_SMO</t>
+  </si>
+  <si>
+    <t>KLP_SSH</t>
+  </si>
+  <si>
+    <t>KLP_DSH</t>
+  </si>
+  <si>
+    <t>KLP_BLS</t>
+  </si>
+  <si>
+    <t>KLP_POR</t>
+  </si>
+  <si>
+    <t>KLP_PSH</t>
+  </si>
+  <si>
+    <t>KLP_WSK</t>
+  </si>
+  <si>
+    <t>KLP_LSK</t>
+  </si>
+  <si>
+    <t>KLP_SK</t>
+  </si>
+  <si>
+    <t>KLP_SB</t>
+  </si>
+  <si>
+    <t>KLP_PIN</t>
+  </si>
+  <si>
+    <t>KLP_REP</t>
+  </si>
+  <si>
+    <t>KLP_RWH</t>
+  </si>
+  <si>
+    <t>KLP_BWH</t>
+  </si>
+  <si>
+    <t>KLP_SWH</t>
+  </si>
+  <si>
+    <t>KLP_TWH</t>
+  </si>
+  <si>
+    <t>KLP_INV</t>
+  </si>
+  <si>
+    <t>KLP_LSQ</t>
+  </si>
+  <si>
+    <t>KLP_ISQ</t>
+  </si>
+  <si>
+    <t>KLP_SCA</t>
+  </si>
+  <si>
+    <t>KLP_QHG</t>
+  </si>
+  <si>
+    <t>KLP_CLA</t>
+  </si>
+  <si>
+    <t>KLP_BFF</t>
+  </si>
+  <si>
+    <t>KLP_BG</t>
+  </si>
+  <si>
+    <t>KLP_LOB</t>
+  </si>
+  <si>
+    <t>KLP_RCB</t>
+  </si>
+  <si>
+    <t>KLP_BMS</t>
+  </si>
+  <si>
+    <t>KLP_NSH</t>
+  </si>
+  <si>
+    <t>KLP_OSH</t>
+  </si>
+  <si>
+    <t>KLP_ZL</t>
+  </si>
+  <si>
+    <t>KLP_BD</t>
+  </si>
+  <si>
+    <t>KLP_MA</t>
+  </si>
+  <si>
+    <t>KLP_MB</t>
+  </si>
+  <si>
+    <t>KLP_SG</t>
+  </si>
+  <si>
+    <t>KLP_BC</t>
+  </si>
+  <si>
+    <t>KLP_ZG</t>
+  </si>
+  <si>
+    <t>KLP_PL</t>
+  </si>
+  <si>
+    <t>KLP_DF</t>
+  </si>
+  <si>
+    <t>KLP_PS</t>
+  </si>
+  <si>
+    <t>KLP_ZM</t>
+  </si>
+  <si>
+    <t>KLP_ZS</t>
+  </si>
+  <si>
+    <t>KLP_PB</t>
+  </si>
+  <si>
+    <t>KLP_BB</t>
+  </si>
+  <si>
+    <t>KLP_BO</t>
+  </si>
+  <si>
+    <t>KUP_MAK</t>
+  </si>
+  <si>
+    <t>KUP_HER</t>
+  </si>
+  <si>
+    <t>KUP_WHK</t>
+  </si>
+  <si>
+    <t>KUP_BLF</t>
+  </si>
+  <si>
+    <t>KUP_WPF</t>
+  </si>
+  <si>
+    <t>KUP_SUF</t>
+  </si>
+  <si>
+    <t>KUP_WIF</t>
+  </si>
+  <si>
+    <t>KUP_WTF</t>
+  </si>
+  <si>
+    <t>KUP_HAL</t>
+  </si>
+  <si>
+    <t>KUP_PLA</t>
+  </si>
+  <si>
+    <t>KUP_FOU</t>
+  </si>
+  <si>
+    <t>KUP_FLA</t>
+  </si>
+  <si>
+    <t>KUP_BFT</t>
+  </si>
+  <si>
+    <t>KUP_TUN</t>
+  </si>
+  <si>
+    <t>KUP_BIL</t>
+  </si>
+  <si>
+    <t>KUP_MPF</t>
+  </si>
+  <si>
+    <t>KUP_BUT</t>
+  </si>
+  <si>
+    <t>KUP_ANC</t>
+  </si>
+  <si>
+    <t>KUP_BPF</t>
+  </si>
+  <si>
+    <t>KUP_GOO</t>
+  </si>
+  <si>
+    <t>KUP_MEN</t>
+  </si>
+  <si>
+    <t>KUP_FDE</t>
+  </si>
+  <si>
+    <t>KUP_COD</t>
+  </si>
+  <si>
+    <t>KUP_SHK</t>
+  </si>
+  <si>
+    <t>KUP_OHK</t>
+  </si>
+  <si>
+    <t>KUP_POL</t>
+  </si>
+  <si>
+    <t>KUP_RHK</t>
+  </si>
+  <si>
+    <t>KUP_BSB</t>
+  </si>
+  <si>
+    <t>KUP_SCU</t>
+  </si>
+  <si>
+    <t>KUP_TYL</t>
+  </si>
+  <si>
+    <t>KUP_RED</t>
+  </si>
+  <si>
+    <t>KUP_OPT</t>
+  </si>
+  <si>
+    <t>KUP_SAL</t>
+  </si>
+  <si>
+    <t>KUP_DRM</t>
+  </si>
+  <si>
+    <t>KUP_STB</t>
+  </si>
+  <si>
+    <t>KUP_TAU</t>
+  </si>
+  <si>
+    <t>KUP_WOL</t>
+  </si>
+  <si>
+    <t>KUP_SDF</t>
+  </si>
+  <si>
+    <t>KUP_FDF</t>
+  </si>
+  <si>
+    <t>KUP_HAD</t>
+  </si>
+  <si>
+    <t>KUP_YTF</t>
+  </si>
+  <si>
+    <t>KUP_DOG</t>
+  </si>
+  <si>
+    <t>KUP_SMO</t>
+  </si>
+  <si>
+    <t>KUP_SSH</t>
+  </si>
+  <si>
+    <t>KUP_DSH</t>
+  </si>
+  <si>
+    <t>KUP_BLS</t>
+  </si>
+  <si>
+    <t>KUP_POR</t>
+  </si>
+  <si>
+    <t>KUP_PSH</t>
+  </si>
+  <si>
+    <t>KUP_WSK</t>
+  </si>
+  <si>
+    <t>KUP_LSK</t>
+  </si>
+  <si>
+    <t>KUP_SK</t>
+  </si>
+  <si>
+    <t>KUP_SB</t>
+  </si>
+  <si>
+    <t>KUP_PIN</t>
+  </si>
+  <si>
+    <t>KUP_REP</t>
+  </si>
+  <si>
+    <t>KUP_RWH</t>
+  </si>
+  <si>
+    <t>KUP_BWH</t>
+  </si>
+  <si>
+    <t>KUP_SWH</t>
+  </si>
+  <si>
+    <t>KUP_TWH</t>
+  </si>
+  <si>
+    <t>KUP_INV</t>
+  </si>
+  <si>
+    <t>KUP_LSQ</t>
+  </si>
+  <si>
+    <t>KUP_ISQ</t>
+  </si>
+  <si>
+    <t>KUP_SCA</t>
+  </si>
+  <si>
+    <t>KUP_QHG</t>
+  </si>
+  <si>
+    <t>KUP_CLA</t>
+  </si>
+  <si>
+    <t>KUP_BFF</t>
+  </si>
+  <si>
+    <t>KUP_BG</t>
+  </si>
+  <si>
+    <t>KUP_LOB</t>
+  </si>
+  <si>
+    <t>KUP_RCB</t>
+  </si>
+  <si>
+    <t>KUP_BMS</t>
+  </si>
+  <si>
+    <t>KUP_NSH</t>
+  </si>
+  <si>
+    <t>KUP_OSH</t>
+  </si>
+  <si>
+    <t>KUP_ZL</t>
+  </si>
+  <si>
+    <t>KUP_BD</t>
+  </si>
+  <si>
+    <t>KUP_MA</t>
+  </si>
+  <si>
+    <t>KUP_MB</t>
+  </si>
+  <si>
+    <t>KUP_SG</t>
+  </si>
+  <si>
+    <t>KUP_BC</t>
+  </si>
+  <si>
+    <t>KUP_ZG</t>
+  </si>
+  <si>
+    <t>KUP_PL</t>
+  </si>
+  <si>
+    <t>KUP_DF</t>
+  </si>
+  <si>
+    <t>KUP_PS</t>
+  </si>
+  <si>
+    <t>KUP_ZM</t>
+  </si>
+  <si>
+    <t>KUP_ZS</t>
+  </si>
+  <si>
+    <t>KUP_PB</t>
+  </si>
+  <si>
+    <t>KUP_BB</t>
+  </si>
+  <si>
+    <t>KUP_BO</t>
   </si>
 </sst>
 </file>
@@ -3872,6 +4389,1400 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B173"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="B142" sqref="B142"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>509</v>
+      </c>
+      <c r="B1" s="1">
+        <v>1.0000000000000001E-5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>510</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1.0000000000000001E-5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>511</v>
+      </c>
+      <c r="B3" s="1">
+        <v>1.0000000000000001E-5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>512</v>
+      </c>
+      <c r="B4" s="1">
+        <v>1.0000000000000001E-5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>513</v>
+      </c>
+      <c r="B5" s="1">
+        <v>1.0000000000000001E-5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>514</v>
+      </c>
+      <c r="B6" s="1">
+        <v>1.0000000000000001E-5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>515</v>
+      </c>
+      <c r="B7" s="1">
+        <v>1.0000000000000001E-5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>516</v>
+      </c>
+      <c r="B8" s="1">
+        <v>1.0000000000000001E-5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>517</v>
+      </c>
+      <c r="B9" s="1">
+        <v>1.0000000000000001E-5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>518</v>
+      </c>
+      <c r="B10" s="1">
+        <v>1.0000000000000001E-5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>519</v>
+      </c>
+      <c r="B11" s="1">
+        <v>1.0000000000000001E-5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>520</v>
+      </c>
+      <c r="B12" s="1">
+        <v>1.0000000000000001E-5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>521</v>
+      </c>
+      <c r="B13" s="1">
+        <v>1.0000000000000001E-5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>522</v>
+      </c>
+      <c r="B14" s="1">
+        <v>1.0000000000000001E-5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>523</v>
+      </c>
+      <c r="B15" s="1">
+        <v>1.0000000000000001E-5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>524</v>
+      </c>
+      <c r="B16" s="1">
+        <v>1.0000000000000001E-5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>525</v>
+      </c>
+      <c r="B17" s="1">
+        <v>1.0000000000000001E-5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>526</v>
+      </c>
+      <c r="B18" s="1">
+        <v>1.0000000000000001E-5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>527</v>
+      </c>
+      <c r="B19" s="1">
+        <v>1.0000000000000001E-5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>528</v>
+      </c>
+      <c r="B20" s="1">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>529</v>
+      </c>
+      <c r="B21" s="1">
+        <v>1.0000000000000001E-5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>530</v>
+      </c>
+      <c r="B22" s="1">
+        <v>1.0000000000000001E-5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>531</v>
+      </c>
+      <c r="B23" s="1">
+        <v>1.0000000000000001E-5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>532</v>
+      </c>
+      <c r="B24" s="1">
+        <v>1.0000000000000001E-5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>533</v>
+      </c>
+      <c r="B25" s="1">
+        <v>1.0000000000000001E-5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>534</v>
+      </c>
+      <c r="B26" s="1">
+        <v>1.0000000000000001E-5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>535</v>
+      </c>
+      <c r="B27" s="1">
+        <v>1.0000000000000001E-5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>536</v>
+      </c>
+      <c r="B28" s="1">
+        <v>1.0000000000000001E-5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>537</v>
+      </c>
+      <c r="B29" s="1">
+        <v>1.0000000000000001E-5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>538</v>
+      </c>
+      <c r="B30" s="1">
+        <v>1.0000000000000001E-5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>539</v>
+      </c>
+      <c r="B31" s="1">
+        <v>1.0000000000000001E-5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>540</v>
+      </c>
+      <c r="B32" s="1">
+        <v>1.0000000000000001E-5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>541</v>
+      </c>
+      <c r="B33" s="1">
+        <v>1.0000000000000001E-5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>542</v>
+      </c>
+      <c r="B34" s="1">
+        <v>1.0000000000000001E-5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>543</v>
+      </c>
+      <c r="B35" s="1">
+        <v>1.0000000000000001E-5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>544</v>
+      </c>
+      <c r="B36" s="1">
+        <v>1.0000000000000001E-5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>545</v>
+      </c>
+      <c r="B37" s="1">
+        <v>1.0000000000000001E-5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>546</v>
+      </c>
+      <c r="B38" s="1">
+        <v>1.0000000000000001E-5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>547</v>
+      </c>
+      <c r="B39" s="1">
+        <v>1.0000000000000001E-5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>548</v>
+      </c>
+      <c r="B40" s="1">
+        <v>1.0000000000000001E-5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>549</v>
+      </c>
+      <c r="B41" s="1">
+        <v>1.0000000000000001E-5</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>550</v>
+      </c>
+      <c r="B42" s="1">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>551</v>
+      </c>
+      <c r="B43" s="1">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>552</v>
+      </c>
+      <c r="B44" s="1">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>553</v>
+      </c>
+      <c r="B45" s="1">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>554</v>
+      </c>
+      <c r="B46" s="1">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>555</v>
+      </c>
+      <c r="B47" s="1">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>556</v>
+      </c>
+      <c r="B48" s="1">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>557</v>
+      </c>
+      <c r="B49" s="1">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>558</v>
+      </c>
+      <c r="B50" s="1">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>559</v>
+      </c>
+      <c r="B51" s="1">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>560</v>
+      </c>
+      <c r="B52" s="1">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>561</v>
+      </c>
+      <c r="B53" s="1">
+        <v>1.0000000000000001E-5</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>562</v>
+      </c>
+      <c r="B54" s="1">
+        <v>1.0000000000000001E-5</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>563</v>
+      </c>
+      <c r="B55" s="1">
+        <v>1E-10</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>564</v>
+      </c>
+      <c r="B56" s="1">
+        <v>1E-10</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>565</v>
+      </c>
+      <c r="B57" s="1">
+        <v>9.9999999999999995E-8</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>566</v>
+      </c>
+      <c r="B58" s="1">
+        <v>9.9999999999999995E-8</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>567</v>
+      </c>
+      <c r="B59" s="1">
+        <v>1.0000000000000001E-5</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>568</v>
+      </c>
+      <c r="B60" s="1">
+        <v>9.9999999999999995E-8</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>569</v>
+      </c>
+      <c r="B61" s="1">
+        <v>9.9999999999999995E-8</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>570</v>
+      </c>
+      <c r="B62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>571</v>
+      </c>
+      <c r="B63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>572</v>
+      </c>
+      <c r="B64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>573</v>
+      </c>
+      <c r="B65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>574</v>
+      </c>
+      <c r="B66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>575</v>
+      </c>
+      <c r="B67" s="1">
+        <v>9.9999999999999995E-8</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>576</v>
+      </c>
+      <c r="B68" s="1">
+        <v>9.9999999999999995E-8</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>577</v>
+      </c>
+      <c r="B69" s="1">
+        <v>9.9999999999999995E-8</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>578</v>
+      </c>
+      <c r="B70" s="1">
+        <v>9.9999999999999995E-8</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>579</v>
+      </c>
+      <c r="B71" s="1">
+        <v>9.9999999999999995E-8</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>580</v>
+      </c>
+      <c r="B72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>581</v>
+      </c>
+      <c r="B73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>582</v>
+      </c>
+      <c r="B74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>583</v>
+      </c>
+      <c r="B75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>584</v>
+      </c>
+      <c r="B76">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>585</v>
+      </c>
+      <c r="B77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>586</v>
+      </c>
+      <c r="B78" s="1">
+        <v>9.9999999999999995E-8</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>587</v>
+      </c>
+      <c r="B79">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>588</v>
+      </c>
+      <c r="B80">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>589</v>
+      </c>
+      <c r="B81">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>590</v>
+      </c>
+      <c r="B82">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>591</v>
+      </c>
+      <c r="B83">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>592</v>
+      </c>
+      <c r="B84">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>593</v>
+      </c>
+      <c r="B85">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>594</v>
+      </c>
+      <c r="B86">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>595</v>
+      </c>
+      <c r="B88">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>596</v>
+      </c>
+      <c r="B89">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>597</v>
+      </c>
+      <c r="B90">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>598</v>
+      </c>
+      <c r="B91">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>599</v>
+      </c>
+      <c r="B92">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>600</v>
+      </c>
+      <c r="B93">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>601</v>
+      </c>
+      <c r="B94">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>602</v>
+      </c>
+      <c r="B95">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>603</v>
+      </c>
+      <c r="B96">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>604</v>
+      </c>
+      <c r="B97">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>605</v>
+      </c>
+      <c r="B98">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>606</v>
+      </c>
+      <c r="B99">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>607</v>
+      </c>
+      <c r="B100">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>608</v>
+      </c>
+      <c r="B101">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>609</v>
+      </c>
+      <c r="B102">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>610</v>
+      </c>
+      <c r="B103">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>611</v>
+      </c>
+      <c r="B104">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>612</v>
+      </c>
+      <c r="B105">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>613</v>
+      </c>
+      <c r="B106">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>614</v>
+      </c>
+      <c r="B107">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>615</v>
+      </c>
+      <c r="B108">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>616</v>
+      </c>
+      <c r="B109">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>617</v>
+      </c>
+      <c r="B110">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>618</v>
+      </c>
+      <c r="B111">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>619</v>
+      </c>
+      <c r="B112">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>620</v>
+      </c>
+      <c r="B113">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>621</v>
+      </c>
+      <c r="B114">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>622</v>
+      </c>
+      <c r="B115">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>623</v>
+      </c>
+      <c r="B116">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>624</v>
+      </c>
+      <c r="B117">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>625</v>
+      </c>
+      <c r="B118">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>626</v>
+      </c>
+      <c r="B119">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>627</v>
+      </c>
+      <c r="B120">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>628</v>
+      </c>
+      <c r="B121">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>629</v>
+      </c>
+      <c r="B122">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
+        <v>630</v>
+      </c>
+      <c r="B123">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
+        <v>631</v>
+      </c>
+      <c r="B124">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
+        <v>632</v>
+      </c>
+      <c r="B125">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
+        <v>633</v>
+      </c>
+      <c r="B126">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
+        <v>634</v>
+      </c>
+      <c r="B127">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
+        <v>635</v>
+      </c>
+      <c r="B128">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
+        <v>636</v>
+      </c>
+      <c r="B129">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
+        <v>637</v>
+      </c>
+      <c r="B130">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
+        <v>638</v>
+      </c>
+      <c r="B131">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
+        <v>639</v>
+      </c>
+      <c r="B132">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A133" t="s">
+        <v>640</v>
+      </c>
+      <c r="B133">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
+        <v>641</v>
+      </c>
+      <c r="B134">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
+        <v>642</v>
+      </c>
+      <c r="B135">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
+        <v>643</v>
+      </c>
+      <c r="B136">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
+        <v>644</v>
+      </c>
+      <c r="B137">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
+        <v>645</v>
+      </c>
+      <c r="B138">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
+        <v>646</v>
+      </c>
+      <c r="B139">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
+        <v>647</v>
+      </c>
+      <c r="B140">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A141" t="s">
+        <v>648</v>
+      </c>
+      <c r="B141">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A142" t="s">
+        <v>649</v>
+      </c>
+      <c r="B142" s="1">
+        <v>4.0000000000000003E-5</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A143" t="s">
+        <v>650</v>
+      </c>
+      <c r="B143" s="1">
+        <v>4.0000000000000003E-5</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A144" t="s">
+        <v>651</v>
+      </c>
+      <c r="B144">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A145" t="s">
+        <v>652</v>
+      </c>
+      <c r="B145">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
+        <v>653</v>
+      </c>
+      <c r="B146">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A147" t="s">
+        <v>654</v>
+      </c>
+      <c r="B147">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A148" t="s">
+        <v>655</v>
+      </c>
+      <c r="B148">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A149" t="s">
+        <v>656</v>
+      </c>
+      <c r="B149">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A150" t="s">
+        <v>657</v>
+      </c>
+      <c r="B150">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A151" t="s">
+        <v>658</v>
+      </c>
+      <c r="B151">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A152" t="s">
+        <v>659</v>
+      </c>
+      <c r="B152">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A153" t="s">
+        <v>660</v>
+      </c>
+      <c r="B153">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A154" t="s">
+        <v>661</v>
+      </c>
+      <c r="B154">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A155" t="s">
+        <v>662</v>
+      </c>
+      <c r="B155">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A156" t="s">
+        <v>663</v>
+      </c>
+      <c r="B156">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A157" t="s">
+        <v>664</v>
+      </c>
+      <c r="B157">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A158" t="s">
+        <v>665</v>
+      </c>
+      <c r="B158">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A159" t="s">
+        <v>666</v>
+      </c>
+      <c r="B159">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A160" t="s">
+        <v>667</v>
+      </c>
+      <c r="B160">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A161" t="s">
+        <v>668</v>
+      </c>
+      <c r="B161">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A162" t="s">
+        <v>669</v>
+      </c>
+      <c r="B162">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A163" t="s">
+        <v>670</v>
+      </c>
+      <c r="B163">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A164" t="s">
+        <v>671</v>
+      </c>
+      <c r="B164">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A165" t="s">
+        <v>672</v>
+      </c>
+      <c r="B165">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A166" t="s">
+        <v>673</v>
+      </c>
+      <c r="B166">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A167" t="s">
+        <v>674</v>
+      </c>
+      <c r="B167">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A168" t="s">
+        <v>675</v>
+      </c>
+      <c r="B168">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A169" t="s">
+        <v>676</v>
+      </c>
+      <c r="B169">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A170" t="s">
+        <v>677</v>
+      </c>
+      <c r="B170">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A171" t="s">
+        <v>678</v>
+      </c>
+      <c r="B171">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A172" t="s">
+        <v>679</v>
+      </c>
+      <c r="B172">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A173" t="s">
+        <v>680</v>
+      </c>
+      <c r="B173">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B5:P93"/>
@@ -20872,7 +22783,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P123"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="P42" sqref="P42"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
tuning pPREY based on diets
</commit_message>
<xml_diff>
--- a/R/C_and_Mum.xlsx
+++ b/R/C_and_Mum.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="988" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="988" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="C_v1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1852" uniqueCount="681">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1849" uniqueCount="679">
   <si>
     <t>FPL</t>
   </si>
@@ -1248,12 +1248,6 @@
   </si>
   <si>
     <t>age</t>
-  </si>
-  <si>
-    <t>large</t>
-  </si>
-  <si>
-    <t>planktivores</t>
   </si>
   <si>
     <t>MAK_age_mat</t>
@@ -2414,8 +2408,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:O70"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D48" sqref="D48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4393,7 +4387,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B173"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+    <sheetView topLeftCell="A82" workbookViewId="0">
       <selection activeCell="B142" sqref="B142"/>
     </sheetView>
   </sheetViews>
@@ -4404,7 +4398,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="B1" s="1">
         <v>1.0000000000000001E-5</v>
@@ -4412,7 +4406,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="B2" s="1">
         <v>1.0000000000000001E-5</v>
@@ -4420,7 +4414,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="B3" s="1">
         <v>1.0000000000000001E-5</v>
@@ -4428,7 +4422,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="B4" s="1">
         <v>1.0000000000000001E-5</v>
@@ -4436,7 +4430,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="B5" s="1">
         <v>1.0000000000000001E-5</v>
@@ -4444,7 +4438,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="B6" s="1">
         <v>1.0000000000000001E-5</v>
@@ -4452,7 +4446,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="B7" s="1">
         <v>1.0000000000000001E-5</v>
@@ -4460,7 +4454,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="B8" s="1">
         <v>1.0000000000000001E-5</v>
@@ -4468,7 +4462,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="B9" s="1">
         <v>1.0000000000000001E-5</v>
@@ -4476,7 +4470,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="B10" s="1">
         <v>1.0000000000000001E-5</v>
@@ -4484,7 +4478,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="B11" s="1">
         <v>1.0000000000000001E-5</v>
@@ -4492,7 +4486,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="B12" s="1">
         <v>1.0000000000000001E-5</v>
@@ -4500,7 +4494,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="B13" s="1">
         <v>1.0000000000000001E-5</v>
@@ -4508,7 +4502,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="B14" s="1">
         <v>1.0000000000000001E-5</v>
@@ -4516,7 +4510,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="B15" s="1">
         <v>1.0000000000000001E-5</v>
@@ -4524,7 +4518,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="B16" s="1">
         <v>1.0000000000000001E-5</v>
@@ -4532,7 +4526,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="B17" s="1">
         <v>1.0000000000000001E-5</v>
@@ -4540,7 +4534,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="B18" s="1">
         <v>1.0000000000000001E-5</v>
@@ -4548,7 +4542,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="B19" s="1">
         <v>1.0000000000000001E-5</v>
@@ -4556,7 +4550,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="B20" s="1">
         <v>1E-4</v>
@@ -4564,7 +4558,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="B21" s="1">
         <v>1.0000000000000001E-5</v>
@@ -4572,7 +4566,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="B22" s="1">
         <v>1.0000000000000001E-5</v>
@@ -4580,7 +4574,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="B23" s="1">
         <v>1.0000000000000001E-5</v>
@@ -4588,7 +4582,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="B24" s="1">
         <v>1.0000000000000001E-5</v>
@@ -4596,7 +4590,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="B25" s="1">
         <v>1.0000000000000001E-5</v>
@@ -4604,7 +4598,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="B26" s="1">
         <v>1.0000000000000001E-5</v>
@@ -4612,7 +4606,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="B27" s="1">
         <v>1.0000000000000001E-5</v>
@@ -4620,7 +4614,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="B28" s="1">
         <v>1.0000000000000001E-5</v>
@@ -4628,7 +4622,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="B29" s="1">
         <v>1.0000000000000001E-5</v>
@@ -4636,7 +4630,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="B30" s="1">
         <v>1.0000000000000001E-5</v>
@@ -4644,7 +4638,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="B31" s="1">
         <v>1.0000000000000001E-5</v>
@@ -4652,7 +4646,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="B32" s="1">
         <v>1.0000000000000001E-5</v>
@@ -4660,7 +4654,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="B33" s="1">
         <v>1.0000000000000001E-5</v>
@@ -4668,7 +4662,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="B34" s="1">
         <v>1.0000000000000001E-5</v>
@@ -4676,7 +4670,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="B35" s="1">
         <v>1.0000000000000001E-5</v>
@@ -4684,7 +4678,7 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="B36" s="1">
         <v>1.0000000000000001E-5</v>
@@ -4692,7 +4686,7 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="B37" s="1">
         <v>1.0000000000000001E-5</v>
@@ -4700,7 +4694,7 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="B38" s="1">
         <v>1.0000000000000001E-5</v>
@@ -4708,7 +4702,7 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="B39" s="1">
         <v>1.0000000000000001E-5</v>
@@ -4716,7 +4710,7 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="B40" s="1">
         <v>1.0000000000000001E-5</v>
@@ -4724,7 +4718,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="B41" s="1">
         <v>1.0000000000000001E-5</v>
@@ -4732,7 +4726,7 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="B42" s="1">
         <v>1E-4</v>
@@ -4740,7 +4734,7 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="B43" s="1">
         <v>1E-4</v>
@@ -4748,7 +4742,7 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="B44" s="1">
         <v>1E-4</v>
@@ -4756,7 +4750,7 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="B45" s="1">
         <v>1E-4</v>
@@ -4764,7 +4758,7 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="B46" s="1">
         <v>1E-4</v>
@@ -4772,7 +4766,7 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="B47" s="1">
         <v>1E-4</v>
@@ -4780,7 +4774,7 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B48" s="1">
         <v>1E-4</v>
@@ -4788,7 +4782,7 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="B49" s="1">
         <v>1E-4</v>
@@ -4796,7 +4790,7 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="B50" s="1">
         <v>1E-4</v>
@@ -4804,7 +4798,7 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="B51" s="1">
         <v>1E-4</v>
@@ -4812,7 +4806,7 @@
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="B52" s="1">
         <v>1E-4</v>
@@ -4820,7 +4814,7 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="B53" s="1">
         <v>1.0000000000000001E-5</v>
@@ -4828,7 +4822,7 @@
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="B54" s="1">
         <v>1.0000000000000001E-5</v>
@@ -4836,7 +4830,7 @@
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="B55" s="1">
         <v>1E-10</v>
@@ -4844,7 +4838,7 @@
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="B56" s="1">
         <v>1E-10</v>
@@ -4852,7 +4846,7 @@
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="B57" s="1">
         <v>9.9999999999999995E-8</v>
@@ -4860,7 +4854,7 @@
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="B58" s="1">
         <v>9.9999999999999995E-8</v>
@@ -4868,7 +4862,7 @@
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="B59" s="1">
         <v>1.0000000000000001E-5</v>
@@ -4876,7 +4870,7 @@
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="B60" s="1">
         <v>9.9999999999999995E-8</v>
@@ -4884,7 +4878,7 @@
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="B61" s="1">
         <v>9.9999999999999995E-8</v>
@@ -4892,7 +4886,7 @@
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="B62">
         <v>0</v>
@@ -4900,7 +4894,7 @@
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="B63">
         <v>0</v>
@@ -4908,7 +4902,7 @@
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="B64">
         <v>0</v>
@@ -4916,7 +4910,7 @@
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="B65">
         <v>0</v>
@@ -4924,7 +4918,7 @@
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="B66">
         <v>0</v>
@@ -4932,7 +4926,7 @@
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="B67" s="1">
         <v>9.9999999999999995E-8</v>
@@ -4940,7 +4934,7 @@
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="B68" s="1">
         <v>9.9999999999999995E-8</v>
@@ -4948,7 +4942,7 @@
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="B69" s="1">
         <v>9.9999999999999995E-8</v>
@@ -4956,7 +4950,7 @@
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="B70" s="1">
         <v>9.9999999999999995E-8</v>
@@ -4964,7 +4958,7 @@
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="B71" s="1">
         <v>9.9999999999999995E-8</v>
@@ -4972,7 +4966,7 @@
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="B72">
         <v>0</v>
@@ -4980,7 +4974,7 @@
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="B73">
         <v>0</v>
@@ -4988,7 +4982,7 @@
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
       <c r="B74">
         <v>0</v>
@@ -4996,7 +4990,7 @@
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B75">
         <v>0</v>
@@ -5004,7 +4998,7 @@
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="B76">
         <v>0</v>
@@ -5012,7 +5006,7 @@
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="B77">
         <v>0</v>
@@ -5020,7 +5014,7 @@
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="B78" s="1">
         <v>9.9999999999999995E-8</v>
@@ -5028,7 +5022,7 @@
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="B79">
         <v>0</v>
@@ -5036,7 +5030,7 @@
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="B80">
         <v>0</v>
@@ -5044,7 +5038,7 @@
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="B81">
         <v>0</v>
@@ -5052,7 +5046,7 @@
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
       <c r="B82">
         <v>0</v>
@@ -5060,7 +5054,7 @@
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="B83">
         <v>0</v>
@@ -5068,7 +5062,7 @@
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
       <c r="B84">
         <v>0</v>
@@ -5076,7 +5070,7 @@
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
       <c r="B85">
         <v>0</v>
@@ -5084,7 +5078,7 @@
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="B86">
         <v>0</v>
@@ -5092,7 +5086,7 @@
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="B88">
         <v>0.8</v>
@@ -5100,7 +5094,7 @@
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
       <c r="B89">
         <v>0.8</v>
@@ -5108,7 +5102,7 @@
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
       <c r="B90">
         <v>0.8</v>
@@ -5116,7 +5110,7 @@
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="B91">
         <v>0.8</v>
@@ -5124,7 +5118,7 @@
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="B92">
         <v>0.8</v>
@@ -5132,7 +5126,7 @@
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="B93">
         <v>0.8</v>
@@ -5140,7 +5134,7 @@
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="B94">
         <v>0.8</v>
@@ -5148,7 +5142,7 @@
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="B95">
         <v>0.8</v>
@@ -5156,7 +5150,7 @@
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="B96">
         <v>0.8</v>
@@ -5164,7 +5158,7 @@
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="B97">
         <v>0.8</v>
@@ -5172,7 +5166,7 @@
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="B98">
         <v>0.8</v>
@@ -5180,7 +5174,7 @@
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="B99">
         <v>0.8</v>
@@ -5188,7 +5182,7 @@
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="B100">
         <v>0.8</v>
@@ -5196,7 +5190,7 @@
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="B101">
         <v>0.8</v>
@@ -5204,7 +5198,7 @@
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="B102">
         <v>0.8</v>
@@ -5212,7 +5206,7 @@
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
       <c r="B103">
         <v>0.3</v>
@@ -5220,7 +5214,7 @@
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="B104">
         <v>0.8</v>
@@ -5228,7 +5222,7 @@
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="B105">
         <v>0.8</v>
@@ -5236,7 +5230,7 @@
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="B106">
         <v>0.8</v>
@@ -5244,7 +5238,7 @@
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="B107">
         <v>0.95</v>
@@ -5252,7 +5246,7 @@
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="B108">
         <v>0.8</v>
@@ -5260,7 +5254,7 @@
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="B109">
         <v>0.8</v>
@@ -5268,7 +5262,7 @@
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="B110">
         <v>0.8</v>
@@ -5276,7 +5270,7 @@
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="B111">
         <v>0.8</v>
@@ -5284,7 +5278,7 @@
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="B112">
         <v>0.8</v>
@@ -5292,7 +5286,7 @@
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
       <c r="B113">
         <v>0.8</v>
@@ -5300,7 +5294,7 @@
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
       <c r="B114">
         <v>0.8</v>
@@ -5308,7 +5302,7 @@
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
       <c r="B115">
         <v>0.8</v>
@@ -5316,7 +5310,7 @@
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="B116">
         <v>0.8</v>
@@ -5324,7 +5318,7 @@
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
       <c r="B117">
         <v>0.8</v>
@@ -5332,7 +5326,7 @@
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
       <c r="B118">
         <v>0.8</v>
@@ -5340,7 +5334,7 @@
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
       <c r="B119">
         <v>0.8</v>
@@ -5348,7 +5342,7 @@
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
       <c r="B120">
         <v>0.8</v>
@@ -5356,7 +5350,7 @@
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
       <c r="B121">
         <v>0.8</v>
@@ -5364,7 +5358,7 @@
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
       <c r="B122">
         <v>0.8</v>
@@ -5372,7 +5366,7 @@
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
       <c r="B123">
         <v>0.8</v>
@@ -5380,7 +5374,7 @@
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="B124">
         <v>0.8</v>
@@ -5388,7 +5382,7 @@
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
       <c r="B125">
         <v>0.8</v>
@@ -5396,7 +5390,7 @@
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
       <c r="B126">
         <v>0.8</v>
@@ -5404,7 +5398,7 @@
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
       <c r="B127">
         <v>0.8</v>
@@ -5412,7 +5406,7 @@
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="B128">
         <v>0.8</v>
@@ -5420,7 +5414,7 @@
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="B129">
         <v>0.8</v>
@@ -5428,7 +5422,7 @@
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="B130">
         <v>0.8</v>
@@ -5436,7 +5430,7 @@
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
       <c r="B131">
         <v>0.8</v>
@@ -5444,7 +5438,7 @@
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="B132">
         <v>0.8</v>
@@ -5452,7 +5446,7 @@
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
       <c r="B133">
         <v>0.8</v>
@@ -5460,7 +5454,7 @@
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
       <c r="B134">
         <v>0.8</v>
@@ -5468,7 +5462,7 @@
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
       <c r="B135">
         <v>0.8</v>
@@ -5476,7 +5470,7 @@
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="B136">
         <v>0.8</v>
@@ -5484,7 +5478,7 @@
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
       <c r="B137">
         <v>0.8</v>
@@ -5492,7 +5486,7 @@
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="B138">
         <v>0.8</v>
@@ -5500,7 +5494,7 @@
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
       <c r="B139">
         <v>0.3</v>
@@ -5508,7 +5502,7 @@
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="B140">
         <v>0.5</v>
@@ -5516,7 +5510,7 @@
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
       <c r="B141">
         <v>0.8</v>
@@ -5524,7 +5518,7 @@
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
       <c r="B142" s="1">
         <v>4.0000000000000003E-5</v>
@@ -5532,7 +5526,7 @@
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
       <c r="B143" s="1">
         <v>4.0000000000000003E-5</v>
@@ -5540,7 +5534,7 @@
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
       <c r="B144">
         <v>20</v>
@@ -5548,7 +5542,7 @@
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
       <c r="B145">
         <v>20</v>
@@ -5556,7 +5550,7 @@
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="B146">
         <v>0.8</v>
@@ -5564,7 +5558,7 @@
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="B147">
         <v>0.6</v>
@@ -5572,7 +5566,7 @@
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="B148">
         <v>0.6</v>
@@ -5580,7 +5574,7 @@
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
       <c r="B149">
         <v>0</v>
@@ -5588,7 +5582,7 @@
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="B150">
         <v>0</v>
@@ -5596,7 +5590,7 @@
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="B151">
         <v>0</v>
@@ -5604,7 +5598,7 @@
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="B152">
         <v>0</v>
@@ -5612,7 +5606,7 @@
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
       <c r="B153">
         <v>0</v>
@@ -5620,7 +5614,7 @@
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
       <c r="B154">
         <v>0.1</v>
@@ -5628,7 +5622,7 @@
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
       <c r="B155">
         <v>0.1</v>
@@ -5636,7 +5630,7 @@
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="B156">
         <v>0.1</v>
@@ -5644,7 +5638,7 @@
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
       <c r="B157">
         <v>0.1</v>
@@ -5652,7 +5646,7 @@
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
       <c r="B158">
         <v>0.1</v>
@@ -5660,7 +5654,7 @@
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="B159">
         <v>0</v>
@@ -5668,7 +5662,7 @@
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
       <c r="B160">
         <v>0</v>
@@ -5676,7 +5670,7 @@
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="B161">
         <v>0</v>
@@ -5684,7 +5678,7 @@
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
       <c r="B162">
         <v>0</v>
@@ -5692,7 +5686,7 @@
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="B163">
         <v>0</v>
@@ -5700,7 +5694,7 @@
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="B164">
         <v>0</v>
@@ -5708,7 +5702,7 @@
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
       <c r="B165">
         <v>0.6</v>
@@ -5716,7 +5710,7 @@
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
       <c r="B166">
         <v>0</v>
@@ -5724,7 +5718,7 @@
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
       <c r="B167">
         <v>0</v>
@@ -5732,7 +5726,7 @@
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="B168">
         <v>0</v>
@@ -5740,7 +5734,7 @@
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
       <c r="B169">
         <v>0</v>
@@ -5748,7 +5742,7 @@
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>677</v>
+        <v>675</v>
       </c>
       <c r="B170">
         <v>0</v>
@@ -5756,7 +5750,7 @@
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
       <c r="B171">
         <v>0</v>
@@ -5764,7 +5758,7 @@
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>679</v>
+        <v>677</v>
       </c>
       <c r="B172">
         <v>0</v>
@@ -5772,7 +5766,7 @@
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
       <c r="B173">
         <v>0</v>
@@ -5787,7 +5781,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B5:P93"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A64" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -9089,7 +9083,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:P92"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A64" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -12391,7 +12385,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:P93"/>
   <sheetViews>
-    <sheetView topLeftCell="A67" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView topLeftCell="A70" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -21026,8 +21020,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G56"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19:XFD19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21835,8 +21829,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F65"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K35" sqref="K35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22781,10 +22775,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P123"/>
+  <dimension ref="A1:J123"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="P42" sqref="P42"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="J32" sqref="J32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22793,24 +22787,24 @@
     <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B1">
         <v>20180419</v>
       </c>
       <c r="C1" t="s">
+        <v>464</v>
+      </c>
+      <c r="D1" t="s">
+        <v>465</v>
+      </c>
+      <c r="F1" t="s">
         <v>466</v>
       </c>
-      <c r="D1" t="s">
-        <v>467</v>
-      </c>
-      <c r="F1" t="s">
-        <v>468</v>
-      </c>
-      <c r="P1" t="s">
-        <v>471</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="J1" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>338</v>
       </c>
@@ -22827,11 +22821,11 @@
       <c r="F2">
         <v>17</v>
       </c>
-      <c r="P2" t="s">
-        <v>508</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="J2" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>339</v>
       </c>
@@ -22848,11 +22842,11 @@
       <c r="F3">
         <v>25</v>
       </c>
-      <c r="P3" s="2" t="s">
-        <v>474</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="J3" s="2" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>340</v>
       </c>
@@ -22869,11 +22863,11 @@
       <c r="F4">
         <v>23</v>
       </c>
-      <c r="P4" t="s">
-        <v>472</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="J4" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>341</v>
       </c>
@@ -22890,11 +22884,11 @@
       <c r="F5">
         <v>9</v>
       </c>
-      <c r="P5" t="s">
-        <v>470</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="J5" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>342</v>
       </c>
@@ -22911,11 +22905,11 @@
       <c r="F6">
         <v>7</v>
       </c>
-      <c r="P6" t="s">
-        <v>475</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="J6" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>343</v>
       </c>
@@ -22932,11 +22926,11 @@
       <c r="F7">
         <v>9</v>
       </c>
-      <c r="P7" t="s">
-        <v>478</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="J7" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>344</v>
       </c>
@@ -22953,11 +22947,11 @@
       <c r="F8">
         <v>14</v>
       </c>
-      <c r="P8" s="2" t="s">
-        <v>476</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="J8" s="2" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>345</v>
       </c>
@@ -22974,11 +22968,11 @@
       <c r="F9">
         <v>25</v>
       </c>
-      <c r="P9" t="s">
-        <v>477</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="J9" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>346</v>
       </c>
@@ -22995,11 +22989,11 @@
       <c r="F10">
         <v>50</v>
       </c>
-      <c r="P10" t="s">
-        <v>473</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="J10" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>347</v>
       </c>
@@ -23016,11 +23010,11 @@
       <c r="F11">
         <v>30</v>
       </c>
-      <c r="P11" t="s">
-        <v>479</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="J11" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>348</v>
       </c>
@@ -23034,11 +23028,11 @@
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="P12" t="s">
-        <v>480</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="J12" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>349</v>
       </c>
@@ -23053,7 +23047,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>350</v>
       </c>
@@ -23070,11 +23064,11 @@
       <c r="F14">
         <v>32</v>
       </c>
-      <c r="P14" t="s">
-        <v>481</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="J14" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>351</v>
       </c>
@@ -23089,7 +23083,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>352</v>
       </c>
@@ -23104,7 +23098,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>353</v>
       </c>
@@ -23119,7 +23113,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>354</v>
       </c>
@@ -23133,11 +23127,11 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="P18" t="s">
-        <v>482</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="J18" s="2" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>355</v>
       </c>
@@ -23152,7 +23146,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>356</v>
       </c>
@@ -23167,7 +23161,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>357</v>
       </c>
@@ -23184,11 +23178,11 @@
       <c r="F21">
         <v>30</v>
       </c>
-      <c r="P21" t="s">
-        <v>483</v>
-      </c>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="J21" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>358</v>
       </c>
@@ -23202,11 +23196,11 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="P22" t="s">
-        <v>484</v>
-      </c>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="J22" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>359</v>
       </c>
@@ -23221,7 +23215,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>360</v>
       </c>
@@ -23238,11 +23232,11 @@
       <c r="F24">
         <v>25</v>
       </c>
-      <c r="P24" t="s">
-        <v>485</v>
-      </c>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="J24" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>361</v>
       </c>
@@ -23259,11 +23253,11 @@
       <c r="F25">
         <v>12</v>
       </c>
-      <c r="P25" t="s">
-        <v>486</v>
-      </c>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="J25" s="2" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>362</v>
       </c>
@@ -23277,11 +23271,11 @@
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="P26" t="s">
-        <v>487</v>
-      </c>
-    </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="J26" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>363</v>
       </c>
@@ -23298,11 +23292,11 @@
       <c r="F27">
         <v>25</v>
       </c>
-      <c r="P27" t="s">
-        <v>488</v>
-      </c>
-    </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="J27" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>364</v>
       </c>
@@ -23316,11 +23310,11 @@
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="P28" t="s">
-        <v>489</v>
-      </c>
-    </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="J28" s="2" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>365</v>
       </c>
@@ -23337,11 +23331,11 @@
       <c r="F29">
         <v>20</v>
       </c>
-      <c r="P29" t="s">
-        <v>490</v>
-      </c>
-    </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="J29" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>366</v>
       </c>
@@ -23358,11 +23352,11 @@
       <c r="F30">
         <v>15</v>
       </c>
-      <c r="P30" t="s">
-        <v>491</v>
-      </c>
-    </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="J30" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>367</v>
       </c>
@@ -23379,11 +23373,11 @@
       <c r="F31">
         <v>35</v>
       </c>
-      <c r="P31" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="J31" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>368</v>
       </c>
@@ -23397,11 +23391,11 @@
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="P32" t="s">
-        <v>493</v>
-      </c>
-    </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="J32" s="2" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>369</v>
       </c>
@@ -23418,11 +23412,11 @@
       <c r="F33">
         <v>18</v>
       </c>
-      <c r="P33" t="s">
-        <v>494</v>
-      </c>
-    </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="J33" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>370</v>
       </c>
@@ -23439,11 +23433,11 @@
       <c r="F34">
         <v>13</v>
       </c>
-      <c r="P34" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="J34" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>371</v>
       </c>
@@ -23458,7 +23452,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>372</v>
       </c>
@@ -23475,11 +23469,11 @@
       <c r="F36">
         <v>30</v>
       </c>
-      <c r="P36" t="s">
-        <v>496</v>
-      </c>
-    </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="J36" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>373</v>
       </c>
@@ -23496,11 +23490,11 @@
       <c r="F37">
         <v>34</v>
       </c>
-      <c r="P37" t="s">
-        <v>497</v>
-      </c>
-    </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="J37" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>374</v>
       </c>
@@ -23514,11 +23508,11 @@
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="P38" t="s">
-        <v>498</v>
-      </c>
-    </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="J38" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>375</v>
       </c>
@@ -23533,7 +23527,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>376</v>
       </c>
@@ -23548,7 +23542,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>377</v>
       </c>
@@ -23565,11 +23559,11 @@
       <c r="F41">
         <v>20</v>
       </c>
-      <c r="P41" t="s">
-        <v>499</v>
-      </c>
-    </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="J41" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>378</v>
       </c>
@@ -23586,11 +23580,11 @@
       <c r="F42">
         <v>14</v>
       </c>
-      <c r="P42" s="2" t="s">
-        <v>469</v>
-      </c>
-    </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="J42" s="2" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>379</v>
       </c>
@@ -23607,11 +23601,11 @@
       <c r="F43" s="3">
         <v>75</v>
       </c>
-      <c r="P43" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="J43" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>380</v>
       </c>
@@ -23625,11 +23619,11 @@
         <f t="shared" si="0"/>
         <v>50</v>
       </c>
-      <c r="P44" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="J44" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>381</v>
       </c>
@@ -23646,11 +23640,11 @@
       <c r="F45">
         <v>34</v>
       </c>
-      <c r="P45" t="s">
-        <v>502</v>
-      </c>
-    </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="J45" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>382</v>
       </c>
@@ -23665,7 +23659,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>383</v>
       </c>
@@ -23682,11 +23676,11 @@
       <c r="F47">
         <v>20</v>
       </c>
-      <c r="P47" t="s">
-        <v>503</v>
-      </c>
-    </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="J47" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>384</v>
       </c>
@@ -23703,11 +23697,11 @@
       <c r="F48">
         <v>30</v>
       </c>
-      <c r="P48" t="s">
-        <v>504</v>
-      </c>
-    </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="J48" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>385</v>
       </c>
@@ -23722,7 +23716,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>386</v>
       </c>
@@ -23739,11 +23733,11 @@
       <c r="F50">
         <v>21</v>
       </c>
-      <c r="P50" t="s">
-        <v>505</v>
-      </c>
-    </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="J50" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>387</v>
       </c>
@@ -23760,11 +23754,11 @@
       <c r="F51">
         <v>12</v>
       </c>
-      <c r="P51" t="s">
-        <v>506</v>
-      </c>
-    </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="J51" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>388</v>
       </c>
@@ -23779,7 +23773,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>389</v>
       </c>
@@ -23794,7 +23788,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>390</v>
       </c>
@@ -23809,7 +23803,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>391</v>
       </c>
@@ -23824,7 +23818,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>392</v>
       </c>
@@ -23845,7 +23839,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>393</v>
       </c>
@@ -23860,7 +23854,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>394</v>
       </c>
@@ -23875,7 +23869,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>395</v>
       </c>
@@ -23890,7 +23884,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>396</v>
       </c>
@@ -23907,11 +23901,11 @@
       <c r="F60">
         <v>10</v>
       </c>
-      <c r="P60" t="s">
-        <v>507</v>
-      </c>
-    </row>
-    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="J60" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>397</v>
       </c>
@@ -23925,7 +23919,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="64" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>402</v>
       </c>
@@ -23941,22 +23935,10 @@
       <c r="H64" t="s">
         <v>399</v>
       </c>
-      <c r="I64" t="s">
-        <v>400</v>
-      </c>
-      <c r="J64" t="s">
-        <v>405</v>
-      </c>
-      <c r="K64" t="s">
-        <v>406</v>
-      </c>
-      <c r="L64">
-        <v>1</v>
-      </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="B65">
         <v>2</v>
@@ -23964,7 +23946,7 @@
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="B66">
         <v>2</v>
@@ -23972,7 +23954,7 @@
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="B67">
         <v>3</v>
@@ -23980,7 +23962,7 @@
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="B68">
         <v>1</v>
@@ -23988,7 +23970,7 @@
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="B69">
         <v>3</v>
@@ -23996,7 +23978,7 @@
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="B70">
         <v>3</v>
@@ -24004,7 +23986,7 @@
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="B71">
         <v>3</v>
@@ -24012,7 +23994,7 @@
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="B72">
         <v>3</v>
@@ -24020,7 +24002,7 @@
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="B73">
         <v>3</v>
@@ -24028,7 +24010,7 @@
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="B74">
         <v>3</v>
@@ -24036,7 +24018,7 @@
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="B75">
         <v>3</v>
@@ -24044,7 +24026,7 @@
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="B76">
         <v>3</v>
@@ -24052,7 +24034,7 @@
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="B77">
         <v>3</v>
@@ -24060,7 +24042,7 @@
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="B78">
         <v>3</v>
@@ -24068,7 +24050,7 @@
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="B79">
         <v>3</v>
@@ -24076,7 +24058,7 @@
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="B80">
         <v>2</v>
@@ -24084,7 +24066,7 @@
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="B81">
         <v>3</v>
@@ -24092,7 +24074,7 @@
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="B82">
         <v>3</v>
@@ -24100,7 +24082,7 @@
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="B83">
         <v>3</v>
@@ -24108,7 +24090,7 @@
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="B84">
         <v>3</v>
@@ -24116,7 +24098,7 @@
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="B85">
         <v>2</v>
@@ -24124,7 +24106,7 @@
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="B86">
         <v>2</v>
@@ -24132,7 +24114,7 @@
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="B87">
         <v>2</v>
@@ -24140,7 +24122,7 @@
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="B88">
         <v>3</v>
@@ -24148,7 +24130,7 @@
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="B89">
         <v>1</v>
@@ -24156,7 +24138,7 @@
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="B90">
         <v>1</v>
@@ -24164,7 +24146,7 @@
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="B91">
         <v>1</v>
@@ -24172,7 +24154,7 @@
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="B92">
         <v>1</v>
@@ -24180,7 +24162,7 @@
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="B93">
         <v>1</v>
@@ -24188,7 +24170,7 @@
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="B94">
         <v>1</v>
@@ -24196,7 +24178,7 @@
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="B95">
         <v>1</v>
@@ -24204,7 +24186,7 @@
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="B96">
         <v>1</v>
@@ -24212,7 +24194,7 @@
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="B97">
         <v>1</v>
@@ -24220,7 +24202,7 @@
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="B98">
         <v>1</v>
@@ -24228,7 +24210,7 @@
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="B99">
         <v>1</v>
@@ -24236,7 +24218,7 @@
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="B100">
         <v>1</v>
@@ -24244,7 +24226,7 @@
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="B101">
         <v>1</v>
@@ -24252,7 +24234,7 @@
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="B102">
         <v>1</v>
@@ -24260,7 +24242,7 @@
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="B103">
         <v>1</v>
@@ -24268,7 +24250,7 @@
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="B104">
         <v>1</v>
@@ -24276,7 +24258,7 @@
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="B105">
         <v>2</v>
@@ -24284,7 +24266,7 @@
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="B106">
         <v>3</v>
@@ -24292,7 +24274,7 @@
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="B107">
         <v>2</v>
@@ -24300,7 +24282,7 @@
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="B108">
         <v>2</v>
@@ -24308,7 +24290,7 @@
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="B109">
         <v>2</v>
@@ -24316,7 +24298,7 @@
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="B110">
         <v>2</v>
@@ -24324,7 +24306,7 @@
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="B111">
         <v>2</v>
@@ -24332,7 +24314,7 @@
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="B112">
         <v>2</v>
@@ -24340,7 +24322,7 @@
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="B113">
         <v>2</v>
@@ -24348,7 +24330,7 @@
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="B114">
         <v>2</v>
@@ -24356,7 +24338,7 @@
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="B115">
         <v>2</v>
@@ -24364,7 +24346,7 @@
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="B116">
         <v>1</v>
@@ -24372,7 +24354,7 @@
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="B117">
         <v>3</v>
@@ -24380,7 +24362,7 @@
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="B118">
         <v>2</v>
@@ -24388,7 +24370,7 @@
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="B119">
         <v>3</v>
@@ -24396,7 +24378,7 @@
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="B120">
         <v>3</v>
@@ -24404,7 +24386,7 @@
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="B121">
         <v>3</v>
@@ -24412,7 +24394,7 @@
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="B122">
         <v>3</v>
@@ -24420,7 +24402,7 @@
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="B123">
         <v>1</v>
@@ -24428,9 +24410,13 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="P3" r:id="rId1"/>
-    <hyperlink ref="P8" r:id="rId2"/>
-    <hyperlink ref="P42" r:id="rId3"/>
+    <hyperlink ref="J3" r:id="rId1"/>
+    <hyperlink ref="J8" r:id="rId2"/>
+    <hyperlink ref="J42" r:id="rId3"/>
+    <hyperlink ref="J28" r:id="rId4"/>
+    <hyperlink ref="J25" r:id="rId5"/>
+    <hyperlink ref="J18" r:id="rId6"/>
+    <hyperlink ref="J32" r:id="rId7"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
desktop changes, details to mum and C xls workbook'
</commit_message>
<xml_diff>
--- a/R/C_and_Mum.xlsx
+++ b/R/C_and_Mum.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="815" activeTab="10"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="815" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="C_v1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1975" uniqueCount="805">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2018" uniqueCount="848">
   <si>
     <t>FPL</t>
   </si>
@@ -1434,9 +1434,6 @@
     <t>max age</t>
   </si>
   <si>
-    <t>max should be…</t>
-  </si>
-  <si>
     <t>http://www.fishbase.org/summary/Limanda-ferruginea.html</t>
   </si>
   <si>
@@ -2449,6 +2446,138 @@
   </si>
   <si>
     <t>20180613dt</t>
+  </si>
+  <si>
+    <t>max size (cm)</t>
+  </si>
+  <si>
+    <t>max weight (g)</t>
+  </si>
+  <si>
+    <t>max age (y)</t>
+  </si>
+  <si>
+    <t>common size (cm)</t>
+  </si>
+  <si>
+    <t>mum_PL_T15       0.4       Maximum growth rate, large phytoplankton (was 0.85) d-1          1.0 - 1.7</t>
+  </si>
+  <si>
+    <t>mum_PS_T15       0.05      Maximum growth rate, small (pico) phytoplankton (was 0.5 then 0.25)  d-1   1.0 - 1.24</t>
+  </si>
+  <si>
+    <t>mum_DF_T15       0.09      Maximum growth rate, dinoflagellates (was 0.51)   d-1            1.0 - 1.24</t>
+  </si>
+  <si>
+    <t>mum_MA_T15       0.1       Maximum growth rate, macroalgae                   d-1               0.1</t>
+  </si>
+  <si>
+    <t>mum_SG_T15       0.07      Maximum growth rate, seagrass                     d-1  (0.07)       0.05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mum_MB_T15       0.18 </t>
+  </si>
+  <si>
+    <t>mum_ZG_T15       0.017     Growth rate of gelatinous zooplankton              mg N d-1      0.02 - 0.35</t>
+  </si>
+  <si>
+    <t>mum_ZL_T15       0.1       Growth rate of largezooplankton (0.04)             mg N d-1      0.02 - 0.35</t>
+  </si>
+  <si>
+    <t>mum_ZM_T15       0.18      Growth rate of meso-zooplankton                    mg N d-1       0.3 - 1.4</t>
+  </si>
+  <si>
+    <t>mum_ZS_T15       0.55      Growth rate of microzooplankton                    mg N d-1       0.5 - 2.5</t>
+  </si>
+  <si>
+    <t>mum_BFS_T15      0.05      Growth rate of shallow filter feeders (0.22)       mg N d-1          0.01</t>
+  </si>
+  <si>
+    <t>mum_BFD_T15      0.0075    Growth rate of deep filter feeders                 mg N d-1          0.01</t>
+  </si>
+  <si>
+    <t>mum_BFF_T15      0.0035    Growth rate of other filter feeders                mg N d-1          0.01</t>
+  </si>
+  <si>
+    <t>mum_BD_T15       0.004     Growth rate of deposit feeders                     mg N d-1      0.005 - 0.07</t>
+  </si>
+  <si>
+    <t>mum_BC_T15       0.0008    Growth rate of infaunal carnivores (0.005)         mg N d-1      0.005 - 0.06</t>
+  </si>
+  <si>
+    <t>mum_BG_T15       0.002     Growth rate of benthic grazers                     mg N d-1      0.001 - 0.01</t>
+  </si>
+  <si>
+    <t>mum_BMS_T15      0.0001    Growth rate of shallow macrozoobenthos             mg N d-1      0.0015 - 0.015</t>
+  </si>
+  <si>
+    <t>mum_BML_T15      0.00012   Growth rate of megazoobenthos (0.00005)            mg N d-1      0.0015 - 0.015</t>
+  </si>
+  <si>
+    <t>mum_BMD_T15      0.0008    Growth rate of deep macrozoobenthos                mg N d-1      0.0015 - 0.015</t>
+  </si>
+  <si>
+    <t>mum_BO_T15       0.04      Growth rate of meiobenthos                         mg N d-1          0.3</t>
+  </si>
+  <si>
+    <t>mum_PB_T15       1.5       Growth rate of pelagic bacteria                    mg N d-1       1.0 - 2.0</t>
+  </si>
+  <si>
+    <t>mum_BB_T15       1.5       Growth rate of sediment bacteria                   mg N d-1       1.0 - 2.0</t>
+  </si>
+  <si>
+    <t>mum_CEP_T15      0.0444   Growth rate of cephalopods (0.08)                  mg N d-1      0.02 - 0.35</t>
+  </si>
+  <si>
+    <t>mum_jCEP_T15     0.046   Growth rate of juvenile cephalopods (0.08)         mg N d-1      0.02 - 0.35</t>
+  </si>
+  <si>
+    <t>mum_PWN_T15      0.003043 Growth rate of prawns (0.00195)                    mg N d-1      0.0015 - 0.015</t>
+  </si>
+  <si>
+    <t>mum_jPWN_T15     0.003043 Growth rate of juvenile prawns (0.00195)           mg N d-1      0.0015 - 0.015</t>
+  </si>
+  <si>
+    <t>http://wrec.igfa.org/WRecDetail.aspx?uid=18806&amp;cn=Flounder,%20summer#.Wyln61VKhaQ</t>
+  </si>
+  <si>
+    <t>http://wrec.igfa.org/WRecDetail.aspx?uid=18966&amp;cn=Hake,%20white#.WylnwlVKhaQ</t>
+  </si>
+  <si>
+    <t>http://wrec.igfa.org/WRecDetail.aspx?uid=24505&amp;cn=Drum,%20red#.WylppFVKhaQ</t>
+  </si>
+  <si>
+    <t>Other source</t>
+  </si>
+  <si>
+    <t>https://www.fishbase.de/Summary/SpeciesSummary.php?ID=545&amp;AT=bay+anchovy</t>
+  </si>
+  <si>
+    <t>https://www.fishbase.de/Summary/SpeciesSummary.php?ID=1133&amp;AT=striped+anchovy</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/American_butterfish</t>
+  </si>
+  <si>
+    <t>http://southshorefishing.net/fish/windowpane.htm</t>
+  </si>
+  <si>
+    <t>http://www.gma.org/fogm/brevoortia_tyrannus.htm</t>
+  </si>
+  <si>
+    <t>http://www.gma.org/fogm/Poronotus_triacanthus.htm</t>
+  </si>
+  <si>
+    <t>https://www.fisheries.noaa.gov/species/acadian-redfish</t>
+  </si>
+  <si>
+    <t>http://wrec.igfa.org/WRecDetail.aspx?uid=35875&amp;cn=Redfish,%20acadian#.WylwQlVKhaQ</t>
+  </si>
+  <si>
+    <t>http://www.dfo-mpo.gc.ca/species-especes/skates/species/winter-eng.html</t>
+  </si>
+  <si>
+    <t>https://www.floridamuseum.ufl.edu/fish/discover/species-profiles/squalus-acanthias/</t>
   </si>
 </sst>
 </file>
@@ -2811,13 +2940,13 @@
   <sheetData>
     <row r="2" spans="2:37" x14ac:dyDescent="0.25">
       <c r="F2" t="s">
+        <v>799</v>
+      </c>
+      <c r="Q2" t="s">
         <v>800</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="AB2" t="s">
         <v>801</v>
-      </c>
-      <c r="AB2" t="s">
-        <v>802</v>
       </c>
     </row>
     <row r="4" spans="2:37" x14ac:dyDescent="0.25">
@@ -7236,19 +7365,23 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J123"/>
+  <dimension ref="A1:AA123"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="H43" sqref="H43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B1">
         <v>20180419</v>
       </c>
@@ -7259,13 +7392,25 @@
         <v>465</v>
       </c>
       <c r="F1" t="s">
-        <v>466</v>
+        <v>806</v>
+      </c>
+      <c r="G1" t="s">
+        <v>805</v>
+      </c>
+      <c r="H1" t="s">
+        <v>804</v>
+      </c>
+      <c r="I1" t="s">
+        <v>807</v>
       </c>
       <c r="J1" t="s">
-        <v>469</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+        <v>468</v>
+      </c>
+      <c r="T1" t="s">
+        <v>837</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>338</v>
       </c>
@@ -7282,11 +7427,20 @@
       <c r="F2">
         <v>17</v>
       </c>
+      <c r="G2">
+        <v>3400</v>
+      </c>
+      <c r="H2">
+        <v>60</v>
+      </c>
+      <c r="I2">
+        <v>30</v>
+      </c>
       <c r="J2" s="2" t="s">
-        <v>506</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>339</v>
       </c>
@@ -7303,11 +7457,20 @@
       <c r="F3">
         <v>25</v>
       </c>
+      <c r="G3">
+        <v>1100</v>
+      </c>
+      <c r="H3">
+        <v>45</v>
+      </c>
+      <c r="I3">
+        <v>30</v>
+      </c>
       <c r="J3" s="2" t="s">
-        <v>472</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>340</v>
       </c>
@@ -7324,11 +7487,20 @@
       <c r="F4">
         <v>23</v>
       </c>
-      <c r="J4" t="s">
-        <v>470</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G4">
+        <v>21000</v>
+      </c>
+      <c r="H4">
+        <v>133</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>469</v>
+      </c>
+      <c r="T4" s="2" t="s">
+        <v>835</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>341</v>
       </c>
@@ -7345,11 +7517,20 @@
       <c r="F5">
         <v>9</v>
       </c>
-      <c r="J5" t="s">
-        <v>468</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G5">
+        <v>14400</v>
+      </c>
+      <c r="H5">
+        <v>130</v>
+      </c>
+      <c r="I5">
+        <v>60</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>342</v>
       </c>
@@ -7366,11 +7547,20 @@
       <c r="F6">
         <v>7</v>
       </c>
-      <c r="J6" t="s">
-        <v>473</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G6">
+        <v>910</v>
+      </c>
+      <c r="H6">
+        <v>46</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>472</v>
+      </c>
+      <c r="T6" s="2" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>343</v>
       </c>
@@ -7387,11 +7577,23 @@
       <c r="F7">
         <v>9</v>
       </c>
-      <c r="J7" t="s">
-        <v>476</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G7">
+        <v>10170</v>
+      </c>
+      <c r="H7">
+        <v>89</v>
+      </c>
+      <c r="I7">
+        <v>40</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>475</v>
+      </c>
+      <c r="T7" s="2" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>344</v>
       </c>
@@ -7408,11 +7610,17 @@
       <c r="F8">
         <v>14</v>
       </c>
+      <c r="G8">
+        <v>3600</v>
+      </c>
+      <c r="H8">
+        <v>64</v>
+      </c>
       <c r="J8" s="2" t="s">
-        <v>474</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>345</v>
       </c>
@@ -7429,11 +7637,17 @@
       <c r="F9">
         <v>25</v>
       </c>
-      <c r="J9" t="s">
-        <v>475</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G9">
+        <v>2500</v>
+      </c>
+      <c r="H9">
+        <v>60</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>346</v>
       </c>
@@ -7450,11 +7664,17 @@
       <c r="F10">
         <v>50</v>
       </c>
-      <c r="J10" t="s">
-        <v>471</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G10">
+        <v>320000</v>
+      </c>
+      <c r="H10">
+        <v>470</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>347</v>
       </c>
@@ -7471,11 +7691,17 @@
       <c r="F11">
         <v>30</v>
       </c>
-      <c r="J11" t="s">
-        <v>477</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G11">
+        <v>6400</v>
+      </c>
+      <c r="H11">
+        <v>82.6</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>348</v>
       </c>
@@ -7489,11 +7715,17 @@
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="J12" t="s">
-        <v>478</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G12">
+        <v>750</v>
+      </c>
+      <c r="H12">
+        <v>43</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>349</v>
       </c>
@@ -7508,7 +7740,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>350</v>
       </c>
@@ -7525,11 +7757,20 @@
       <c r="F14">
         <v>32</v>
       </c>
-      <c r="J14" t="s">
-        <v>479</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G14">
+        <v>684000</v>
+      </c>
+      <c r="H14">
+        <v>458</v>
+      </c>
+      <c r="I14">
+        <v>200</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>351</v>
       </c>
@@ -7544,7 +7785,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>352</v>
       </c>
@@ -7559,7 +7800,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>353</v>
       </c>
@@ -7574,7 +7815,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>354</v>
       </c>
@@ -7588,11 +7829,26 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
+      <c r="G18">
+        <v>567</v>
+      </c>
+      <c r="H18">
+        <v>30</v>
+      </c>
+      <c r="I18">
+        <v>20</v>
+      </c>
       <c r="J18" s="2" t="s">
-        <v>480</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+        <v>479</v>
+      </c>
+      <c r="T18" s="2" t="s">
+        <v>840</v>
+      </c>
+      <c r="Z18" s="2" t="s">
+        <v>843</v>
+      </c>
+    </row>
+    <row r="19" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>355</v>
       </c>
@@ -7606,8 +7862,26 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F19">
+        <v>5</v>
+      </c>
+      <c r="G19">
+        <v>50</v>
+      </c>
+      <c r="H19">
+        <v>15</v>
+      </c>
+      <c r="I19">
+        <v>10</v>
+      </c>
+      <c r="J19" s="2" t="s">
+        <v>838</v>
+      </c>
+      <c r="T19" s="2" t="s">
+        <v>839</v>
+      </c>
+    </row>
+    <row r="20" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>356</v>
       </c>
@@ -7622,7 +7896,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>357</v>
       </c>
@@ -7639,11 +7913,20 @@
       <c r="F21">
         <v>30</v>
       </c>
-      <c r="J21" t="s">
-        <v>481</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G21">
+        <v>22600</v>
+      </c>
+      <c r="H21">
+        <v>120</v>
+      </c>
+      <c r="I21">
+        <v>90</v>
+      </c>
+      <c r="J21" s="2" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="22" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>358</v>
       </c>
@@ -7657,11 +7940,23 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="J22" t="s">
-        <v>482</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G22">
+        <v>822</v>
+      </c>
+      <c r="H22">
+        <v>50</v>
+      </c>
+      <c r="I22">
+        <v>25</v>
+      </c>
+      <c r="J22" s="2" t="s">
+        <v>481</v>
+      </c>
+      <c r="T22" s="2" t="s">
+        <v>842</v>
+      </c>
+    </row>
+    <row r="23" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>359</v>
       </c>
@@ -7676,7 +7971,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>360</v>
       </c>
@@ -7693,11 +7988,20 @@
       <c r="F24">
         <v>25</v>
       </c>
-      <c r="J24" t="s">
-        <v>483</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G24">
+        <v>96000</v>
+      </c>
+      <c r="H24">
+        <v>200</v>
+      </c>
+      <c r="I24">
+        <v>100</v>
+      </c>
+      <c r="J24" s="2" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="25" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>361</v>
       </c>
@@ -7714,11 +8018,20 @@
       <c r="F25">
         <v>12</v>
       </c>
+      <c r="G25">
+        <v>2300</v>
+      </c>
+      <c r="H25">
+        <v>76</v>
+      </c>
+      <c r="I25">
+        <v>37</v>
+      </c>
       <c r="J25" s="2" t="s">
-        <v>484</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="26" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>362</v>
       </c>
@@ -7732,11 +8045,17 @@
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="J26" t="s">
-        <v>485</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H26">
+        <v>70</v>
+      </c>
+      <c r="I26">
+        <v>30</v>
+      </c>
+      <c r="J26" s="2" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="27" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>363</v>
       </c>
@@ -7753,11 +8072,20 @@
       <c r="F27">
         <v>25</v>
       </c>
-      <c r="J27" t="s">
-        <v>486</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G27">
+        <v>32000</v>
+      </c>
+      <c r="H27">
+        <v>130</v>
+      </c>
+      <c r="I27">
+        <v>60</v>
+      </c>
+      <c r="J27" s="2" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="28" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>364</v>
       </c>
@@ -7771,11 +8099,17 @@
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
+      <c r="G28">
+        <v>3600</v>
+      </c>
+      <c r="H28">
+        <v>66</v>
+      </c>
       <c r="J28" s="2" t="s">
-        <v>487</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="29" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>365</v>
       </c>
@@ -7792,11 +8126,20 @@
       <c r="F29">
         <v>20</v>
       </c>
-      <c r="J29" t="s">
-        <v>488</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G29">
+        <v>4300</v>
+      </c>
+      <c r="H29">
+        <v>66</v>
+      </c>
+      <c r="I29">
+        <v>30</v>
+      </c>
+      <c r="J29" s="2" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="30" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>366</v>
       </c>
@@ -7813,11 +8156,20 @@
       <c r="F30">
         <v>15</v>
       </c>
-      <c r="J30" t="s">
-        <v>489</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G30">
+        <v>2100</v>
+      </c>
+      <c r="H30">
+        <v>46</v>
+      </c>
+      <c r="I30">
+        <v>25</v>
+      </c>
+      <c r="J30" s="2" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="31" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>367</v>
       </c>
@@ -7834,11 +8186,20 @@
       <c r="F31">
         <v>35</v>
       </c>
-      <c r="J31" t="s">
-        <v>490</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G31">
+        <v>30000</v>
+      </c>
+      <c r="H31">
+        <v>125</v>
+      </c>
+      <c r="I31">
+        <v>90</v>
+      </c>
+      <c r="J31" s="2" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="32" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>368</v>
       </c>
@@ -7852,11 +8213,26 @@
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
+      <c r="F32">
+        <v>50</v>
+      </c>
+      <c r="G32">
+        <v>1130</v>
+      </c>
+      <c r="H32">
+        <v>50.8</v>
+      </c>
       <c r="J32" s="2" t="s">
-        <v>491</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+        <v>490</v>
+      </c>
+      <c r="T32" s="2" t="s">
+        <v>844</v>
+      </c>
+      <c r="AA32" s="2" t="s">
+        <v>845</v>
+      </c>
+    </row>
+    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>369</v>
       </c>
@@ -7873,11 +8249,17 @@
       <c r="F33">
         <v>18</v>
       </c>
-      <c r="J33" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G33">
+        <v>5400</v>
+      </c>
+      <c r="H33">
+        <v>110</v>
+      </c>
+      <c r="J33" s="2" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>370</v>
       </c>
@@ -7894,11 +8276,20 @@
       <c r="F34">
         <v>13</v>
       </c>
-      <c r="J34" t="s">
-        <v>493</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G34">
+        <v>46800</v>
+      </c>
+      <c r="H34">
+        <v>150</v>
+      </c>
+      <c r="I34">
+        <v>30</v>
+      </c>
+      <c r="J34" s="2" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>371</v>
       </c>
@@ -7912,8 +8303,17 @@
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G35">
+        <v>43000</v>
+      </c>
+      <c r="H35">
+        <v>145</v>
+      </c>
+      <c r="T35" s="2" t="s">
+        <v>836</v>
+      </c>
+    </row>
+    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>372</v>
       </c>
@@ -7930,11 +8330,20 @@
       <c r="F36">
         <v>30</v>
       </c>
-      <c r="J36" t="s">
-        <v>494</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G36">
+        <v>57000</v>
+      </c>
+      <c r="H36">
+        <v>200</v>
+      </c>
+      <c r="I36">
+        <v>120</v>
+      </c>
+      <c r="J36" s="2" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>373</v>
       </c>
@@ -7951,11 +8360,17 @@
       <c r="F37">
         <v>34</v>
       </c>
-      <c r="J37" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G37">
+        <v>11300</v>
+      </c>
+      <c r="H37">
+        <v>91</v>
+      </c>
+      <c r="J37" s="2" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>374</v>
       </c>
@@ -7969,11 +8384,17 @@
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="J38" t="s">
-        <v>496</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G38">
+        <v>23600</v>
+      </c>
+      <c r="H38">
+        <v>150</v>
+      </c>
+      <c r="J38" s="2" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>375</v>
       </c>
@@ -7988,7 +8409,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>376</v>
       </c>
@@ -8003,7 +8424,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>377</v>
       </c>
@@ -8020,11 +8441,20 @@
       <c r="F41">
         <v>20</v>
       </c>
-      <c r="J41" t="s">
-        <v>497</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G41">
+        <v>16800</v>
+      </c>
+      <c r="H41">
+        <v>112</v>
+      </c>
+      <c r="I41">
+        <v>35</v>
+      </c>
+      <c r="J41" s="2" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>378</v>
       </c>
@@ -8041,11 +8471,17 @@
       <c r="F42">
         <v>14</v>
       </c>
+      <c r="G42">
+        <v>1500</v>
+      </c>
+      <c r="H42">
+        <v>64</v>
+      </c>
       <c r="J42" s="2" t="s">
-        <v>467</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>379</v>
       </c>
@@ -8060,13 +8496,25 @@
         <v>40</v>
       </c>
       <c r="F43" s="3">
-        <v>75</v>
-      </c>
-      <c r="J43" t="s">
-        <v>498</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+      <c r="G43">
+        <v>9100</v>
+      </c>
+      <c r="H43">
+        <v>160</v>
+      </c>
+      <c r="I43">
+        <v>100</v>
+      </c>
+      <c r="J43" s="2" t="s">
+        <v>497</v>
+      </c>
+      <c r="T43" s="2" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>380</v>
       </c>
@@ -8080,11 +8528,20 @@
         <f t="shared" si="0"/>
         <v>50</v>
       </c>
-      <c r="J44" t="s">
-        <v>499</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G44">
+        <v>12200</v>
+      </c>
+      <c r="H44">
+        <v>150</v>
+      </c>
+      <c r="I44">
+        <v>100</v>
+      </c>
+      <c r="J44" s="2" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>381</v>
       </c>
@@ -8101,11 +8558,20 @@
       <c r="F45">
         <v>34</v>
       </c>
-      <c r="J45" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G45">
+        <v>118000</v>
+      </c>
+      <c r="H45">
+        <v>250</v>
+      </c>
+      <c r="I45">
+        <v>200</v>
+      </c>
+      <c r="J45" s="2" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>382</v>
       </c>
@@ -8120,7 +8586,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>383</v>
       </c>
@@ -8137,11 +8603,20 @@
       <c r="F47">
         <v>20</v>
       </c>
-      <c r="J47" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G47">
+        <v>206000</v>
+      </c>
+      <c r="H47">
+        <v>400</v>
+      </c>
+      <c r="I47">
+        <v>335</v>
+      </c>
+      <c r="J47" s="2" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="48" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>384</v>
       </c>
@@ -8158,11 +8633,20 @@
       <c r="F48">
         <v>30</v>
       </c>
-      <c r="J48" t="s">
-        <v>502</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G48">
+        <v>230000</v>
+      </c>
+      <c r="H48">
+        <v>350</v>
+      </c>
+      <c r="I48">
+        <v>244</v>
+      </c>
+      <c r="J48" s="2" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="49" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>385</v>
       </c>
@@ -8177,7 +8661,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>386</v>
       </c>
@@ -8194,11 +8678,17 @@
       <c r="F50">
         <v>21</v>
       </c>
-      <c r="J50" t="s">
-        <v>503</v>
-      </c>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H50">
+        <v>110</v>
+      </c>
+      <c r="J50" s="2" t="s">
+        <v>502</v>
+      </c>
+      <c r="T50" s="2" t="s">
+        <v>846</v>
+      </c>
+    </row>
+    <row r="51" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>387</v>
       </c>
@@ -8215,11 +8705,14 @@
       <c r="F51">
         <v>12</v>
       </c>
-      <c r="J51" t="s">
-        <v>504</v>
-      </c>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H51">
+        <v>54</v>
+      </c>
+      <c r="J51" s="2" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="52" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>388</v>
       </c>
@@ -8234,7 +8727,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>389</v>
       </c>
@@ -8249,7 +8742,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>390</v>
       </c>
@@ -8264,7 +8757,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>391</v>
       </c>
@@ -8279,7 +8772,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>392</v>
       </c>
@@ -8300,7 +8793,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>393</v>
       </c>
@@ -8315,7 +8808,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>394</v>
       </c>
@@ -8330,7 +8823,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>395</v>
       </c>
@@ -8345,7 +8838,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>396</v>
       </c>
@@ -8362,11 +8855,14 @@
       <c r="F60">
         <v>10</v>
       </c>
-      <c r="J60" t="s">
-        <v>505</v>
-      </c>
-    </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H60">
+        <v>38</v>
+      </c>
+      <c r="J60" s="2" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="63" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>397</v>
       </c>
@@ -8380,7 +8876,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>402</v>
       </c>
@@ -8870,6 +9366,34 @@
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="H2:H60">
+    <cfRule type="dataBar" priority="2">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF555A"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{121280B2-F02C-4BC7-B69E-FB5E1DA1B528}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G2:G60">
+    <cfRule type="dataBar" priority="1">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF008AEF"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{355C23AE-1761-4CE8-AD0F-2676FEA5D63C}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="J3" r:id="rId1"/>
     <hyperlink ref="J8" r:id="rId2"/>
@@ -8879,8 +9403,84 @@
     <hyperlink ref="J18" r:id="rId6"/>
     <hyperlink ref="J32" r:id="rId7"/>
     <hyperlink ref="J2" r:id="rId8"/>
+    <hyperlink ref="J4" r:id="rId9"/>
+    <hyperlink ref="J5" r:id="rId10"/>
+    <hyperlink ref="J6" r:id="rId11"/>
+    <hyperlink ref="J7" r:id="rId12"/>
+    <hyperlink ref="J9" r:id="rId13"/>
+    <hyperlink ref="J10" r:id="rId14"/>
+    <hyperlink ref="J11" r:id="rId15"/>
+    <hyperlink ref="J12" r:id="rId16"/>
+    <hyperlink ref="J14" r:id="rId17"/>
+    <hyperlink ref="J21" r:id="rId18"/>
+    <hyperlink ref="J22" r:id="rId19"/>
+    <hyperlink ref="J24" r:id="rId20"/>
+    <hyperlink ref="J26" r:id="rId21"/>
+    <hyperlink ref="J27" r:id="rId22"/>
+    <hyperlink ref="J29" r:id="rId23"/>
+    <hyperlink ref="J30" r:id="rId24"/>
+    <hyperlink ref="J31" r:id="rId25"/>
+    <hyperlink ref="J33" r:id="rId26"/>
+    <hyperlink ref="J34" r:id="rId27"/>
+    <hyperlink ref="J36" r:id="rId28"/>
+    <hyperlink ref="J37" r:id="rId29"/>
+    <hyperlink ref="J38" r:id="rId30"/>
+    <hyperlink ref="J41" r:id="rId31"/>
+    <hyperlink ref="J43" r:id="rId32"/>
+    <hyperlink ref="J44" r:id="rId33"/>
+    <hyperlink ref="J45" r:id="rId34"/>
+    <hyperlink ref="J47" r:id="rId35"/>
+    <hyperlink ref="J48" r:id="rId36"/>
+    <hyperlink ref="J50" r:id="rId37"/>
+    <hyperlink ref="J51" r:id="rId38"/>
+    <hyperlink ref="J60" r:id="rId39"/>
+    <hyperlink ref="T7" r:id="rId40" location=".Wyln61VKhaQ"/>
+    <hyperlink ref="T4" r:id="rId41" location=".WylnwlVKhaQ"/>
+    <hyperlink ref="T35" r:id="rId42" location=".WylppFVKhaQ"/>
+    <hyperlink ref="J19" r:id="rId43"/>
+    <hyperlink ref="T19" r:id="rId44"/>
+    <hyperlink ref="T18" r:id="rId45"/>
+    <hyperlink ref="T6" r:id="rId46"/>
+    <hyperlink ref="T22" r:id="rId47"/>
+    <hyperlink ref="Z18" r:id="rId48"/>
+    <hyperlink ref="T32" r:id="rId49"/>
+    <hyperlink ref="AA32" r:id="rId50" location=".WylwQlVKhaQ"/>
+    <hyperlink ref="T50" r:id="rId51"/>
+    <hyperlink ref="T43" r:id="rId52"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{121280B2-F02C-4BC7-B69E-FB5E1DA1B528}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FFFF555A"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>H2:H60</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{355C23AE-1761-4CE8-AD0F-2676FEA5D63C}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF008AEF"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>G2:G60</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -8888,7 +9488,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B173"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A127" workbookViewId="0">
+    <sheetView topLeftCell="A127" workbookViewId="0">
       <selection activeCell="B142" sqref="B142"/>
     </sheetView>
   </sheetViews>
@@ -8899,7 +9499,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="B1" s="1">
         <v>1.0000000000000001E-5</v>
@@ -8907,7 +9507,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="B2" s="1">
         <v>1.0000000000000001E-5</v>
@@ -8915,7 +9515,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="B3" s="1">
         <v>1.0000000000000001E-5</v>
@@ -8923,7 +9523,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B4" s="1">
         <v>1.0000000000000001E-5</v>
@@ -8931,7 +9531,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="B5" s="1">
         <v>1.0000000000000001E-5</v>
@@ -8939,7 +9539,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="B6" s="1">
         <v>1.0000000000000001E-5</v>
@@ -8947,7 +9547,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="B7" s="1">
         <v>1.0000000000000001E-5</v>
@@ -8955,7 +9555,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="B8" s="1">
         <v>1.0000000000000001E-5</v>
@@ -8963,7 +9563,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="B9" s="1">
         <v>1.0000000000000001E-5</v>
@@ -8971,7 +9571,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="B10" s="1">
         <v>1.0000000000000001E-5</v>
@@ -8979,7 +9579,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="B11" s="1">
         <v>1.0000000000000001E-5</v>
@@ -8987,7 +9587,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="B12" s="1">
         <v>1.0000000000000001E-5</v>
@@ -8995,7 +9595,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="B13" s="1">
         <v>1.0000000000000001E-5</v>
@@ -9003,7 +9603,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="B14" s="1">
         <v>1.0000000000000001E-5</v>
@@ -9011,7 +9611,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="B15" s="1">
         <v>1.0000000000000001E-5</v>
@@ -9019,7 +9619,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="B16" s="1">
         <v>1.0000000000000001E-5</v>
@@ -9027,7 +9627,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="B17" s="1">
         <v>1.0000000000000001E-5</v>
@@ -9035,7 +9635,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="B18" s="1">
         <v>1.0000000000000001E-5</v>
@@ -9043,7 +9643,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="B19" s="1">
         <v>1.0000000000000001E-5</v>
@@ -9051,7 +9651,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="B20" s="1">
         <v>1E-4</v>
@@ -9059,7 +9659,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="B21" s="1">
         <v>1.0000000000000001E-5</v>
@@ -9067,7 +9667,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="B22" s="1">
         <v>1.0000000000000001E-5</v>
@@ -9075,7 +9675,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="B23" s="1">
         <v>1.0000000000000001E-5</v>
@@ -9083,7 +9683,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="B24" s="1">
         <v>1.0000000000000001E-5</v>
@@ -9091,7 +9691,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="B25" s="1">
         <v>1.0000000000000001E-5</v>
@@ -9099,7 +9699,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="B26" s="1">
         <v>1.0000000000000001E-5</v>
@@ -9107,7 +9707,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="B27" s="1">
         <v>1.0000000000000001E-5</v>
@@ -9115,7 +9715,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="B28" s="1">
         <v>1.0000000000000001E-5</v>
@@ -9123,7 +9723,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="B29" s="1">
         <v>1.0000000000000001E-5</v>
@@ -9131,7 +9731,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="B30" s="1">
         <v>1.0000000000000001E-5</v>
@@ -9139,7 +9739,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="B31" s="1">
         <v>1.0000000000000001E-5</v>
@@ -9147,7 +9747,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="B32" s="1">
         <v>1.0000000000000001E-5</v>
@@ -9155,7 +9755,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="B33" s="1">
         <v>1.0000000000000001E-5</v>
@@ -9163,7 +9763,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="B34" s="1">
         <v>1.0000000000000001E-5</v>
@@ -9171,7 +9771,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="B35" s="1">
         <v>1.0000000000000001E-5</v>
@@ -9179,7 +9779,7 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="B36" s="1">
         <v>1.0000000000000001E-5</v>
@@ -9187,7 +9787,7 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="B37" s="1">
         <v>1.0000000000000001E-5</v>
@@ -9195,7 +9795,7 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="B38" s="1">
         <v>1.0000000000000001E-5</v>
@@ -9203,7 +9803,7 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B39" s="1">
         <v>1.0000000000000001E-5</v>
@@ -9211,7 +9811,7 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="B40" s="1">
         <v>1.0000000000000001E-5</v>
@@ -9219,7 +9819,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="B41" s="1">
         <v>1.0000000000000001E-5</v>
@@ -9227,7 +9827,7 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="B42" s="1">
         <v>1E-4</v>
@@ -9235,7 +9835,7 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="B43" s="1">
         <v>1E-4</v>
@@ -9243,7 +9843,7 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="B44" s="1">
         <v>1E-4</v>
@@ -9251,7 +9851,7 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="B45" s="1">
         <v>1E-4</v>
@@ -9259,7 +9859,7 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="B46" s="1">
         <v>1E-4</v>
@@ -9267,7 +9867,7 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="B47" s="1">
         <v>1E-4</v>
@@ -9275,7 +9875,7 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="B48" s="1">
         <v>1E-4</v>
@@ -9283,7 +9883,7 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="B49" s="1">
         <v>1E-4</v>
@@ -9291,7 +9891,7 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="B50" s="1">
         <v>1E-4</v>
@@ -9299,7 +9899,7 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="B51" s="1">
         <v>1E-4</v>
@@ -9307,7 +9907,7 @@
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="B52" s="1">
         <v>1E-4</v>
@@ -9315,7 +9915,7 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="B53" s="1">
         <v>1.0000000000000001E-5</v>
@@ -9323,7 +9923,7 @@
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="B54" s="1">
         <v>1.0000000000000001E-5</v>
@@ -9331,7 +9931,7 @@
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="B55" s="1">
         <v>1E-10</v>
@@ -9339,7 +9939,7 @@
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="B56" s="1">
         <v>1E-10</v>
@@ -9347,7 +9947,7 @@
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="B57" s="1">
         <v>9.9999999999999995E-8</v>
@@ -9355,7 +9955,7 @@
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="B58" s="1">
         <v>9.9999999999999995E-8</v>
@@ -9363,7 +9963,7 @@
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="B59" s="1">
         <v>1.0000000000000001E-5</v>
@@ -9371,7 +9971,7 @@
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="B60" s="1">
         <v>9.9999999999999995E-8</v>
@@ -9379,7 +9979,7 @@
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="B61" s="1">
         <v>9.9999999999999995E-8</v>
@@ -9387,7 +9987,7 @@
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="B62">
         <v>0</v>
@@ -9395,7 +9995,7 @@
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="B63">
         <v>0</v>
@@ -9403,7 +10003,7 @@
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="B64">
         <v>0</v>
@@ -9411,7 +10011,7 @@
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="B65">
         <v>0</v>
@@ -9419,7 +10019,7 @@
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="B66">
         <v>0</v>
@@ -9427,7 +10027,7 @@
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="B67" s="1">
         <v>9.9999999999999995E-8</v>
@@ -9435,7 +10035,7 @@
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="B68" s="1">
         <v>9.9999999999999995E-8</v>
@@ -9443,7 +10043,7 @@
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="B69" s="1">
         <v>9.9999999999999995E-8</v>
@@ -9451,7 +10051,7 @@
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="B70" s="1">
         <v>9.9999999999999995E-8</v>
@@ -9459,7 +10059,7 @@
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="B71" s="1">
         <v>9.9999999999999995E-8</v>
@@ -9467,7 +10067,7 @@
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="B72">
         <v>0</v>
@@ -9475,7 +10075,7 @@
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="B73">
         <v>0</v>
@@ -9483,7 +10083,7 @@
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="B74">
         <v>0</v>
@@ -9491,7 +10091,7 @@
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="B75">
         <v>0</v>
@@ -9499,7 +10099,7 @@
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="B76">
         <v>0</v>
@@ -9507,7 +10107,7 @@
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="B77">
         <v>0</v>
@@ -9515,7 +10115,7 @@
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="B78" s="1">
         <v>9.9999999999999995E-8</v>
@@ -9523,7 +10123,7 @@
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="B79">
         <v>0</v>
@@ -9531,7 +10131,7 @@
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="B80">
         <v>0</v>
@@ -9539,7 +10139,7 @@
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="B81">
         <v>0</v>
@@ -9547,7 +10147,7 @@
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="B82">
         <v>0</v>
@@ -9555,7 +10155,7 @@
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="B83">
         <v>0</v>
@@ -9563,7 +10163,7 @@
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="B84">
         <v>0</v>
@@ -9571,7 +10171,7 @@
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="B85">
         <v>0</v>
@@ -9579,7 +10179,7 @@
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="B86">
         <v>0</v>
@@ -9587,7 +10187,7 @@
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="B88">
         <v>0.8</v>
@@ -9595,7 +10195,7 @@
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="B89">
         <v>0.8</v>
@@ -9603,7 +10203,7 @@
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="B90">
         <v>0.8</v>
@@ -9611,7 +10211,7 @@
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="B91">
         <v>0.8</v>
@@ -9619,7 +10219,7 @@
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="B92">
         <v>0.8</v>
@@ -9627,7 +10227,7 @@
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="B93">
         <v>0.8</v>
@@ -9635,7 +10235,7 @@
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="B94">
         <v>0.8</v>
@@ -9643,7 +10243,7 @@
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="B95">
         <v>0.8</v>
@@ -9651,7 +10251,7 @@
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="B96">
         <v>0.8</v>
@@ -9659,7 +10259,7 @@
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="B97">
         <v>0.8</v>
@@ -9667,7 +10267,7 @@
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="B98">
         <v>0.8</v>
@@ -9675,7 +10275,7 @@
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="B99">
         <v>0.8</v>
@@ -9683,7 +10283,7 @@
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="B100">
         <v>0.8</v>
@@ -9691,7 +10291,7 @@
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="B101">
         <v>0.8</v>
@@ -9699,7 +10299,7 @@
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="B102">
         <v>0.8</v>
@@ -9707,7 +10307,7 @@
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="B103">
         <v>0.3</v>
@@ -9715,7 +10315,7 @@
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="B104">
         <v>0.8</v>
@@ -9723,7 +10323,7 @@
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="B105">
         <v>0.8</v>
@@ -9731,7 +10331,7 @@
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="B106">
         <v>0.8</v>
@@ -9739,7 +10339,7 @@
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="B107">
         <v>0.95</v>
@@ -9747,7 +10347,7 @@
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="B108">
         <v>0.8</v>
@@ -9755,7 +10355,7 @@
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="B109">
         <v>0.8</v>
@@ -9763,7 +10363,7 @@
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="B110">
         <v>0.8</v>
@@ -9771,7 +10371,7 @@
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="B111">
         <v>0.8</v>
@@ -9779,7 +10379,7 @@
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="B112">
         <v>0.8</v>
@@ -9787,7 +10387,7 @@
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="B113">
         <v>0.8</v>
@@ -9795,7 +10395,7 @@
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="B114">
         <v>0.8</v>
@@ -9803,7 +10403,7 @@
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="B115">
         <v>0.8</v>
@@ -9811,7 +10411,7 @@
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="B116">
         <v>0.8</v>
@@ -9819,7 +10419,7 @@
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="B117">
         <v>0.8</v>
@@ -9827,7 +10427,7 @@
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="B118">
         <v>0.8</v>
@@ -9835,7 +10435,7 @@
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="B119">
         <v>0.8</v>
@@ -9843,7 +10443,7 @@
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="B120">
         <v>0.8</v>
@@ -9851,7 +10451,7 @@
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="B121">
         <v>0.8</v>
@@ -9859,7 +10459,7 @@
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="B122">
         <v>0.8</v>
@@ -9867,7 +10467,7 @@
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="B123">
         <v>0.8</v>
@@ -9875,7 +10475,7 @@
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="B124">
         <v>0.8</v>
@@ -9883,7 +10483,7 @@
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="B125">
         <v>0.8</v>
@@ -9891,7 +10491,7 @@
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="B126">
         <v>0.8</v>
@@ -9899,7 +10499,7 @@
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="B127">
         <v>0.8</v>
@@ -9907,7 +10507,7 @@
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="B128">
         <v>0.8</v>
@@ -9915,7 +10515,7 @@
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="B129">
         <v>0.8</v>
@@ -9923,7 +10523,7 @@
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="B130">
         <v>0.8</v>
@@ -9931,7 +10531,7 @@
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="B131">
         <v>0.8</v>
@@ -9939,7 +10539,7 @@
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="B132">
         <v>0.8</v>
@@ -9947,7 +10547,7 @@
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="B133">
         <v>0.8</v>
@@ -9955,7 +10555,7 @@
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="B134">
         <v>0.8</v>
@@ -9963,7 +10563,7 @@
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="B135">
         <v>0.8</v>
@@ -9971,7 +10571,7 @@
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="B136">
         <v>0.8</v>
@@ -9979,7 +10579,7 @@
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="B137">
         <v>0.8</v>
@@ -9987,7 +10587,7 @@
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="B138">
         <v>0.8</v>
@@ -9995,7 +10595,7 @@
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="B139">
         <v>0.3</v>
@@ -10003,7 +10603,7 @@
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="B140">
         <v>0.5</v>
@@ -10011,7 +10611,7 @@
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="B141">
         <v>0.8</v>
@@ -10019,7 +10619,7 @@
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="B142" s="1">
         <v>4.0000000000000003E-5</v>
@@ -10027,7 +10627,7 @@
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="B143" s="1">
         <v>0.8</v>
@@ -10035,7 +10635,7 @@
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="B144">
         <v>20</v>
@@ -10043,7 +10643,7 @@
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="B145">
         <v>20</v>
@@ -10051,7 +10651,7 @@
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="B146">
         <v>0.8</v>
@@ -10059,7 +10659,7 @@
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="B147">
         <v>0.6</v>
@@ -10067,7 +10667,7 @@
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="B148">
         <v>0.6</v>
@@ -10075,7 +10675,7 @@
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="B149">
         <v>0</v>
@@ -10083,7 +10683,7 @@
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="B150">
         <v>0</v>
@@ -10091,7 +10691,7 @@
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="B151">
         <v>0</v>
@@ -10099,7 +10699,7 @@
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="B152">
         <v>0</v>
@@ -10107,7 +10707,7 @@
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="B153">
         <v>0</v>
@@ -10115,7 +10715,7 @@
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="B154">
         <v>0.1</v>
@@ -10123,7 +10723,7 @@
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="B155">
         <v>0.1</v>
@@ -10131,7 +10731,7 @@
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="B156">
         <v>0.1</v>
@@ -10139,7 +10739,7 @@
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="B157">
         <v>0.1</v>
@@ -10147,7 +10747,7 @@
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="B158">
         <v>0.1</v>
@@ -10155,7 +10755,7 @@
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="B159">
         <v>0</v>
@@ -10163,7 +10763,7 @@
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="B160">
         <v>0</v>
@@ -10171,7 +10771,7 @@
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="B161">
         <v>0</v>
@@ -10179,7 +10779,7 @@
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="B162">
         <v>0</v>
@@ -10187,7 +10787,7 @@
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="B163">
         <v>0</v>
@@ -10195,7 +10795,7 @@
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="B164">
         <v>0</v>
@@ -10203,7 +10803,7 @@
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="B165">
         <v>0.6</v>
@@ -10211,7 +10811,7 @@
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="B166">
         <v>0</v>
@@ -10219,7 +10819,7 @@
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="B167">
         <v>0</v>
@@ -10227,7 +10827,7 @@
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="B168">
         <v>0</v>
@@ -10235,7 +10835,7 @@
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="B169">
         <v>0</v>
@@ -10243,7 +10843,7 @@
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="B170">
         <v>0</v>
@@ -10251,7 +10851,7 @@
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="B171">
         <v>0</v>
@@ -10259,7 +10859,7 @@
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="B172">
         <v>0</v>
@@ -10267,7 +10867,7 @@
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="B173">
         <v>0</v>
@@ -10280,10 +10880,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:O69"/>
+  <dimension ref="B3:O97"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3:O37"/>
+    <sheetView topLeftCell="A67" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C99" sqref="C99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12279,6 +12879,136 @@
       </c>
       <c r="E69">
         <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B72" t="s">
+        <v>808</v>
+      </c>
+    </row>
+    <row r="73" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B73" t="s">
+        <v>809</v>
+      </c>
+    </row>
+    <row r="74" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B74" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="75" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B75" t="s">
+        <v>811</v>
+      </c>
+    </row>
+    <row r="76" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B76" t="s">
+        <v>812</v>
+      </c>
+    </row>
+    <row r="77" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B77" t="s">
+        <v>813</v>
+      </c>
+    </row>
+    <row r="78" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B78" t="s">
+        <v>814</v>
+      </c>
+    </row>
+    <row r="79" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B79" t="s">
+        <v>815</v>
+      </c>
+    </row>
+    <row r="80" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B80" t="s">
+        <v>816</v>
+      </c>
+    </row>
+    <row r="81" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B81" t="s">
+        <v>817</v>
+      </c>
+    </row>
+    <row r="82" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B82" t="s">
+        <v>818</v>
+      </c>
+    </row>
+    <row r="83" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B83" t="s">
+        <v>819</v>
+      </c>
+    </row>
+    <row r="84" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B84" t="s">
+        <v>820</v>
+      </c>
+    </row>
+    <row r="85" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B85" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="86" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B86" t="s">
+        <v>822</v>
+      </c>
+    </row>
+    <row r="87" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B87" t="s">
+        <v>823</v>
+      </c>
+    </row>
+    <row r="88" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B88" t="s">
+        <v>824</v>
+      </c>
+    </row>
+    <row r="89" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B89" t="s">
+        <v>825</v>
+      </c>
+    </row>
+    <row r="90" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B90" t="s">
+        <v>826</v>
+      </c>
+    </row>
+    <row r="91" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B91" t="s">
+        <v>827</v>
+      </c>
+    </row>
+    <row r="92" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B92" t="s">
+        <v>828</v>
+      </c>
+    </row>
+    <row r="93" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B93" t="s">
+        <v>829</v>
+      </c>
+    </row>
+    <row r="94" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B94" t="s">
+        <v>830</v>
+      </c>
+    </row>
+    <row r="95" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B95" t="s">
+        <v>831</v>
+      </c>
+    </row>
+    <row r="96" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B96" t="s">
+        <v>832</v>
+      </c>
+    </row>
+    <row r="97" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B97" t="s">
+        <v>833</v>
       </c>
     </row>
   </sheetData>
@@ -25547,7 +26277,7 @@
         <v>20180530</v>
       </c>
       <c r="G1" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -26410,7 +27140,7 @@
   <dimension ref="A1:G65"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+      <selection activeCell="A26" sqref="A26:XFD26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -26436,7 +27166,7 @@
         <v>20180530</v>
       </c>
       <c r="G1" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -27461,26 +28191,26 @@
   <sheetData>
     <row r="1" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B1" s="3" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="C1" s="3"/>
       <c r="M1" s="3" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="N1" s="3"/>
       <c r="X1" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
     </row>
     <row r="2" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="C2">
         <v>10</v>
       </c>
       <c r="M2" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="N2">
         <v>10</v>
@@ -27632,13 +28362,13 @@
     </row>
     <row r="5" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="C5">
         <v>10</v>
       </c>
       <c r="M5" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="N5">
         <v>10</v>
@@ -27826,13 +28556,13 @@
     </row>
     <row r="8" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="C8">
         <v>10</v>
       </c>
       <c r="M8" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="N8">
         <v>10</v>
@@ -28020,13 +28750,13 @@
     </row>
     <row r="11" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="C11">
         <v>10</v>
       </c>
       <c r="M11" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="N11">
         <v>10</v>
@@ -28214,13 +28944,13 @@
     </row>
     <row r="14" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="C14">
         <v>10</v>
       </c>
       <c r="M14" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="N14">
         <v>10</v>
@@ -28408,13 +29138,13 @@
     </row>
     <row r="17" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="C17">
         <v>10</v>
       </c>
       <c r="M17" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="N17">
         <v>10</v>
@@ -28602,13 +29332,13 @@
     </row>
     <row r="20" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="C20">
         <v>10</v>
       </c>
       <c r="M20" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="N20">
         <v>10</v>
@@ -28796,13 +29526,13 @@
     </row>
     <row r="23" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="C23">
         <v>10</v>
       </c>
       <c r="M23" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="N23">
         <v>10</v>
@@ -28990,13 +29720,13 @@
     </row>
     <row r="26" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="C26">
         <v>10</v>
       </c>
       <c r="M26" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="N26">
         <v>10</v>
@@ -29184,13 +29914,13 @@
     </row>
     <row r="29" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="C29">
         <v>10</v>
       </c>
       <c r="M29" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="N29">
         <v>10</v>
@@ -29378,13 +30108,13 @@
     </row>
     <row r="32" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="C32">
         <v>10</v>
       </c>
       <c r="M32" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="N32">
         <v>10</v>
@@ -29572,13 +30302,13 @@
     </row>
     <row r="35" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="C35">
         <v>10</v>
       </c>
       <c r="M35" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="N35">
         <v>10</v>
@@ -29766,13 +30496,13 @@
     </row>
     <row r="38" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="C38">
         <v>10</v>
       </c>
       <c r="M38" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="N38">
         <v>10</v>
@@ -29960,13 +30690,13 @@
     </row>
     <row r="41" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="C41">
         <v>10</v>
       </c>
       <c r="M41" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="N41">
         <v>10</v>
@@ -30154,13 +30884,13 @@
     </row>
     <row r="44" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="C44">
         <v>10</v>
       </c>
       <c r="M44" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="N44">
         <v>10</v>
@@ -30348,13 +31078,13 @@
     </row>
     <row r="47" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="C47">
         <v>10</v>
       </c>
       <c r="M47" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="N47">
         <v>10</v>
@@ -30542,13 +31272,13 @@
     </row>
     <row r="50" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="C50">
         <v>10</v>
       </c>
       <c r="M50" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="N50">
         <v>10</v>
@@ -30736,13 +31466,13 @@
     </row>
     <row r="53" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="C53">
         <v>10</v>
       </c>
       <c r="M53" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="N53">
         <v>10</v>
@@ -30930,13 +31660,13 @@
     </row>
     <row r="56" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="C56">
         <v>10</v>
       </c>
       <c r="M56" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="N56">
         <v>10</v>
@@ -31124,13 +31854,13 @@
     </row>
     <row r="59" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="C59">
         <v>10</v>
       </c>
       <c r="M59" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="N59">
         <v>10</v>
@@ -31318,13 +32048,13 @@
     </row>
     <row r="62" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="C62">
         <v>10</v>
       </c>
       <c r="M62" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="N62">
         <v>10</v>
@@ -31512,13 +32242,13 @@
     </row>
     <row r="65" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="C65">
         <v>10</v>
       </c>
       <c r="M65" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="N65">
         <v>10</v>
@@ -31706,13 +32436,13 @@
     </row>
     <row r="68" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="C68">
         <v>10</v>
       </c>
       <c r="M68" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="N68">
         <v>10</v>
@@ -31900,13 +32630,13 @@
     </row>
     <row r="71" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C71">
         <v>10</v>
       </c>
       <c r="M71" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="N71">
         <v>10</v>
@@ -32094,13 +32824,13 @@
     </row>
     <row r="74" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B74" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="C74">
         <v>10</v>
       </c>
       <c r="M74" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="N74">
         <v>10</v>
@@ -32288,13 +33018,13 @@
     </row>
     <row r="77" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B77" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="C77">
         <v>10</v>
       </c>
       <c r="M77" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="N77">
         <v>10</v>
@@ -32482,13 +33212,13 @@
     </row>
     <row r="80" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B80" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="C80">
         <v>10</v>
       </c>
       <c r="M80" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="N80">
         <v>10</v>
@@ -32676,13 +33406,13 @@
     </row>
     <row r="83" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B83" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="C83">
         <v>10</v>
       </c>
       <c r="M83" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="N83">
         <v>10</v>
@@ -32870,13 +33600,13 @@
     </row>
     <row r="86" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B86" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="C86">
         <v>10</v>
       </c>
       <c r="M86" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="N86">
         <v>10</v>
@@ -33064,13 +33794,13 @@
     </row>
     <row r="89" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B89" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="C89">
         <v>10</v>
       </c>
       <c r="M89" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="N89">
         <v>10</v>
@@ -33258,13 +33988,13 @@
     </row>
     <row r="92" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B92" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="C92">
         <v>10</v>
       </c>
       <c r="M92" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="N92">
         <v>10</v>
@@ -33452,13 +34182,13 @@
     </row>
     <row r="95" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B95" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="C95">
         <v>10</v>
       </c>
       <c r="M95" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="N95">
         <v>10</v>
@@ -33646,13 +34376,13 @@
     </row>
     <row r="98" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B98" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="C98">
         <v>10</v>
       </c>
       <c r="M98" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="N98">
         <v>10</v>
@@ -33840,13 +34570,13 @@
     </row>
     <row r="101" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B101" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="C101">
         <v>10</v>
       </c>
       <c r="M101" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="N101">
         <v>10</v>
@@ -34034,13 +34764,13 @@
     </row>
     <row r="104" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B104" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="C104">
         <v>10</v>
       </c>
       <c r="M104" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="N104">
         <v>10</v>
@@ -34228,13 +34958,13 @@
     </row>
     <row r="107" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B107" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="C107">
         <v>10</v>
       </c>
       <c r="M107" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="N107">
         <v>10</v>
@@ -34422,13 +35152,13 @@
     </row>
     <row r="110" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B110" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="C110">
         <v>10</v>
       </c>
       <c r="M110" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="N110">
         <v>10</v>
@@ -34616,13 +35346,13 @@
     </row>
     <row r="113" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B113" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="C113">
         <v>10</v>
       </c>
       <c r="M113" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="N113">
         <v>10</v>
@@ -34810,13 +35540,13 @@
     </row>
     <row r="116" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B116" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="C116">
         <v>10</v>
       </c>
       <c r="M116" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="N116">
         <v>10</v>
@@ -35004,13 +35734,13 @@
     </row>
     <row r="119" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B119" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="C119">
         <v>10</v>
       </c>
       <c r="M119" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="N119">
         <v>10</v>
@@ -35198,13 +35928,13 @@
     </row>
     <row r="122" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B122" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="C122">
         <v>10</v>
       </c>
       <c r="M122" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="N122">
         <v>10</v>
@@ -35392,13 +36122,13 @@
     </row>
     <row r="125" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B125" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="C125">
         <v>10</v>
       </c>
       <c r="M125" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="N125">
         <v>10</v>
@@ -35586,13 +36316,13 @@
     </row>
     <row r="128" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B128" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="C128">
         <v>10</v>
       </c>
       <c r="M128" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="N128">
         <v>10</v>
@@ -35780,13 +36510,13 @@
     </row>
     <row r="131" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B131" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="C131">
         <v>10</v>
       </c>
       <c r="M131" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="N131">
         <v>10</v>
@@ -35974,13 +36704,13 @@
     </row>
     <row r="134" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B134" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="C134">
         <v>10</v>
       </c>
       <c r="M134" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="N134">
         <v>10</v>
@@ -36168,13 +36898,13 @@
     </row>
     <row r="137" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B137" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="C137">
         <v>10</v>
       </c>
       <c r="M137" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="N137">
         <v>10</v>
@@ -36362,13 +37092,13 @@
     </row>
     <row r="140" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B140" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="C140">
         <v>10</v>
       </c>
       <c r="M140" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="N140">
         <v>10</v>
@@ -36556,13 +37286,13 @@
     </row>
     <row r="143" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B143" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="C143">
         <v>10</v>
       </c>
       <c r="M143" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="N143">
         <v>10</v>
@@ -36750,13 +37480,13 @@
     </row>
     <row r="146" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B146" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="C146">
         <v>10</v>
       </c>
       <c r="M146" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="N146">
         <v>10</v>
@@ -36944,13 +37674,13 @@
     </row>
     <row r="149" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B149" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="C149">
         <v>10</v>
       </c>
       <c r="M149" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="N149">
         <v>10</v>
@@ -37138,13 +37868,13 @@
     </row>
     <row r="152" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B152" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="C152">
         <v>10</v>
       </c>
       <c r="M152" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="N152">
         <v>10</v>
@@ -37332,13 +38062,13 @@
     </row>
     <row r="155" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B155" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="C155">
         <v>10</v>
       </c>
       <c r="M155" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="N155">
         <v>10</v>
@@ -37526,13 +38256,13 @@
     </row>
     <row r="158" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B158" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="C158">
         <v>10</v>
       </c>
       <c r="M158" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="N158">
         <v>10</v>
@@ -37720,13 +38450,13 @@
     </row>
     <row r="161" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B161" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="C161">
         <v>10</v>
       </c>
       <c r="M161" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="N161">
         <v>10</v>
@@ -37914,13 +38644,13 @@
     </row>
     <row r="164" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B164" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="C164">
         <v>10</v>
       </c>
       <c r="M164" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="N164">
         <v>10</v>
@@ -38108,13 +38838,13 @@
     </row>
     <row r="167" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B167" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="C167">
         <v>10</v>
       </c>
       <c r="M167" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="N167">
         <v>10</v>
@@ -38302,13 +39032,13 @@
     </row>
     <row r="170" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B170" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="C170">
         <v>10</v>
       </c>
       <c r="M170" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="N170">
         <v>10</v>
@@ -38496,13 +39226,13 @@
     </row>
     <row r="173" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B173" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="C173">
         <v>10</v>
       </c>
       <c r="M173" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="N173">
         <v>10</v>
@@ -38690,13 +39420,13 @@
     </row>
     <row r="176" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B176" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="C176">
         <v>10</v>
       </c>
       <c r="M176" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="N176">
         <v>10</v>

</xml_diff>

<commit_message>
fixing weight and length params based on RN and SN
</commit_message>
<xml_diff>
--- a/R/C_and_Mum.xlsx
+++ b/R/C_and_Mum.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <workbookProtection lockWindows="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="740" firstSheet="1" activeTab="12"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="835" firstSheet="1" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="C_v1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
     <sheet name="ageclass" sheetId="10" r:id="rId10"/>
     <sheet name="gape" sheetId="11" r:id="rId11"/>
     <sheet name="size" sheetId="12" r:id="rId12"/>
-    <sheet name="RN+SN" sheetId="13" r:id="rId13"/>
+    <sheet name="RN_SN" sheetId="13" r:id="rId13"/>
   </sheets>
   <calcPr calcId="162913" iterateDelta="1E-4"/>
   <extLst>
@@ -3659,7 +3659,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:AK70"/>
   <sheetViews>
-    <sheetView windowProtection="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView windowProtection="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="AB4" sqref="AB4"/>
     </sheetView>
   </sheetViews>
@@ -12207,7 +12207,7 @@
   <dimension ref="A1:T60"/>
   <sheetViews>
     <sheetView windowProtection="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14679,10 +14679,10 @@
   <dimension ref="A1:W581"/>
   <sheetViews>
     <sheetView windowProtection="1" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="R32" sqref="R32"/>
+      <selection pane="bottomRight" activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14824,7 +14824,7 @@
         <v>228.18913710000001</v>
       </c>
       <c r="E3">
-        <f t="shared" ref="E2:E65" si="2">C3*3.65*5.7*20/1000</f>
+        <f t="shared" ref="E3:E65" si="2">C3*3.65*5.7*20/1000</f>
         <v>35.829999984435005</v>
       </c>
       <c r="F3">

</xml_diff>

<commit_message>
updating species von bert profiles for SN RN
</commit_message>
<xml_diff>
--- a/R/C_and_Mum.xlsx
+++ b/R/C_and_Mum.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <workbookProtection lockWindows="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="989" activeTab="11"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="892" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="C_v1" sheetId="1" r:id="rId1"/>
@@ -8092,11 +8092,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA122"/>
   <sheetViews>
-    <sheetView windowProtection="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B47" activePane="bottomRight" state="frozen"/>
+    <sheetView windowProtection="1" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A110" sqref="A110"/>
-      <selection pane="bottomRight" activeCell="B63" sqref="B63:F63"/>
+      <selection pane="bottomRight" activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8113,7 +8113,7 @@
     <col min="10" max="1025" width="8.140625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>20180419</v>
       </c>
@@ -8145,9 +8145,9 @@
         <v>498</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>499</v>
+        <v>534</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -8156,86 +8156,74 @@
         <v>10</v>
       </c>
       <c r="D2">
-        <f t="shared" ref="D2:D33" si="0">C2*B2</f>
+        <f>C2*B2</f>
         <v>10</v>
       </c>
       <c r="F2">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="G2">
-        <v>3400</v>
+        <v>50</v>
       </c>
       <c r="H2">
-        <v>60</v>
+        <v>15</v>
       </c>
       <c r="I2">
+        <v>10</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>535</v>
+      </c>
+      <c r="T2" s="3" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>525</v>
+      </c>
+      <c r="B3">
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <v>10</v>
+      </c>
+      <c r="D3">
+        <f>C3*B3</f>
         <v>30</v>
       </c>
-      <c r="J2" s="3" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>501</v>
-      </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="C3">
-        <v>10</v>
-      </c>
-      <c r="D3">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
       <c r="F3">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="G3">
-        <v>1100</v>
+        <v>684000</v>
       </c>
       <c r="H3">
-        <v>45</v>
+        <v>458</v>
       </c>
       <c r="I3">
+        <v>200</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>528</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>10</v>
+      </c>
+      <c r="D4">
+        <f>C4*B4</f>
         <v>30</v>
       </c>
-      <c r="J3" s="3" t="s">
-        <v>502</v>
-      </c>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>503</v>
-      </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="C4">
-        <v>10</v>
-      </c>
-      <c r="D4">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="F4">
-        <v>23</v>
-      </c>
-      <c r="G4">
-        <v>21000</v>
-      </c>
-      <c r="H4">
-        <v>133</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>504</v>
-      </c>
-      <c r="T4" s="3" t="s">
-        <v>505</v>
-      </c>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>506</v>
       </c>
@@ -8246,7 +8234,7 @@
         <v>10</v>
       </c>
       <c r="D5">
-        <f t="shared" si="0"/>
+        <f>C5*B5</f>
         <v>10</v>
       </c>
       <c r="F5">
@@ -8265,72 +8253,54 @@
         <v>507</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>508</v>
+        <v>590</v>
       </c>
       <c r="B6">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C6">
         <v>10</v>
       </c>
       <c r="D6">
-        <f t="shared" si="0"/>
+        <f>C6*B6</f>
+        <v>70</v>
+      </c>
+      <c r="F6">
         <v>20</v>
       </c>
-      <c r="F6">
-        <v>7</v>
-      </c>
       <c r="G6">
-        <v>910</v>
+        <v>206000</v>
       </c>
       <c r="H6">
-        <v>46</v>
+        <v>400</v>
+      </c>
+      <c r="I6">
+        <v>335</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>509</v>
-      </c>
-      <c r="T6" s="3" t="s">
-        <v>510</v>
-      </c>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>511</v>
+        <v>537</v>
       </c>
       <c r="B7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C7">
         <v>10</v>
       </c>
       <c r="D7">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="F7">
-        <v>9</v>
-      </c>
-      <c r="G7">
-        <v>10170</v>
-      </c>
-      <c r="H7">
-        <v>89</v>
-      </c>
-      <c r="I7">
-        <v>40</v>
-      </c>
-      <c r="J7" s="3" t="s">
-        <v>512</v>
-      </c>
-      <c r="T7" s="3" t="s">
-        <v>513</v>
-      </c>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+        <f>C7*B7</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>514</v>
+        <v>554</v>
       </c>
       <c r="B8">
         <v>2</v>
@@ -8339,79 +8309,79 @@
         <v>10</v>
       </c>
       <c r="D8">
-        <f t="shared" si="0"/>
+        <f>C8*B8</f>
         <v>20</v>
       </c>
       <c r="F8">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="G8">
-        <v>3600</v>
+        <v>4300</v>
       </c>
       <c r="H8">
-        <v>64</v>
+        <v>66</v>
+      </c>
+      <c r="I8">
+        <v>30</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>515</v>
-      </c>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>516</v>
+        <v>530</v>
       </c>
       <c r="B9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C9">
         <v>10</v>
       </c>
       <c r="D9">
-        <f t="shared" si="0"/>
+        <f>C9*B9</f>
+        <v>10</v>
+      </c>
+      <c r="G9">
+        <v>567</v>
+      </c>
+      <c r="H9">
+        <v>30</v>
+      </c>
+      <c r="I9">
         <v>20</v>
       </c>
-      <c r="F9">
-        <v>25</v>
-      </c>
-      <c r="G9">
-        <v>2500</v>
-      </c>
-      <c r="H9">
-        <v>60</v>
-      </c>
       <c r="J9" s="3" t="s">
-        <v>517</v>
-      </c>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+        <v>531</v>
+      </c>
+      <c r="T9" s="3" t="s">
+        <v>532</v>
+      </c>
+      <c r="Z9" s="3" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>518</v>
+        <v>605</v>
       </c>
       <c r="B10">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="C10">
         <v>10</v>
       </c>
       <c r="D10">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="F10">
-        <v>50</v>
-      </c>
-      <c r="G10">
-        <v>320000</v>
-      </c>
-      <c r="H10">
-        <v>470</v>
-      </c>
-      <c r="J10" s="3" t="s">
-        <v>519</v>
-      </c>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+        <f>C10*B10</f>
+        <v>90</v>
+      </c>
+      <c r="J10" s="4" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>520</v>
+        <v>544</v>
       </c>
       <c r="B11">
         <v>2</v>
@@ -8420,49 +8390,61 @@
         <v>10</v>
       </c>
       <c r="D11">
-        <f t="shared" si="0"/>
+        <f>C11*B11</f>
         <v>20</v>
       </c>
       <c r="F11">
+        <v>25</v>
+      </c>
+      <c r="G11">
+        <v>96000</v>
+      </c>
+      <c r="H11">
+        <v>200</v>
+      </c>
+      <c r="I11">
+        <v>100</v>
+      </c>
+      <c r="J11" s="3" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>582</v>
+      </c>
+      <c r="B12">
+        <v>4</v>
+      </c>
+      <c r="C12">
+        <v>10</v>
+      </c>
+      <c r="D12">
+        <f>C12*B12</f>
+        <v>40</v>
+      </c>
+      <c r="F12" s="2">
         <v>30</v>
       </c>
-      <c r="G11">
-        <v>6400</v>
-      </c>
-      <c r="H11">
-        <v>82.6</v>
-      </c>
-      <c r="J11" s="3" t="s">
-        <v>521</v>
-      </c>
-    </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>522</v>
-      </c>
-      <c r="B12">
-        <v>2</v>
-      </c>
-      <c r="C12">
-        <v>10</v>
-      </c>
-      <c r="D12">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
       <c r="G12">
-        <v>750</v>
+        <v>9100</v>
       </c>
       <c r="H12">
-        <v>43</v>
+        <v>160</v>
+      </c>
+      <c r="I12">
+        <v>100</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>523</v>
-      </c>
-    </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+        <v>583</v>
+      </c>
+      <c r="T12" s="3" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>524</v>
+        <v>568</v>
       </c>
       <c r="B13">
         <v>2</v>
@@ -8471,358 +8453,346 @@
         <v>10</v>
       </c>
       <c r="D13">
-        <f t="shared" si="0"/>
+        <f>C13*B13</f>
         <v>20</v>
       </c>
-    </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="G13">
+        <v>43000</v>
+      </c>
+      <c r="H13">
+        <v>145</v>
+      </c>
+      <c r="T13" s="3" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>525</v>
+        <v>589</v>
       </c>
       <c r="B14">
+        <v>5</v>
+      </c>
+      <c r="C14">
+        <v>10</v>
+      </c>
+      <c r="D14">
+        <f>C14*B14</f>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>543</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15">
+        <v>10</v>
+      </c>
+      <c r="D15">
+        <f>C15*B15</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>577</v>
+      </c>
+      <c r="B16">
+        <v>2</v>
+      </c>
+      <c r="C16">
+        <v>10</v>
+      </c>
+      <c r="D16">
+        <f>C16*B16</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>524</v>
+      </c>
+      <c r="B17">
+        <v>2</v>
+      </c>
+      <c r="C17">
+        <v>10</v>
+      </c>
+      <c r="D17">
+        <f>C17*B17</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>522</v>
+      </c>
+      <c r="B18">
+        <v>2</v>
+      </c>
+      <c r="C18">
+        <v>10</v>
+      </c>
+      <c r="D18">
+        <f>C18*B18</f>
+        <v>20</v>
+      </c>
+      <c r="G18">
+        <v>750</v>
+      </c>
+      <c r="H18">
+        <v>43</v>
+      </c>
+      <c r="J18" s="3" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>538</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19">
+        <v>10</v>
+      </c>
+      <c r="D19">
+        <f>C19*B19</f>
+        <v>10</v>
+      </c>
+      <c r="F19">
+        <v>30</v>
+      </c>
+      <c r="G19">
+        <v>22600</v>
+      </c>
+      <c r="H19">
+        <v>120</v>
+      </c>
+      <c r="I19">
+        <v>90</v>
+      </c>
+      <c r="J19" s="3" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>578</v>
+      </c>
+      <c r="B20">
+        <v>2</v>
+      </c>
+      <c r="C20">
+        <v>10</v>
+      </c>
+      <c r="D20">
+        <f>C20*B20</f>
+        <v>20</v>
+      </c>
+      <c r="F20">
+        <v>20</v>
+      </c>
+      <c r="G20">
+        <v>16800</v>
+      </c>
+      <c r="H20">
+        <v>112</v>
+      </c>
+      <c r="I20">
+        <v>35</v>
+      </c>
+      <c r="J20" s="3" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>518</v>
+      </c>
+      <c r="B21">
+        <v>2</v>
+      </c>
+      <c r="C21">
+        <v>10</v>
+      </c>
+      <c r="D21">
+        <f>C21*B21</f>
+        <v>20</v>
+      </c>
+      <c r="F21">
+        <v>50</v>
+      </c>
+      <c r="G21">
+        <v>320000</v>
+      </c>
+      <c r="H21">
+        <v>470</v>
+      </c>
+      <c r="J21" s="3" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>501</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22">
+        <v>10</v>
+      </c>
+      <c r="D22">
+        <f>C22*B22</f>
+        <v>10</v>
+      </c>
+      <c r="F22">
+        <v>25</v>
+      </c>
+      <c r="G22">
+        <v>1100</v>
+      </c>
+      <c r="H22">
+        <v>45</v>
+      </c>
+      <c r="I22">
+        <v>30</v>
+      </c>
+      <c r="J22" s="3" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>609</v>
+      </c>
+      <c r="B23">
+        <v>2</v>
+      </c>
+      <c r="C23">
+        <v>10</v>
+      </c>
+      <c r="D23">
+        <f>C23*B23</f>
+        <v>20</v>
+      </c>
+      <c r="F23">
+        <v>10</v>
+      </c>
+      <c r="H23">
+        <v>38</v>
+      </c>
+      <c r="J23" s="3" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>598</v>
+      </c>
+      <c r="B24">
         <v>3</v>
       </c>
-      <c r="C14">
-        <v>10</v>
-      </c>
-      <c r="D14">
-        <f t="shared" si="0"/>
+      <c r="C24">
+        <v>10</v>
+      </c>
+      <c r="D24">
+        <f>C24*B24</f>
         <v>30</v>
       </c>
-      <c r="F14">
-        <v>32</v>
-      </c>
-      <c r="G14">
-        <v>684000</v>
-      </c>
-      <c r="H14">
-        <v>458</v>
-      </c>
-      <c r="I14">
-        <v>200</v>
-      </c>
-      <c r="J14" s="3" t="s">
-        <v>526</v>
-      </c>
-    </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>527</v>
-      </c>
-      <c r="B15">
-        <v>3</v>
-      </c>
-      <c r="C15">
-        <v>10</v>
-      </c>
-      <c r="D15">
-        <f t="shared" si="0"/>
+      <c r="F24">
+        <v>12</v>
+      </c>
+      <c r="H24">
+        <v>54</v>
+      </c>
+      <c r="J24" s="3" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>499</v>
+      </c>
+      <c r="B25">
+        <v>1</v>
+      </c>
+      <c r="C25">
+        <v>10</v>
+      </c>
+      <c r="D25">
+        <f>C25*B25</f>
+        <v>10</v>
+      </c>
+      <c r="F25">
+        <v>17</v>
+      </c>
+      <c r="G25">
+        <v>3400</v>
+      </c>
+      <c r="H25">
+        <v>60</v>
+      </c>
+      <c r="I25">
         <v>30</v>
       </c>
-    </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>528</v>
-      </c>
-      <c r="B16">
-        <v>3</v>
-      </c>
-      <c r="C16">
-        <v>10</v>
-      </c>
-      <c r="D16">
-        <f t="shared" si="0"/>
-        <v>30</v>
-      </c>
-    </row>
-    <row r="17" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="J25" s="3" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>540</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26">
+        <v>10</v>
+      </c>
+      <c r="D26">
+        <f>C26*B26</f>
+        <v>10</v>
+      </c>
+      <c r="G26">
+        <v>822</v>
+      </c>
+      <c r="H26">
+        <v>50</v>
+      </c>
+      <c r="I26">
+        <v>25</v>
+      </c>
+      <c r="J26" s="3" t="s">
+        <v>541</v>
+      </c>
+      <c r="T26" s="3" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>529</v>
       </c>
-      <c r="B17">
-        <v>1</v>
-      </c>
-      <c r="C17">
-        <v>10</v>
-      </c>
-      <c r="D17">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="18" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>530</v>
-      </c>
-      <c r="B18">
-        <v>1</v>
-      </c>
-      <c r="C18">
-        <v>10</v>
-      </c>
-      <c r="D18">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="G18">
-        <v>567</v>
-      </c>
-      <c r="H18">
-        <v>30</v>
-      </c>
-      <c r="I18">
-        <v>20</v>
-      </c>
-      <c r="J18" s="3" t="s">
-        <v>531</v>
-      </c>
-      <c r="T18" s="3" t="s">
-        <v>532</v>
-      </c>
-      <c r="Z18" s="3" t="s">
-        <v>533</v>
-      </c>
-    </row>
-    <row r="19" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>534</v>
-      </c>
-      <c r="B19">
-        <v>1</v>
-      </c>
-      <c r="C19">
-        <v>10</v>
-      </c>
-      <c r="D19">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="F19">
-        <v>5</v>
-      </c>
-      <c r="G19">
-        <v>50</v>
-      </c>
-      <c r="H19">
-        <v>15</v>
-      </c>
-      <c r="I19">
-        <v>10</v>
-      </c>
-      <c r="J19" s="3" t="s">
-        <v>535</v>
-      </c>
-      <c r="T19" s="3" t="s">
-        <v>536</v>
-      </c>
-    </row>
-    <row r="20" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>537</v>
-      </c>
-      <c r="B20">
-        <v>1</v>
-      </c>
-      <c r="C20">
-        <v>10</v>
-      </c>
-      <c r="D20">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="21" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>538</v>
-      </c>
-      <c r="B21">
-        <v>1</v>
-      </c>
-      <c r="C21">
-        <v>10</v>
-      </c>
-      <c r="D21">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="F21">
-        <v>30</v>
-      </c>
-      <c r="G21">
-        <v>22600</v>
-      </c>
-      <c r="H21">
-        <v>120</v>
-      </c>
-      <c r="I21">
-        <v>90</v>
-      </c>
-      <c r="J21" s="3" t="s">
-        <v>539</v>
-      </c>
-    </row>
-    <row r="22" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>540</v>
-      </c>
-      <c r="B22">
-        <v>1</v>
-      </c>
-      <c r="C22">
-        <v>10</v>
-      </c>
-      <c r="D22">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="G22">
-        <v>822</v>
-      </c>
-      <c r="H22">
-        <v>50</v>
-      </c>
-      <c r="I22">
-        <v>25</v>
-      </c>
-      <c r="J22" s="3" t="s">
-        <v>541</v>
-      </c>
-      <c r="T22" s="3" t="s">
-        <v>542</v>
-      </c>
-    </row>
-    <row r="23" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>543</v>
-      </c>
-      <c r="B23">
-        <v>1</v>
-      </c>
-      <c r="C23">
-        <v>10</v>
-      </c>
-      <c r="D23">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="24" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>544</v>
-      </c>
-      <c r="B24">
-        <v>2</v>
-      </c>
-      <c r="C24">
-        <v>10</v>
-      </c>
-      <c r="D24">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="F24">
-        <v>25</v>
-      </c>
-      <c r="G24">
-        <v>96000</v>
-      </c>
-      <c r="H24">
-        <v>200</v>
-      </c>
-      <c r="I24">
-        <v>100</v>
-      </c>
-      <c r="J24" s="3" t="s">
-        <v>545</v>
-      </c>
-    </row>
-    <row r="25" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>546</v>
-      </c>
-      <c r="B25">
-        <v>1</v>
-      </c>
-      <c r="C25">
-        <v>10</v>
-      </c>
-      <c r="D25">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="F25">
-        <v>12</v>
-      </c>
-      <c r="G25">
-        <v>2300</v>
-      </c>
-      <c r="H25">
-        <v>76</v>
-      </c>
-      <c r="I25">
-        <v>37</v>
-      </c>
-      <c r="J25" s="3" t="s">
-        <v>547</v>
-      </c>
-    </row>
-    <row r="26" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+      <c r="B27">
+        <v>1</v>
+      </c>
+      <c r="C27">
+        <v>10</v>
+      </c>
+      <c r="D27">
+        <f>C27*B27</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>548</v>
-      </c>
-      <c r="B26">
-        <v>2</v>
-      </c>
-      <c r="C26">
-        <v>10</v>
-      </c>
-      <c r="D26">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="H26">
-        <v>70</v>
-      </c>
-      <c r="I26">
-        <v>30</v>
-      </c>
-      <c r="J26" s="3" t="s">
-        <v>549</v>
-      </c>
-    </row>
-    <row r="27" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>550</v>
-      </c>
-      <c r="B27">
-        <v>2</v>
-      </c>
-      <c r="C27">
-        <v>10</v>
-      </c>
-      <c r="D27">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="F27">
-        <v>25</v>
-      </c>
-      <c r="G27">
-        <v>32000</v>
-      </c>
-      <c r="H27">
-        <v>130</v>
-      </c>
-      <c r="I27">
-        <v>60</v>
-      </c>
-      <c r="J27" s="3" t="s">
-        <v>551</v>
-      </c>
-    </row>
-    <row r="28" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>552</v>
       </c>
       <c r="B28">
         <v>2</v>
@@ -8831,22 +8801,22 @@
         <v>10</v>
       </c>
       <c r="D28">
-        <f t="shared" si="0"/>
+        <f>C28*B28</f>
         <v>20</v>
       </c>
-      <c r="G28">
-        <v>3600</v>
-      </c>
       <c r="H28">
-        <v>66</v>
+        <v>70</v>
+      </c>
+      <c r="I28">
+        <v>30</v>
       </c>
       <c r="J28" s="3" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="29" spans="1:27" x14ac:dyDescent="0.25">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>554</v>
+        <v>564</v>
       </c>
       <c r="B29">
         <v>2</v>
@@ -8855,58 +8825,40 @@
         <v>10</v>
       </c>
       <c r="D29">
-        <f t="shared" si="0"/>
+        <f>C29*B29</f>
         <v>20</v>
       </c>
       <c r="F29">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G29">
-        <v>4300</v>
+        <v>5400</v>
       </c>
       <c r="H29">
-        <v>66</v>
-      </c>
-      <c r="I29">
+        <v>110</v>
+      </c>
+      <c r="J29" s="3" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>602</v>
+      </c>
+      <c r="B30">
+        <v>3</v>
+      </c>
+      <c r="C30">
+        <v>10</v>
+      </c>
+      <c r="D30">
+        <f>C30*B30</f>
         <v>30</v>
       </c>
-      <c r="J29" s="3" t="s">
-        <v>555</v>
-      </c>
-    </row>
-    <row r="30" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>556</v>
-      </c>
-      <c r="B30">
-        <v>2</v>
-      </c>
-      <c r="C30">
-        <v>10</v>
-      </c>
-      <c r="D30">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="F30">
-        <v>15</v>
-      </c>
-      <c r="G30">
-        <v>2100</v>
-      </c>
-      <c r="H30">
-        <v>46</v>
-      </c>
-      <c r="I30">
-        <v>25</v>
-      </c>
-      <c r="J30" s="3" t="s">
-        <v>557</v>
-      </c>
-    </row>
-    <row r="31" spans="1:27" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>558</v>
+        <v>520</v>
       </c>
       <c r="B31">
         <v>2</v>
@@ -8915,28 +8867,25 @@
         <v>10</v>
       </c>
       <c r="D31">
-        <f t="shared" si="0"/>
+        <f>C31*B31</f>
         <v>20</v>
       </c>
       <c r="F31">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="G31">
-        <v>30000</v>
+        <v>6400</v>
       </c>
       <c r="H31">
-        <v>125</v>
-      </c>
-      <c r="I31">
-        <v>90</v>
+        <v>82.6</v>
       </c>
       <c r="J31" s="3" t="s">
-        <v>559</v>
-      </c>
-    </row>
-    <row r="32" spans="1:27" x14ac:dyDescent="0.25">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>560</v>
+        <v>550</v>
       </c>
       <c r="B32">
         <v>2</v>
@@ -8945,88 +8894,73 @@
         <v>10</v>
       </c>
       <c r="D32">
-        <f t="shared" si="0"/>
+        <f>C32*B32</f>
         <v>20</v>
       </c>
       <c r="F32">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="G32">
-        <v>1130</v>
+        <v>32000</v>
       </c>
       <c r="H32">
-        <v>50.8</v>
+        <v>130</v>
+      </c>
+      <c r="I32">
+        <v>60</v>
       </c>
       <c r="J32" s="3" t="s">
-        <v>561</v>
-      </c>
-      <c r="T32" s="3" t="s">
-        <v>562</v>
-      </c>
-      <c r="AA32" s="3" t="s">
-        <v>563</v>
-      </c>
-    </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="33" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>564</v>
+        <v>592</v>
       </c>
       <c r="B33">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C33">
         <v>10</v>
       </c>
       <c r="D33">
-        <f t="shared" si="0"/>
-        <v>20</v>
+        <f>C33*B33</f>
+        <v>70</v>
       </c>
       <c r="F33">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="G33">
-        <v>5400</v>
+        <v>230000</v>
       </c>
       <c r="H33">
-        <v>110</v>
+        <v>350</v>
+      </c>
+      <c r="I33">
+        <v>244</v>
       </c>
       <c r="J33" s="3" t="s">
-        <v>565</v>
-      </c>
-    </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="34" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>566</v>
+        <v>594</v>
       </c>
       <c r="B34">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C34">
         <v>10</v>
       </c>
       <c r="D34">
-        <f t="shared" ref="D34:D65" si="1">C34*B34</f>
-        <v>20</v>
-      </c>
-      <c r="F34">
-        <v>13</v>
-      </c>
-      <c r="G34">
-        <v>46800</v>
-      </c>
-      <c r="H34">
-        <v>150</v>
-      </c>
-      <c r="I34">
-        <v>30</v>
-      </c>
-      <c r="J34" s="3" t="s">
-        <v>567</v>
-      </c>
-    </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
+        <f>C34*B34</f>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="35" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>568</v>
+        <v>560</v>
       </c>
       <c r="B35">
         <v>2</v>
@@ -9035,52 +8969,46 @@
         <v>10</v>
       </c>
       <c r="D35">
-        <f t="shared" si="1"/>
+        <f>C35*B35</f>
         <v>20</v>
       </c>
+      <c r="F35">
+        <v>50</v>
+      </c>
       <c r="G35">
-        <v>43000</v>
+        <v>1130</v>
       </c>
       <c r="H35">
-        <v>145</v>
+        <v>50.8</v>
+      </c>
+      <c r="J35" s="3" t="s">
+        <v>561</v>
       </c>
       <c r="T35" s="3" t="s">
-        <v>569</v>
-      </c>
-    </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
+        <v>562</v>
+      </c>
+      <c r="AA35" s="3" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="36" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>570</v>
+        <v>603</v>
       </c>
       <c r="B36">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="C36">
         <v>10</v>
       </c>
       <c r="D36">
-        <f t="shared" si="1"/>
-        <v>20</v>
-      </c>
-      <c r="F36">
-        <v>30</v>
-      </c>
-      <c r="G36">
-        <v>57000</v>
-      </c>
-      <c r="H36">
-        <v>200</v>
-      </c>
-      <c r="I36">
-        <v>120</v>
-      </c>
-      <c r="J36" s="3" t="s">
-        <v>571</v>
-      </c>
-    </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
+        <f>C36*B36</f>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="37" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>572</v>
+        <v>552</v>
       </c>
       <c r="B37">
         <v>2</v>
@@ -9089,49 +9017,43 @@
         <v>10</v>
       </c>
       <c r="D37">
-        <f t="shared" si="1"/>
+        <f>C37*B37</f>
         <v>20</v>
       </c>
-      <c r="F37">
-        <v>34</v>
-      </c>
       <c r="G37">
-        <v>11300</v>
+        <v>3600</v>
       </c>
       <c r="H37">
-        <v>91</v>
+        <v>66</v>
       </c>
       <c r="J37" s="3" t="s">
-        <v>573</v>
-      </c>
-    </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="38" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>574</v>
+        <v>604</v>
       </c>
       <c r="B38">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="C38">
         <v>10</v>
       </c>
       <c r="D38">
-        <f t="shared" si="1"/>
-        <v>20</v>
+        <f>C38*B38</f>
+        <v>90</v>
+      </c>
+      <c r="F38">
+        <v>70</v>
       </c>
       <c r="G38">
-        <v>23600</v>
-      </c>
-      <c r="H38">
-        <v>150</v>
-      </c>
-      <c r="J38" s="3" t="s">
-        <v>575</v>
-      </c>
-    </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="39" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>576</v>
+        <v>566</v>
       </c>
       <c r="B39">
         <v>2</v>
@@ -9140,13 +9062,28 @@
         <v>10</v>
       </c>
       <c r="D39">
-        <f t="shared" si="1"/>
+        <f>C39*B39</f>
         <v>20</v>
       </c>
-    </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="F39">
+        <v>13</v>
+      </c>
+      <c r="G39">
+        <v>46800</v>
+      </c>
+      <c r="H39">
+        <v>150</v>
+      </c>
+      <c r="I39">
+        <v>30</v>
+      </c>
+      <c r="J39" s="3" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="40" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>577</v>
+        <v>601</v>
       </c>
       <c r="B40">
         <v>2</v>
@@ -9155,13 +9092,13 @@
         <v>10</v>
       </c>
       <c r="D40">
-        <f t="shared" si="1"/>
+        <f>C40*B40</f>
         <v>20</v>
       </c>
     </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>578</v>
+        <v>556</v>
       </c>
       <c r="B41">
         <v>2</v>
@@ -9170,115 +9107,88 @@
         <v>10</v>
       </c>
       <c r="D41">
-        <f t="shared" si="1"/>
+        <f>C41*B41</f>
         <v>20</v>
       </c>
       <c r="F41">
+        <v>15</v>
+      </c>
+      <c r="G41">
+        <v>2100</v>
+      </c>
+      <c r="H41">
+        <v>46</v>
+      </c>
+      <c r="I41">
+        <v>25</v>
+      </c>
+      <c r="J41" s="3" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="42" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>576</v>
+      </c>
+      <c r="B42">
+        <v>2</v>
+      </c>
+      <c r="C42">
+        <v>10</v>
+      </c>
+      <c r="D42">
+        <f>C42*B42</f>
         <v>20</v>
       </c>
-      <c r="G41">
-        <v>16800</v>
-      </c>
-      <c r="H41">
-        <v>112</v>
-      </c>
-      <c r="I41">
-        <v>35</v>
-      </c>
-      <c r="J41" s="3" t="s">
-        <v>579</v>
-      </c>
-    </row>
-    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>580</v>
-      </c>
-      <c r="B42">
-        <v>1</v>
-      </c>
-      <c r="C42">
-        <v>10</v>
-      </c>
-      <c r="D42">
-        <f t="shared" si="1"/>
-        <v>10</v>
-      </c>
-      <c r="F42">
-        <v>14</v>
-      </c>
-      <c r="G42">
-        <v>1500</v>
-      </c>
-      <c r="H42">
-        <v>64</v>
-      </c>
-      <c r="J42" s="3" t="s">
-        <v>581</v>
-      </c>
-    </row>
-    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="43" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>582</v>
+        <v>546</v>
       </c>
       <c r="B43">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C43">
         <v>10</v>
       </c>
       <c r="D43">
-        <f t="shared" si="1"/>
-        <v>40</v>
-      </c>
-      <c r="F43" s="2">
+        <f>C43*B43</f>
+        <v>10</v>
+      </c>
+      <c r="F43">
+        <v>12</v>
+      </c>
+      <c r="G43">
+        <v>2300</v>
+      </c>
+      <c r="H43">
+        <v>76</v>
+      </c>
+      <c r="I43">
+        <v>37</v>
+      </c>
+      <c r="J43" s="3" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="44" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>600</v>
+      </c>
+      <c r="B44">
+        <v>3</v>
+      </c>
+      <c r="C44">
+        <v>10</v>
+      </c>
+      <c r="D44">
+        <f>C44*B44</f>
         <v>30</v>
       </c>
-      <c r="G43">
-        <v>9100</v>
-      </c>
-      <c r="H43">
-        <v>160</v>
-      </c>
-      <c r="I43">
-        <v>100</v>
-      </c>
-      <c r="J43" s="3" t="s">
-        <v>583</v>
-      </c>
-      <c r="T43" s="3" t="s">
-        <v>584</v>
-      </c>
-    </row>
-    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
+    </row>
+    <row r="45" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
         <v>585</v>
-      </c>
-      <c r="B44">
-        <v>5</v>
-      </c>
-      <c r="C44">
-        <v>10</v>
-      </c>
-      <c r="D44">
-        <f t="shared" si="1"/>
-        <v>50</v>
-      </c>
-      <c r="G44">
-        <v>12200</v>
-      </c>
-      <c r="H44">
-        <v>150</v>
-      </c>
-      <c r="I44">
-        <v>100</v>
-      </c>
-      <c r="J44" s="3" t="s">
-        <v>586</v>
-      </c>
-    </row>
-    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>587</v>
       </c>
       <c r="B45">
         <v>5</v>
@@ -9287,28 +9197,25 @@
         <v>10</v>
       </c>
       <c r="D45">
-        <f t="shared" si="1"/>
+        <f>C45*B45</f>
         <v>50</v>
       </c>
-      <c r="F45">
-        <v>34</v>
-      </c>
       <c r="G45">
-        <v>118000</v>
+        <v>12200</v>
       </c>
       <c r="H45">
-        <v>250</v>
+        <v>150</v>
       </c>
       <c r="I45">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="J45" s="3" t="s">
-        <v>588</v>
-      </c>
-    </row>
-    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="46" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="B46">
         <v>5</v>
@@ -9317,73 +9224,91 @@
         <v>10</v>
       </c>
       <c r="D46">
-        <f t="shared" si="1"/>
+        <f>C46*B46</f>
         <v>50</v>
       </c>
-    </row>
-    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="F46">
+        <v>34</v>
+      </c>
+      <c r="G46">
+        <v>118000</v>
+      </c>
+      <c r="H46">
+        <v>250</v>
+      </c>
+      <c r="I46">
+        <v>200</v>
+      </c>
+      <c r="J46" s="3" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="47" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>590</v>
+        <v>570</v>
       </c>
       <c r="B47">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C47">
         <v>10</v>
       </c>
       <c r="D47">
-        <f t="shared" si="1"/>
-        <v>70</v>
+        <f>C47*B47</f>
+        <v>20</v>
       </c>
       <c r="F47">
+        <v>30</v>
+      </c>
+      <c r="G47">
+        <v>57000</v>
+      </c>
+      <c r="H47">
+        <v>200</v>
+      </c>
+      <c r="I47">
+        <v>120</v>
+      </c>
+      <c r="J47" s="3" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="48" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>511</v>
+      </c>
+      <c r="B48">
+        <v>2</v>
+      </c>
+      <c r="C48">
+        <v>10</v>
+      </c>
+      <c r="D48">
+        <f>C48*B48</f>
         <v>20</v>
       </c>
-      <c r="G47">
-        <v>206000</v>
-      </c>
-      <c r="H47">
-        <v>400</v>
-      </c>
-      <c r="I47">
-        <v>335</v>
-      </c>
-      <c r="J47" s="3" t="s">
-        <v>591</v>
-      </c>
-    </row>
-    <row r="48" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>592</v>
-      </c>
-      <c r="B48">
-        <v>7</v>
-      </c>
-      <c r="C48">
-        <v>10</v>
-      </c>
-      <c r="D48">
-        <f t="shared" si="1"/>
-        <v>70</v>
-      </c>
       <c r="F48">
-        <v>30</v>
+        <v>9</v>
       </c>
       <c r="G48">
-        <v>230000</v>
+        <v>10170</v>
       </c>
       <c r="H48">
-        <v>350</v>
+        <v>89</v>
       </c>
       <c r="I48">
-        <v>244</v>
+        <v>40</v>
       </c>
       <c r="J48" s="3" t="s">
-        <v>593</v>
+        <v>512</v>
+      </c>
+      <c r="T48" s="3" t="s">
+        <v>513</v>
       </c>
     </row>
     <row r="49" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>594</v>
+        <v>607</v>
       </c>
       <c r="B49">
         <v>7</v>
@@ -9392,40 +9317,40 @@
         <v>10</v>
       </c>
       <c r="D49">
-        <f t="shared" si="1"/>
+        <f>C49*B49</f>
         <v>70</v>
       </c>
     </row>
     <row r="50" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>595</v>
+        <v>572</v>
       </c>
       <c r="B50">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C50">
         <v>10</v>
       </c>
       <c r="D50">
-        <f t="shared" si="1"/>
-        <v>30</v>
+        <f>C50*B50</f>
+        <v>20</v>
       </c>
       <c r="F50">
-        <v>21</v>
+        <v>34</v>
+      </c>
+      <c r="G50">
+        <v>11300</v>
       </c>
       <c r="H50">
-        <v>110</v>
+        <v>91</v>
       </c>
       <c r="J50" s="3" t="s">
-        <v>596</v>
-      </c>
-      <c r="T50" s="3" t="s">
-        <v>597</v>
+        <v>573</v>
       </c>
     </row>
     <row r="51" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>598</v>
+        <v>527</v>
       </c>
       <c r="B51">
         <v>3</v>
@@ -9434,37 +9359,28 @@
         <v>10</v>
       </c>
       <c r="D51">
-        <f t="shared" si="1"/>
+        <f>C51*B51</f>
         <v>30</v>
-      </c>
-      <c r="F51">
-        <v>12</v>
-      </c>
-      <c r="H51">
-        <v>54</v>
-      </c>
-      <c r="J51" s="3" t="s">
-        <v>599</v>
       </c>
     </row>
     <row r="52" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>600</v>
+        <v>608</v>
       </c>
       <c r="B52">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C52">
         <v>10</v>
       </c>
       <c r="D52">
-        <f t="shared" si="1"/>
-        <v>30</v>
+        <f>C52*B52</f>
+        <v>70</v>
       </c>
     </row>
     <row r="53" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>601</v>
+        <v>558</v>
       </c>
       <c r="B53">
         <v>2</v>
@@ -9473,131 +9389,215 @@
         <v>10</v>
       </c>
       <c r="D53">
-        <f t="shared" si="1"/>
+        <f>C53*B53</f>
         <v>20</v>
+      </c>
+      <c r="F53">
+        <v>35</v>
+      </c>
+      <c r="G53">
+        <v>30000</v>
+      </c>
+      <c r="H53">
+        <v>125</v>
+      </c>
+      <c r="I53">
+        <v>90</v>
+      </c>
+      <c r="J53" s="3" t="s">
+        <v>559</v>
       </c>
     </row>
     <row r="54" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>602</v>
+        <v>503</v>
       </c>
       <c r="B54">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C54">
         <v>10</v>
       </c>
       <c r="D54">
-        <f t="shared" si="1"/>
-        <v>30</v>
+        <f>C54*B54</f>
+        <v>10</v>
+      </c>
+      <c r="F54">
+        <v>23</v>
+      </c>
+      <c r="G54">
+        <v>21000</v>
+      </c>
+      <c r="H54">
+        <v>133</v>
+      </c>
+      <c r="J54" s="3" t="s">
+        <v>504</v>
+      </c>
+      <c r="T54" s="3" t="s">
+        <v>505</v>
       </c>
     </row>
     <row r="55" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>603</v>
+        <v>514</v>
       </c>
       <c r="B55">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="C55">
         <v>10</v>
       </c>
       <c r="D55">
-        <f t="shared" si="1"/>
-        <v>80</v>
+        <f>C55*B55</f>
+        <v>20</v>
+      </c>
+      <c r="F55">
+        <v>14</v>
+      </c>
+      <c r="G55">
+        <v>3600</v>
+      </c>
+      <c r="H55">
+        <v>64</v>
+      </c>
+      <c r="J55" s="3" t="s">
+        <v>515</v>
       </c>
     </row>
     <row r="56" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>604</v>
+        <v>574</v>
       </c>
       <c r="B56">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="C56">
         <v>10</v>
       </c>
       <c r="D56">
-        <f t="shared" si="1"/>
-        <v>90</v>
-      </c>
-      <c r="F56">
-        <v>70</v>
+        <f>C56*B56</f>
+        <v>20</v>
       </c>
       <c r="G56">
-        <v>90</v>
+        <v>23600</v>
+      </c>
+      <c r="H56">
+        <v>150</v>
+      </c>
+      <c r="J56" s="3" t="s">
+        <v>575</v>
       </c>
     </row>
     <row r="57" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>605</v>
+        <v>508</v>
       </c>
       <c r="B57">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="C57">
         <v>10</v>
       </c>
       <c r="D57">
-        <f t="shared" si="1"/>
-        <v>90</v>
-      </c>
-      <c r="J57" s="4" t="s">
-        <v>606</v>
+        <f>C57*B57</f>
+        <v>20</v>
+      </c>
+      <c r="F57">
+        <v>7</v>
+      </c>
+      <c r="G57">
+        <v>910</v>
+      </c>
+      <c r="H57">
+        <v>46</v>
+      </c>
+      <c r="J57" s="3" t="s">
+        <v>509</v>
+      </c>
+      <c r="T57" s="3" t="s">
+        <v>510</v>
       </c>
     </row>
     <row r="58" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>607</v>
+        <v>595</v>
       </c>
       <c r="B58">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C58">
         <v>10</v>
       </c>
       <c r="D58">
-        <f t="shared" si="1"/>
-        <v>70</v>
+        <f>C58*B58</f>
+        <v>30</v>
+      </c>
+      <c r="F58">
+        <v>21</v>
+      </c>
+      <c r="H58">
+        <v>110</v>
+      </c>
+      <c r="J58" s="3" t="s">
+        <v>596</v>
+      </c>
+      <c r="T58" s="3" t="s">
+        <v>597</v>
       </c>
     </row>
     <row r="59" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>608</v>
+        <v>516</v>
       </c>
       <c r="B59">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C59">
         <v>10</v>
       </c>
       <c r="D59">
-        <f t="shared" si="1"/>
-        <v>70</v>
+        <f>C59*B59</f>
+        <v>20</v>
+      </c>
+      <c r="F59">
+        <v>25</v>
+      </c>
+      <c r="G59">
+        <v>2500</v>
+      </c>
+      <c r="H59">
+        <v>60</v>
+      </c>
+      <c r="J59" s="3" t="s">
+        <v>517</v>
       </c>
     </row>
     <row r="60" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>609</v>
+        <v>580</v>
       </c>
       <c r="B60">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C60">
         <v>10</v>
       </c>
       <c r="D60">
-        <f t="shared" si="1"/>
-        <v>20</v>
+        <f>C60*B60</f>
+        <v>10</v>
       </c>
       <c r="F60">
-        <v>10</v>
+        <v>14</v>
+      </c>
+      <c r="G60">
+        <v>1500</v>
       </c>
       <c r="H60">
-        <v>38</v>
+        <v>64</v>
       </c>
       <c r="J60" s="3" t="s">
-        <v>610</v>
+        <v>581</v>
       </c>
     </row>
     <row r="62" spans="1:20" x14ac:dyDescent="0.25">
@@ -9636,7 +9636,7 @@
         <v>10</v>
       </c>
       <c r="F64">
-        <f t="shared" ref="F64:F95" si="2">E64*D64</f>
+        <f t="shared" ref="F64:F95" si="0">E64*D64</f>
         <v>10</v>
       </c>
     </row>
@@ -9654,7 +9654,7 @@
         <v>10</v>
       </c>
       <c r="F65">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
     </row>
@@ -9672,7 +9672,7 @@
         <v>10</v>
       </c>
       <c r="F66">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
     </row>
@@ -9690,7 +9690,7 @@
         <v>10</v>
       </c>
       <c r="F67">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
     </row>
@@ -9708,7 +9708,7 @@
         <v>10</v>
       </c>
       <c r="F68">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
     </row>
@@ -9726,7 +9726,7 @@
         <v>10</v>
       </c>
       <c r="F69">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
     </row>
@@ -9744,7 +9744,7 @@
         <v>10</v>
       </c>
       <c r="F70">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
     </row>
@@ -9762,7 +9762,7 @@
         <v>10</v>
       </c>
       <c r="F71">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
     </row>
@@ -9780,7 +9780,7 @@
         <v>10</v>
       </c>
       <c r="F72">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
     </row>
@@ -9798,7 +9798,7 @@
         <v>10</v>
       </c>
       <c r="F73">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
     </row>
@@ -9816,7 +9816,7 @@
         <v>10</v>
       </c>
       <c r="F74">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
     </row>
@@ -9834,7 +9834,7 @@
         <v>10</v>
       </c>
       <c r="F75">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
     </row>
@@ -9852,7 +9852,7 @@
         <v>10</v>
       </c>
       <c r="F76">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>30</v>
       </c>
     </row>
@@ -9870,7 +9870,7 @@
         <v>10</v>
       </c>
       <c r="F77">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>30</v>
       </c>
     </row>
@@ -9888,7 +9888,7 @@
         <v>10</v>
       </c>
       <c r="F78">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>30</v>
       </c>
     </row>
@@ -9906,7 +9906,7 @@
         <v>10</v>
       </c>
       <c r="F79">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
     </row>
@@ -9924,7 +9924,7 @@
         <v>10</v>
       </c>
       <c r="F80">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
     </row>
@@ -9942,7 +9942,7 @@
         <v>10</v>
       </c>
       <c r="F81">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
     </row>
@@ -9960,7 +9960,7 @@
         <v>10</v>
       </c>
       <c r="F82">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
     </row>
@@ -9978,7 +9978,7 @@
         <v>10</v>
       </c>
       <c r="F83">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
     </row>
@@ -9996,7 +9996,7 @@
         <v>10</v>
       </c>
       <c r="F84">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
     </row>
@@ -10014,7 +10014,7 @@
         <v>10</v>
       </c>
       <c r="F85">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
     </row>
@@ -10032,7 +10032,7 @@
         <v>10</v>
       </c>
       <c r="F86">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
     </row>
@@ -10050,7 +10050,7 @@
         <v>10</v>
       </c>
       <c r="F87">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
     </row>
@@ -10068,7 +10068,7 @@
         <v>10</v>
       </c>
       <c r="F88">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
     </row>
@@ -10086,7 +10086,7 @@
         <v>10</v>
       </c>
       <c r="F89">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
     </row>
@@ -10104,7 +10104,7 @@
         <v>10</v>
       </c>
       <c r="F90">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
     </row>
@@ -10122,7 +10122,7 @@
         <v>10</v>
       </c>
       <c r="F91">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
     </row>
@@ -10140,7 +10140,7 @@
         <v>10</v>
       </c>
       <c r="F92">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
     </row>
@@ -10158,7 +10158,7 @@
         <v>10</v>
       </c>
       <c r="F93">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
     </row>
@@ -10176,7 +10176,7 @@
         <v>10</v>
       </c>
       <c r="F94">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
     </row>
@@ -10194,7 +10194,7 @@
         <v>10</v>
       </c>
       <c r="F95">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
     </row>
@@ -10212,7 +10212,7 @@
         <v>10</v>
       </c>
       <c r="F96">
-        <f t="shared" ref="F96:F127" si="3">E96*D96</f>
+        <f t="shared" ref="F96:F122" si="1">E96*D96</f>
         <v>20</v>
       </c>
     </row>
@@ -10230,7 +10230,7 @@
         <v>10</v>
       </c>
       <c r="F97">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
     </row>
@@ -10248,7 +10248,7 @@
         <v>10</v>
       </c>
       <c r="F98">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
     </row>
@@ -10266,7 +10266,7 @@
         <v>10</v>
       </c>
       <c r="F99">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
     </row>
@@ -10284,7 +10284,7 @@
         <v>10</v>
       </c>
       <c r="F100">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
     </row>
@@ -10302,7 +10302,7 @@
         <v>10</v>
       </c>
       <c r="F101">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
     </row>
@@ -10320,7 +10320,7 @@
         <v>10</v>
       </c>
       <c r="F102">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
     </row>
@@ -10338,7 +10338,7 @@
         <v>10</v>
       </c>
       <c r="F103">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
     </row>
@@ -10356,7 +10356,7 @@
         <v>10</v>
       </c>
       <c r="F104">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
     </row>
@@ -10374,7 +10374,7 @@
         <v>10</v>
       </c>
       <c r="F105">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>40</v>
       </c>
     </row>
@@ -10392,7 +10392,7 @@
         <v>10</v>
       </c>
       <c r="F106">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>50</v>
       </c>
     </row>
@@ -10410,7 +10410,7 @@
         <v>10</v>
       </c>
       <c r="F107">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>50</v>
       </c>
     </row>
@@ -10428,7 +10428,7 @@
         <v>10</v>
       </c>
       <c r="F108">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>50</v>
       </c>
     </row>
@@ -10446,7 +10446,7 @@
         <v>10</v>
       </c>
       <c r="F109">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>70</v>
       </c>
     </row>
@@ -10464,7 +10464,7 @@
         <v>10</v>
       </c>
       <c r="F110">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>70</v>
       </c>
     </row>
@@ -10482,7 +10482,7 @@
         <v>10</v>
       </c>
       <c r="F111">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>70</v>
       </c>
     </row>
@@ -10500,7 +10500,7 @@
         <v>10</v>
       </c>
       <c r="F112">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>30</v>
       </c>
     </row>
@@ -10518,7 +10518,7 @@
         <v>10</v>
       </c>
       <c r="F113">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>30</v>
       </c>
     </row>
@@ -10536,7 +10536,7 @@
         <v>10</v>
       </c>
       <c r="F114">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>30</v>
       </c>
     </row>
@@ -10554,7 +10554,7 @@
         <v>10</v>
       </c>
       <c r="F115">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
     </row>
@@ -10572,7 +10572,7 @@
         <v>10</v>
       </c>
       <c r="F116">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>30</v>
       </c>
     </row>
@@ -10590,7 +10590,7 @@
         <v>10</v>
       </c>
       <c r="F117">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>80</v>
       </c>
     </row>
@@ -10608,7 +10608,7 @@
         <v>10</v>
       </c>
       <c r="F118">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>90</v>
       </c>
     </row>
@@ -10626,7 +10626,7 @@
         <v>10</v>
       </c>
       <c r="F119">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>90</v>
       </c>
     </row>
@@ -10644,7 +10644,7 @@
         <v>10</v>
       </c>
       <c r="F120">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>70</v>
       </c>
     </row>
@@ -10662,7 +10662,7 @@
         <v>10</v>
       </c>
       <c r="F121">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>70</v>
       </c>
     </row>
@@ -10680,11 +10680,14 @@
         <v>10</v>
       </c>
       <c r="F122">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="A2:AA61">
+    <sortCondition ref="A2:A61"/>
+  </sortState>
   <conditionalFormatting sqref="H2:H60">
     <cfRule type="dataBar" priority="2">
       <dataBar>
@@ -10714,59 +10717,59 @@
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="J2" r:id="rId1"/>
-    <hyperlink ref="J3" r:id="rId2"/>
-    <hyperlink ref="J4" r:id="rId3"/>
-    <hyperlink ref="T4" r:id="rId4" location=".WylnwlVKhaQ"/>
+    <hyperlink ref="J25" r:id="rId1"/>
+    <hyperlink ref="J22" r:id="rId2"/>
+    <hyperlink ref="J54" r:id="rId3"/>
+    <hyperlink ref="T54" r:id="rId4" location=".WylnwlVKhaQ"/>
     <hyperlink ref="J5" r:id="rId5"/>
-    <hyperlink ref="J6" r:id="rId6"/>
-    <hyperlink ref="T6" r:id="rId7"/>
-    <hyperlink ref="J7" r:id="rId8"/>
-    <hyperlink ref="T7" r:id="rId9" location=".Wyln61VKhaQ"/>
-    <hyperlink ref="J8" r:id="rId10"/>
-    <hyperlink ref="J9" r:id="rId11"/>
-    <hyperlink ref="J10" r:id="rId12"/>
-    <hyperlink ref="J11" r:id="rId13"/>
-    <hyperlink ref="J12" r:id="rId14"/>
-    <hyperlink ref="J14" r:id="rId15"/>
-    <hyperlink ref="J18" r:id="rId16"/>
-    <hyperlink ref="T18" r:id="rId17"/>
-    <hyperlink ref="Z18" r:id="rId18"/>
-    <hyperlink ref="J19" r:id="rId19"/>
-    <hyperlink ref="T19" r:id="rId20"/>
-    <hyperlink ref="J21" r:id="rId21"/>
-    <hyperlink ref="J22" r:id="rId22"/>
-    <hyperlink ref="T22" r:id="rId23"/>
-    <hyperlink ref="J24" r:id="rId24"/>
-    <hyperlink ref="J25" r:id="rId25"/>
-    <hyperlink ref="J26" r:id="rId26"/>
-    <hyperlink ref="J27" r:id="rId27"/>
-    <hyperlink ref="J28" r:id="rId28"/>
-    <hyperlink ref="J29" r:id="rId29"/>
-    <hyperlink ref="J30" r:id="rId30"/>
-    <hyperlink ref="J31" r:id="rId31"/>
-    <hyperlink ref="J32" r:id="rId32"/>
-    <hyperlink ref="T32" r:id="rId33"/>
-    <hyperlink ref="AA32" r:id="rId34" location=".WylwQlVKhaQ"/>
-    <hyperlink ref="J33" r:id="rId35"/>
-    <hyperlink ref="J34" r:id="rId36"/>
-    <hyperlink ref="T35" r:id="rId37" location=".WylppFVKhaQ"/>
-    <hyperlink ref="J36" r:id="rId38"/>
-    <hyperlink ref="J37" r:id="rId39"/>
-    <hyperlink ref="J38" r:id="rId40"/>
-    <hyperlink ref="J41" r:id="rId41"/>
-    <hyperlink ref="J42" r:id="rId42"/>
-    <hyperlink ref="J43" r:id="rId43"/>
-    <hyperlink ref="T43" r:id="rId44"/>
-    <hyperlink ref="J44" r:id="rId45"/>
-    <hyperlink ref="J45" r:id="rId46"/>
-    <hyperlink ref="J47" r:id="rId47"/>
-    <hyperlink ref="J48" r:id="rId48"/>
-    <hyperlink ref="J50" r:id="rId49"/>
-    <hyperlink ref="T50" r:id="rId50"/>
-    <hyperlink ref="J51" r:id="rId51"/>
-    <hyperlink ref="J57" r:id="rId52"/>
-    <hyperlink ref="J60" r:id="rId53"/>
+    <hyperlink ref="J57" r:id="rId6"/>
+    <hyperlink ref="T57" r:id="rId7"/>
+    <hyperlink ref="J48" r:id="rId8"/>
+    <hyperlink ref="T48" r:id="rId9" location=".Wyln61VKhaQ"/>
+    <hyperlink ref="J55" r:id="rId10"/>
+    <hyperlink ref="J59" r:id="rId11"/>
+    <hyperlink ref="J21" r:id="rId12"/>
+    <hyperlink ref="J31" r:id="rId13"/>
+    <hyperlink ref="J18" r:id="rId14"/>
+    <hyperlink ref="J3" r:id="rId15"/>
+    <hyperlink ref="J9" r:id="rId16"/>
+    <hyperlink ref="T9" r:id="rId17"/>
+    <hyperlink ref="Z9" r:id="rId18"/>
+    <hyperlink ref="J2" r:id="rId19"/>
+    <hyperlink ref="T2" r:id="rId20"/>
+    <hyperlink ref="J19" r:id="rId21"/>
+    <hyperlink ref="J26" r:id="rId22"/>
+    <hyperlink ref="T26" r:id="rId23"/>
+    <hyperlink ref="J11" r:id="rId24"/>
+    <hyperlink ref="J43" r:id="rId25"/>
+    <hyperlink ref="J28" r:id="rId26"/>
+    <hyperlink ref="J32" r:id="rId27"/>
+    <hyperlink ref="J37" r:id="rId28"/>
+    <hyperlink ref="J8" r:id="rId29"/>
+    <hyperlink ref="J41" r:id="rId30"/>
+    <hyperlink ref="J53" r:id="rId31"/>
+    <hyperlink ref="J35" r:id="rId32"/>
+    <hyperlink ref="T35" r:id="rId33"/>
+    <hyperlink ref="AA35" r:id="rId34" location=".WylwQlVKhaQ"/>
+    <hyperlink ref="J29" r:id="rId35"/>
+    <hyperlink ref="J39" r:id="rId36"/>
+    <hyperlink ref="T13" r:id="rId37" location=".WylppFVKhaQ"/>
+    <hyperlink ref="J47" r:id="rId38"/>
+    <hyperlink ref="J50" r:id="rId39"/>
+    <hyperlink ref="J56" r:id="rId40"/>
+    <hyperlink ref="J20" r:id="rId41"/>
+    <hyperlink ref="J60" r:id="rId42"/>
+    <hyperlink ref="J12" r:id="rId43"/>
+    <hyperlink ref="T12" r:id="rId44"/>
+    <hyperlink ref="J45" r:id="rId45"/>
+    <hyperlink ref="J46" r:id="rId46"/>
+    <hyperlink ref="J6" r:id="rId47"/>
+    <hyperlink ref="J33" r:id="rId48"/>
+    <hyperlink ref="J58" r:id="rId49"/>
+    <hyperlink ref="T58" r:id="rId50"/>
+    <hyperlink ref="J24" r:id="rId51"/>
+    <hyperlink ref="J10" r:id="rId52"/>
+    <hyperlink ref="J23" r:id="rId53"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -12201,8 +12204,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T60"/>
   <sheetViews>
-    <sheetView windowProtection="1" tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="S20" sqref="S20"/>
+    <sheetView windowProtection="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O35" sqref="O35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
finishing fish von bertallanfy params
</commit_message>
<xml_diff>
--- a/R/C_and_Mum.xlsx
+++ b/R/C_and_Mum.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3169" uniqueCount="1062">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3259" uniqueCount="1063">
   <si>
     <t>C</t>
   </si>
@@ -3223,6 +3223,9 @@
   </si>
   <si>
     <t>Shallow_Demersal_Fish</t>
+  </si>
+  <si>
+    <t>NumAgeClassSize</t>
   </si>
 </sst>
 </file>
@@ -8090,13 +8093,13 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA122"/>
+  <dimension ref="A1:AA152"/>
   <sheetViews>
     <sheetView windowProtection="1" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B11" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B45" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A110" sqref="A110"/>
-      <selection pane="bottomRight" activeCell="J20" sqref="J20"/>
+      <selection pane="bottomRight" activeCell="M129" sqref="M129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8156,7 +8159,7 @@
         <v>10</v>
       </c>
       <c r="D2">
-        <f>C2*B2</f>
+        <f t="shared" ref="D2:D33" si="0">C2*B2</f>
         <v>10</v>
       </c>
       <c r="F2">
@@ -8189,7 +8192,7 @@
         <v>10</v>
       </c>
       <c r="D3">
-        <f>C3*B3</f>
+        <f t="shared" si="0"/>
         <v>30</v>
       </c>
       <c r="F3">
@@ -8219,7 +8222,7 @@
         <v>10</v>
       </c>
       <c r="D4">
-        <f>C4*B4</f>
+        <f t="shared" si="0"/>
         <v>30</v>
       </c>
     </row>
@@ -8234,7 +8237,7 @@
         <v>10</v>
       </c>
       <c r="D5">
-        <f>C5*B5</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="F5">
@@ -8264,7 +8267,7 @@
         <v>10</v>
       </c>
       <c r="D6">
-        <f>C6*B6</f>
+        <f t="shared" si="0"/>
         <v>70</v>
       </c>
       <c r="F6">
@@ -8294,7 +8297,7 @@
         <v>10</v>
       </c>
       <c r="D7">
-        <f>C7*B7</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
     </row>
@@ -8309,7 +8312,7 @@
         <v>10</v>
       </c>
       <c r="D8">
-        <f>C8*B8</f>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="F8">
@@ -8339,7 +8342,7 @@
         <v>10</v>
       </c>
       <c r="D9">
-        <f>C9*B9</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="G9">
@@ -8372,7 +8375,7 @@
         <v>10</v>
       </c>
       <c r="D10">
-        <f>C10*B10</f>
+        <f t="shared" si="0"/>
         <v>90</v>
       </c>
       <c r="J10" s="4" t="s">
@@ -8390,7 +8393,7 @@
         <v>10</v>
       </c>
       <c r="D11">
-        <f>C11*B11</f>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="F11">
@@ -8420,7 +8423,7 @@
         <v>10</v>
       </c>
       <c r="D12">
-        <f>C12*B12</f>
+        <f t="shared" si="0"/>
         <v>40</v>
       </c>
       <c r="F12" s="2">
@@ -8453,7 +8456,7 @@
         <v>10</v>
       </c>
       <c r="D13">
-        <f>C13*B13</f>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="G13">
@@ -8477,7 +8480,7 @@
         <v>10</v>
       </c>
       <c r="D14">
-        <f>C14*B14</f>
+        <f t="shared" si="0"/>
         <v>50</v>
       </c>
     </row>
@@ -8492,7 +8495,7 @@
         <v>10</v>
       </c>
       <c r="D15">
-        <f>C15*B15</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
     </row>
@@ -8507,7 +8510,7 @@
         <v>10</v>
       </c>
       <c r="D16">
-        <f>C16*B16</f>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
     </row>
@@ -8522,7 +8525,7 @@
         <v>10</v>
       </c>
       <c r="D17">
-        <f>C17*B17</f>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
     </row>
@@ -8537,7 +8540,7 @@
         <v>10</v>
       </c>
       <c r="D18">
-        <f>C18*B18</f>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="G18">
@@ -8561,7 +8564,7 @@
         <v>10</v>
       </c>
       <c r="D19">
-        <f>C19*B19</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="F19">
@@ -8591,7 +8594,7 @@
         <v>10</v>
       </c>
       <c r="D20">
-        <f>C20*B20</f>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="F20">
@@ -8621,7 +8624,7 @@
         <v>10</v>
       </c>
       <c r="D21">
-        <f>C21*B21</f>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="F21">
@@ -8648,7 +8651,7 @@
         <v>10</v>
       </c>
       <c r="D22">
-        <f>C22*B22</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="F22">
@@ -8678,7 +8681,7 @@
         <v>10</v>
       </c>
       <c r="D23">
-        <f>C23*B23</f>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="F23">
@@ -8702,7 +8705,7 @@
         <v>10</v>
       </c>
       <c r="D24">
-        <f>C24*B24</f>
+        <f t="shared" si="0"/>
         <v>30</v>
       </c>
       <c r="F24">
@@ -8726,7 +8729,7 @@
         <v>10</v>
       </c>
       <c r="D25">
-        <f>C25*B25</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="F25">
@@ -8756,7 +8759,7 @@
         <v>10</v>
       </c>
       <c r="D26">
-        <f>C26*B26</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="G26">
@@ -8786,7 +8789,7 @@
         <v>10</v>
       </c>
       <c r="D27">
-        <f>C27*B27</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
     </row>
@@ -8801,7 +8804,7 @@
         <v>10</v>
       </c>
       <c r="D28">
-        <f>C28*B28</f>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="H28">
@@ -8825,7 +8828,7 @@
         <v>10</v>
       </c>
       <c r="D29">
-        <f>C29*B29</f>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="F29">
@@ -8852,7 +8855,7 @@
         <v>10</v>
       </c>
       <c r="D30">
-        <f>C30*B30</f>
+        <f t="shared" si="0"/>
         <v>30</v>
       </c>
     </row>
@@ -8867,7 +8870,7 @@
         <v>10</v>
       </c>
       <c r="D31">
-        <f>C31*B31</f>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="F31">
@@ -8894,7 +8897,7 @@
         <v>10</v>
       </c>
       <c r="D32">
-        <f>C32*B32</f>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="F32">
@@ -8924,7 +8927,7 @@
         <v>10</v>
       </c>
       <c r="D33">
-        <f>C33*B33</f>
+        <f t="shared" si="0"/>
         <v>70</v>
       </c>
       <c r="F33">
@@ -8954,7 +8957,7 @@
         <v>10</v>
       </c>
       <c r="D34">
-        <f>C34*B34</f>
+        <f t="shared" ref="D34:D65" si="1">C34*B34</f>
         <v>70</v>
       </c>
     </row>
@@ -8969,7 +8972,7 @@
         <v>10</v>
       </c>
       <c r="D35">
-        <f>C35*B35</f>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="F35">
@@ -9002,7 +9005,7 @@
         <v>10</v>
       </c>
       <c r="D36">
-        <f>C36*B36</f>
+        <f t="shared" si="1"/>
         <v>80</v>
       </c>
     </row>
@@ -9017,7 +9020,7 @@
         <v>10</v>
       </c>
       <c r="D37">
-        <f>C37*B37</f>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="G37">
@@ -9041,7 +9044,7 @@
         <v>10</v>
       </c>
       <c r="D38">
-        <f>C38*B38</f>
+        <f t="shared" si="1"/>
         <v>90</v>
       </c>
       <c r="F38">
@@ -9062,7 +9065,7 @@
         <v>10</v>
       </c>
       <c r="D39">
-        <f>C39*B39</f>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="F39">
@@ -9092,7 +9095,7 @@
         <v>10</v>
       </c>
       <c r="D40">
-        <f>C40*B40</f>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
     </row>
@@ -9107,7 +9110,7 @@
         <v>10</v>
       </c>
       <c r="D41">
-        <f>C41*B41</f>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="F41">
@@ -9137,7 +9140,7 @@
         <v>10</v>
       </c>
       <c r="D42">
-        <f>C42*B42</f>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
     </row>
@@ -9152,7 +9155,7 @@
         <v>10</v>
       </c>
       <c r="D43">
-        <f>C43*B43</f>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="F43">
@@ -9182,7 +9185,7 @@
         <v>10</v>
       </c>
       <c r="D44">
-        <f>C44*B44</f>
+        <f t="shared" si="1"/>
         <v>30</v>
       </c>
     </row>
@@ -9197,7 +9200,7 @@
         <v>10</v>
       </c>
       <c r="D45">
-        <f>C45*B45</f>
+        <f t="shared" si="1"/>
         <v>50</v>
       </c>
       <c r="G45">
@@ -9224,7 +9227,7 @@
         <v>10</v>
       </c>
       <c r="D46">
-        <f>C46*B46</f>
+        <f t="shared" si="1"/>
         <v>50</v>
       </c>
       <c r="F46">
@@ -9254,7 +9257,7 @@
         <v>10</v>
       </c>
       <c r="D47">
-        <f>C47*B47</f>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="F47">
@@ -9284,7 +9287,7 @@
         <v>10</v>
       </c>
       <c r="D48">
-        <f>C48*B48</f>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="F48">
@@ -9317,7 +9320,7 @@
         <v>10</v>
       </c>
       <c r="D49">
-        <f>C49*B49</f>
+        <f t="shared" si="1"/>
         <v>70</v>
       </c>
     </row>
@@ -9332,7 +9335,7 @@
         <v>10</v>
       </c>
       <c r="D50">
-        <f>C50*B50</f>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="F50">
@@ -9359,7 +9362,7 @@
         <v>10</v>
       </c>
       <c r="D51">
-        <f>C51*B51</f>
+        <f t="shared" si="1"/>
         <v>30</v>
       </c>
     </row>
@@ -9374,7 +9377,7 @@
         <v>10</v>
       </c>
       <c r="D52">
-        <f>C52*B52</f>
+        <f t="shared" si="1"/>
         <v>70</v>
       </c>
     </row>
@@ -9389,7 +9392,7 @@
         <v>10</v>
       </c>
       <c r="D53">
-        <f>C53*B53</f>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="F53">
@@ -9419,7 +9422,7 @@
         <v>10</v>
       </c>
       <c r="D54">
-        <f>C54*B54</f>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="F54">
@@ -9449,7 +9452,7 @@
         <v>10</v>
       </c>
       <c r="D55">
-        <f>C55*B55</f>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="F55">
@@ -9476,7 +9479,7 @@
         <v>10</v>
       </c>
       <c r="D56">
-        <f>C56*B56</f>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="G56">
@@ -9500,7 +9503,7 @@
         <v>10</v>
       </c>
       <c r="D57">
-        <f>C57*B57</f>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="F57">
@@ -9530,7 +9533,7 @@
         <v>10</v>
       </c>
       <c r="D58">
-        <f>C58*B58</f>
+        <f t="shared" si="1"/>
         <v>30</v>
       </c>
       <c r="F58">
@@ -9557,7 +9560,7 @@
         <v>10</v>
       </c>
       <c r="D59">
-        <f>C59*B59</f>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="F59">
@@ -9584,7 +9587,7 @@
         <v>10</v>
       </c>
       <c r="D60">
-        <f>C60*B60</f>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="F60">
@@ -9621,6 +9624,9 @@
       <c r="F63" t="s">
         <v>492</v>
       </c>
+      <c r="I63" t="s">
+        <v>1062</v>
+      </c>
     </row>
     <row r="64" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
@@ -9636,11 +9642,21 @@
         <v>10</v>
       </c>
       <c r="F64">
-        <f t="shared" ref="F64:F95" si="0">E64*D64</f>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" ref="F64:F95" si="2">E64*D64</f>
+        <v>10</v>
+      </c>
+      <c r="H64" t="s">
+        <v>172</v>
+      </c>
+      <c r="I64">
+        <v>1</v>
+      </c>
+      <c r="K64" t="b">
+        <f>I64=D64</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>616</v>
       </c>
@@ -9654,11 +9670,21 @@
         <v>10</v>
       </c>
       <c r="F65">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="H65" t="s">
+        <v>175</v>
+      </c>
+      <c r="I65">
+        <v>1</v>
+      </c>
+      <c r="K65" t="b">
+        <f t="shared" ref="K65:K128" si="3">I65=D65</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>617</v>
       </c>
@@ -9672,11 +9698,21 @@
         <v>10</v>
       </c>
       <c r="F66">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="H66" t="s">
+        <v>177</v>
+      </c>
+      <c r="I66">
+        <v>1</v>
+      </c>
+      <c r="K66" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>618</v>
       </c>
@@ -9690,11 +9726,21 @@
         <v>10</v>
       </c>
       <c r="F67">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="H67" t="s">
+        <v>179</v>
+      </c>
+      <c r="I67">
+        <v>1</v>
+      </c>
+      <c r="K67" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>619</v>
       </c>
@@ -9708,11 +9754,21 @@
         <v>10</v>
       </c>
       <c r="F68">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>20</v>
       </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H68" t="s">
+        <v>181</v>
+      </c>
+      <c r="I68">
+        <v>2</v>
+      </c>
+      <c r="K68" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>620</v>
       </c>
@@ -9726,11 +9782,21 @@
         <v>10</v>
       </c>
       <c r="F69">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>20</v>
       </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H69" t="s">
+        <v>183</v>
+      </c>
+      <c r="I69">
+        <v>2</v>
+      </c>
+      <c r="K69" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>621</v>
       </c>
@@ -9744,11 +9810,21 @@
         <v>10</v>
       </c>
       <c r="F70">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>20</v>
       </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H70" t="s">
+        <v>185</v>
+      </c>
+      <c r="I70">
+        <v>2</v>
+      </c>
+      <c r="K70" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>622</v>
       </c>
@@ -9762,11 +9838,21 @@
         <v>10</v>
       </c>
       <c r="F71">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>20</v>
       </c>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H71" t="s">
+        <v>187</v>
+      </c>
+      <c r="I71">
+        <v>2</v>
+      </c>
+      <c r="K71" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>623</v>
       </c>
@@ -9780,11 +9866,21 @@
         <v>10</v>
       </c>
       <c r="F72">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>20</v>
       </c>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H72" t="s">
+        <v>189</v>
+      </c>
+      <c r="I72">
+        <v>2</v>
+      </c>
+      <c r="K72" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>624</v>
       </c>
@@ -9798,11 +9894,21 @@
         <v>10</v>
       </c>
       <c r="F73">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>20</v>
       </c>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H73" t="s">
+        <v>191</v>
+      </c>
+      <c r="I73">
+        <v>2</v>
+      </c>
+      <c r="K73" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>625</v>
       </c>
@@ -9816,11 +9922,21 @@
         <v>10</v>
       </c>
       <c r="F74">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>20</v>
       </c>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H74" t="s">
+        <v>193</v>
+      </c>
+      <c r="I74">
+        <v>2</v>
+      </c>
+      <c r="K74" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>626</v>
       </c>
@@ -9834,11 +9950,21 @@
         <v>10</v>
       </c>
       <c r="F75">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>20</v>
       </c>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H75" t="s">
+        <v>195</v>
+      </c>
+      <c r="I75">
+        <v>2</v>
+      </c>
+      <c r="K75" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>627</v>
       </c>
@@ -9852,11 +9978,21 @@
         <v>10</v>
       </c>
       <c r="F76">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>30</v>
       </c>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H76" t="s">
+        <v>197</v>
+      </c>
+      <c r="I76">
+        <v>3</v>
+      </c>
+      <c r="K76" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>628</v>
       </c>
@@ -9870,11 +10006,21 @@
         <v>10</v>
       </c>
       <c r="F77">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>30</v>
       </c>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H77" t="s">
+        <v>199</v>
+      </c>
+      <c r="I77">
+        <v>3</v>
+      </c>
+      <c r="K77" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>629</v>
       </c>
@@ -9888,11 +10034,21 @@
         <v>10</v>
       </c>
       <c r="F78">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>30</v>
       </c>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H78" t="s">
+        <v>201</v>
+      </c>
+      <c r="I78">
+        <v>3</v>
+      </c>
+      <c r="K78" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>630</v>
       </c>
@@ -9906,11 +10062,21 @@
         <v>10</v>
       </c>
       <c r="F79">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="H79" t="s">
+        <v>203</v>
+      </c>
+      <c r="I79">
+        <v>1</v>
+      </c>
+      <c r="K79" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>631</v>
       </c>
@@ -9924,11 +10090,21 @@
         <v>10</v>
       </c>
       <c r="F80">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="H80" t="s">
+        <v>205</v>
+      </c>
+      <c r="I80">
+        <v>1</v>
+      </c>
+      <c r="K80" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>632</v>
       </c>
@@ -9942,11 +10118,21 @@
         <v>10</v>
       </c>
       <c r="F81">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="H81" t="s">
+        <v>207</v>
+      </c>
+      <c r="I81">
+        <v>1</v>
+      </c>
+      <c r="K81" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>633</v>
       </c>
@@ -9960,11 +10146,21 @@
         <v>10</v>
       </c>
       <c r="F82">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="H82" t="s">
+        <v>209</v>
+      </c>
+      <c r="I82">
+        <v>1</v>
+      </c>
+      <c r="K82" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>634</v>
       </c>
@@ -9978,11 +10174,21 @@
         <v>10</v>
       </c>
       <c r="F83">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="H83" t="s">
+        <v>211</v>
+      </c>
+      <c r="I83">
+        <v>1</v>
+      </c>
+      <c r="K83" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>635</v>
       </c>
@@ -9996,11 +10202,21 @@
         <v>10</v>
       </c>
       <c r="F84">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="H84" t="s">
+        <v>213</v>
+      </c>
+      <c r="I84">
+        <v>1</v>
+      </c>
+      <c r="K84" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>636</v>
       </c>
@@ -10014,11 +10230,21 @@
         <v>10</v>
       </c>
       <c r="F85">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="H85" t="s">
+        <v>29</v>
+      </c>
+      <c r="I85">
+        <v>1</v>
+      </c>
+      <c r="K85" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>637</v>
       </c>
@@ -10032,11 +10258,21 @@
         <v>10</v>
       </c>
       <c r="F86">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>20</v>
       </c>
-    </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H86" t="s">
+        <v>215</v>
+      </c>
+      <c r="I86">
+        <v>2</v>
+      </c>
+      <c r="K86" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>638</v>
       </c>
@@ -10050,11 +10286,21 @@
         <v>10</v>
       </c>
       <c r="F87">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="H87" t="s">
+        <v>217</v>
+      </c>
+      <c r="I87">
+        <v>1</v>
+      </c>
+      <c r="K87" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>639</v>
       </c>
@@ -10068,11 +10314,21 @@
         <v>10</v>
       </c>
       <c r="F88">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>20</v>
       </c>
-    </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H88" t="s">
+        <v>219</v>
+      </c>
+      <c r="I88">
+        <v>2</v>
+      </c>
+      <c r="K88" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>640</v>
       </c>
@@ -10086,11 +10342,21 @@
         <v>10</v>
       </c>
       <c r="F89">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>20</v>
       </c>
-    </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H89" t="s">
+        <v>221</v>
+      </c>
+      <c r="I89">
+        <v>2</v>
+      </c>
+      <c r="K89" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>641</v>
       </c>
@@ -10104,11 +10370,21 @@
         <v>10</v>
       </c>
       <c r="F90">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>20</v>
       </c>
-    </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H90" t="s">
+        <v>223</v>
+      </c>
+      <c r="I90">
+        <v>2</v>
+      </c>
+      <c r="K90" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>642</v>
       </c>
@@ -10122,11 +10398,21 @@
         <v>10</v>
       </c>
       <c r="F91">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>20</v>
       </c>
-    </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H91" t="s">
+        <v>225</v>
+      </c>
+      <c r="I91">
+        <v>2</v>
+      </c>
+      <c r="K91" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>643</v>
       </c>
@@ -10140,11 +10426,21 @@
         <v>10</v>
       </c>
       <c r="F92">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>20</v>
       </c>
-    </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H92" t="s">
+        <v>227</v>
+      </c>
+      <c r="I92">
+        <v>2</v>
+      </c>
+      <c r="K92" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>644</v>
       </c>
@@ -10158,11 +10454,21 @@
         <v>10</v>
       </c>
       <c r="F93">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>20</v>
       </c>
-    </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H93" t="s">
+        <v>229</v>
+      </c>
+      <c r="I93">
+        <v>2</v>
+      </c>
+      <c r="K93" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>645</v>
       </c>
@@ -10176,11 +10482,21 @@
         <v>10</v>
       </c>
       <c r="F94">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>20</v>
       </c>
-    </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H94" t="s">
+        <v>231</v>
+      </c>
+      <c r="I94">
+        <v>2</v>
+      </c>
+      <c r="K94" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>646</v>
       </c>
@@ -10194,11 +10510,21 @@
         <v>10</v>
       </c>
       <c r="F95">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>20</v>
       </c>
-    </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H95" t="s">
+        <v>233</v>
+      </c>
+      <c r="I95">
+        <v>2</v>
+      </c>
+      <c r="K95" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>647</v>
       </c>
@@ -10212,11 +10538,21 @@
         <v>10</v>
       </c>
       <c r="F96">
-        <f t="shared" ref="F96:F122" si="1">E96*D96</f>
+        <f t="shared" ref="F96:F122" si="4">E96*D96</f>
         <v>20</v>
       </c>
-    </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H96" t="s">
+        <v>235</v>
+      </c>
+      <c r="I96">
+        <v>2</v>
+      </c>
+      <c r="K96" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>648</v>
       </c>
@@ -10230,11 +10566,21 @@
         <v>10</v>
       </c>
       <c r="F97">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>20</v>
       </c>
-    </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H97" t="s">
+        <v>237</v>
+      </c>
+      <c r="I97">
+        <v>2</v>
+      </c>
+      <c r="K97" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>649</v>
       </c>
@@ -10248,11 +10594,21 @@
         <v>10</v>
       </c>
       <c r="F98">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>20</v>
       </c>
-    </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H98" t="s">
+        <v>239</v>
+      </c>
+      <c r="I98">
+        <v>2</v>
+      </c>
+      <c r="K98" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>650</v>
       </c>
@@ -10266,11 +10622,21 @@
         <v>10</v>
       </c>
       <c r="F99">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>20</v>
       </c>
-    </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H99" t="s">
+        <v>241</v>
+      </c>
+      <c r="I99">
+        <v>2</v>
+      </c>
+      <c r="K99" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>651</v>
       </c>
@@ -10284,11 +10650,21 @@
         <v>10</v>
       </c>
       <c r="F100">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>20</v>
       </c>
-    </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H100" t="s">
+        <v>243</v>
+      </c>
+      <c r="I100">
+        <v>2</v>
+      </c>
+      <c r="K100" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>652</v>
       </c>
@@ -10302,11 +10678,21 @@
         <v>10</v>
       </c>
       <c r="F101">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>20</v>
       </c>
-    </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H101" t="s">
+        <v>245</v>
+      </c>
+      <c r="I101">
+        <v>2</v>
+      </c>
+      <c r="K101" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>653</v>
       </c>
@@ -10320,11 +10706,21 @@
         <v>10</v>
       </c>
       <c r="F102">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>20</v>
       </c>
-    </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H102" t="s">
+        <v>43</v>
+      </c>
+      <c r="I102">
+        <v>2</v>
+      </c>
+      <c r="K102" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>654</v>
       </c>
@@ -10338,11 +10734,21 @@
         <v>10</v>
       </c>
       <c r="F103">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>20</v>
       </c>
-    </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H103" t="s">
+        <v>247</v>
+      </c>
+      <c r="I103">
+        <v>2</v>
+      </c>
+      <c r="K103" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>655</v>
       </c>
@@ -10356,11 +10762,21 @@
         <v>10</v>
       </c>
       <c r="F104">
-        <f t="shared" si="1"/>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>10</v>
+      </c>
+      <c r="H104" t="s">
+        <v>249</v>
+      </c>
+      <c r="I104">
+        <v>1</v>
+      </c>
+      <c r="K104" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>656</v>
       </c>
@@ -10374,11 +10790,21 @@
         <v>10</v>
       </c>
       <c r="F105">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>40</v>
       </c>
-    </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H105" t="s">
+        <v>251</v>
+      </c>
+      <c r="I105">
+        <v>4</v>
+      </c>
+      <c r="K105" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>657</v>
       </c>
@@ -10392,11 +10818,21 @@
         <v>10</v>
       </c>
       <c r="F106">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>50</v>
       </c>
-    </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H106" t="s">
+        <v>254</v>
+      </c>
+      <c r="I106">
+        <v>5</v>
+      </c>
+      <c r="K106" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>658</v>
       </c>
@@ -10410,11 +10846,21 @@
         <v>10</v>
       </c>
       <c r="F107">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>50</v>
       </c>
-    </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H107" t="s">
+        <v>256</v>
+      </c>
+      <c r="I107">
+        <v>5</v>
+      </c>
+      <c r="K107" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>659</v>
       </c>
@@ -10428,11 +10874,21 @@
         <v>10</v>
       </c>
       <c r="F108">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>50</v>
       </c>
-    </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H108" t="s">
+        <v>258</v>
+      </c>
+      <c r="I108">
+        <v>5</v>
+      </c>
+      <c r="K108" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>660</v>
       </c>
@@ -10446,11 +10902,21 @@
         <v>10</v>
       </c>
       <c r="F109">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>70</v>
       </c>
-    </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H109" t="s">
+        <v>259</v>
+      </c>
+      <c r="I109">
+        <v>7</v>
+      </c>
+      <c r="K109" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>661</v>
       </c>
@@ -10464,11 +10930,21 @@
         <v>10</v>
       </c>
       <c r="F110">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>70</v>
       </c>
-    </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H110" t="s">
+        <v>261</v>
+      </c>
+      <c r="I110">
+        <v>7</v>
+      </c>
+      <c r="K110" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>662</v>
       </c>
@@ -10482,11 +10958,21 @@
         <v>10</v>
       </c>
       <c r="F111">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>70</v>
       </c>
-    </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H111" t="s">
+        <v>263</v>
+      </c>
+      <c r="I111">
+        <v>7</v>
+      </c>
+      <c r="K111" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>663</v>
       </c>
@@ -10500,11 +10986,21 @@
         <v>10</v>
       </c>
       <c r="F112">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>30</v>
       </c>
-    </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H112" t="s">
+        <v>265</v>
+      </c>
+      <c r="I112">
+        <v>3</v>
+      </c>
+      <c r="K112" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="113" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>664</v>
       </c>
@@ -10518,11 +11014,21 @@
         <v>10</v>
       </c>
       <c r="F113">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>30</v>
       </c>
-    </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H113" t="s">
+        <v>267</v>
+      </c>
+      <c r="I113">
+        <v>3</v>
+      </c>
+      <c r="K113" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>665</v>
       </c>
@@ -10536,11 +11042,21 @@
         <v>10</v>
       </c>
       <c r="F114">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>30</v>
       </c>
-    </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H114" t="s">
+        <v>269</v>
+      </c>
+      <c r="I114">
+        <v>3</v>
+      </c>
+      <c r="K114" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="115" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>666</v>
       </c>
@@ -10554,11 +11070,21 @@
         <v>10</v>
       </c>
       <c r="F115">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>20</v>
       </c>
-    </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H115" t="s">
+        <v>57</v>
+      </c>
+      <c r="I115">
+        <v>2</v>
+      </c>
+      <c r="K115" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="116" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>667</v>
       </c>
@@ -10572,11 +11098,21 @@
         <v>10</v>
       </c>
       <c r="F116">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>30</v>
       </c>
-    </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H116" t="s">
+        <v>61</v>
+      </c>
+      <c r="I116">
+        <v>3</v>
+      </c>
+      <c r="K116" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="117" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>668</v>
       </c>
@@ -10590,11 +11126,21 @@
         <v>10</v>
       </c>
       <c r="F117">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>80</v>
       </c>
-    </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H117" t="s">
+        <v>63</v>
+      </c>
+      <c r="I117">
+        <v>8</v>
+      </c>
+      <c r="K117" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="118" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>669</v>
       </c>
@@ -10608,11 +11154,21 @@
         <v>10</v>
       </c>
       <c r="F118">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>90</v>
       </c>
-    </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H118" t="s">
+        <v>274</v>
+      </c>
+      <c r="I118">
+        <v>9</v>
+      </c>
+      <c r="K118" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="119" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>670</v>
       </c>
@@ -10626,11 +11182,21 @@
         <v>10</v>
       </c>
       <c r="F119">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>90</v>
       </c>
-    </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H119" t="s">
+        <v>276</v>
+      </c>
+      <c r="I119">
+        <v>9</v>
+      </c>
+      <c r="K119" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="120" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>671</v>
       </c>
@@ -10644,11 +11210,21 @@
         <v>10</v>
       </c>
       <c r="F120">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>70</v>
       </c>
-    </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H120" t="s">
+        <v>277</v>
+      </c>
+      <c r="I120">
+        <v>7</v>
+      </c>
+      <c r="K120" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="121" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>672</v>
       </c>
@@ -10662,11 +11238,21 @@
         <v>10</v>
       </c>
       <c r="F121">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>70</v>
       </c>
-    </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H121" t="s">
+        <v>278</v>
+      </c>
+      <c r="I121">
+        <v>7</v>
+      </c>
+      <c r="K121" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="122" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>673</v>
       </c>
@@ -10680,8 +11266,378 @@
         <v>10</v>
       </c>
       <c r="F122">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>20</v>
+      </c>
+      <c r="H122" t="s">
+        <v>279</v>
+      </c>
+      <c r="I122">
+        <v>2</v>
+      </c>
+      <c r="K122" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="123" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H123" t="s">
+        <v>281</v>
+      </c>
+      <c r="I123">
+        <v>1</v>
+      </c>
+      <c r="K123" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H124" t="s">
+        <v>283</v>
+      </c>
+      <c r="I124">
+        <v>1</v>
+      </c>
+      <c r="K124" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H125" t="s">
+        <v>285</v>
+      </c>
+      <c r="I125">
+        <v>1</v>
+      </c>
+      <c r="K125" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H126" t="s">
+        <v>287</v>
+      </c>
+      <c r="I126">
+        <v>1</v>
+      </c>
+      <c r="K126" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H127" t="s">
+        <v>289</v>
+      </c>
+      <c r="I127">
+        <v>1</v>
+      </c>
+      <c r="K127" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H128" t="s">
+        <v>78</v>
+      </c>
+      <c r="I128">
+        <v>1</v>
+      </c>
+      <c r="K128" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H129" t="s">
+        <v>82</v>
+      </c>
+      <c r="I129">
+        <v>1</v>
+      </c>
+      <c r="K129" t="b">
+        <f t="shared" ref="K129:K152" si="5">I129=D129</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H130" t="s">
+        <v>291</v>
+      </c>
+      <c r="I130">
+        <v>1</v>
+      </c>
+      <c r="K130" t="b">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H131" t="s">
+        <v>293</v>
+      </c>
+      <c r="I131">
+        <v>1</v>
+      </c>
+      <c r="K131" t="b">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H132" t="s">
+        <v>90</v>
+      </c>
+      <c r="I132">
+        <v>1</v>
+      </c>
+      <c r="K132" t="b">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="133" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H133" t="s">
+        <v>295</v>
+      </c>
+      <c r="I133">
+        <v>1</v>
+      </c>
+      <c r="K133" t="b">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="134" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H134" t="s">
+        <v>297</v>
+      </c>
+      <c r="I134">
+        <v>1</v>
+      </c>
+      <c r="K134" t="b">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="135" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H135" t="s">
+        <v>94</v>
+      </c>
+      <c r="I135">
+        <v>1</v>
+      </c>
+      <c r="K135" t="b">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H136" t="s">
+        <v>97</v>
+      </c>
+      <c r="I136">
+        <v>1</v>
+      </c>
+      <c r="K136" t="b">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="137" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H137" t="s">
+        <v>100</v>
+      </c>
+      <c r="I137">
+        <v>1</v>
+      </c>
+      <c r="K137" t="b">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="138" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H138" t="s">
+        <v>103</v>
+      </c>
+      <c r="I138">
+        <v>1</v>
+      </c>
+      <c r="K138" t="b">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="139" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H139" t="s">
+        <v>105</v>
+      </c>
+      <c r="I139">
+        <v>1</v>
+      </c>
+      <c r="K139" t="b">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="140" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H140" t="s">
+        <v>107</v>
+      </c>
+      <c r="I140">
+        <v>1</v>
+      </c>
+      <c r="K140" t="b">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="141" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H141" t="s">
+        <v>109</v>
+      </c>
+      <c r="I141">
+        <v>1</v>
+      </c>
+      <c r="K141" t="b">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="142" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H142" t="s">
+        <v>111</v>
+      </c>
+      <c r="I142">
+        <v>1</v>
+      </c>
+      <c r="K142" t="b">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="143" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H143" t="s">
+        <v>114</v>
+      </c>
+      <c r="I143">
+        <v>1</v>
+      </c>
+      <c r="K143" t="b">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="144" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H144" t="s">
+        <v>116</v>
+      </c>
+      <c r="I144">
+        <v>1</v>
+      </c>
+      <c r="K144" t="b">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="145" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H145" t="s">
+        <v>119</v>
+      </c>
+      <c r="I145">
+        <v>1</v>
+      </c>
+      <c r="K145" t="b">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="146" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H146" t="s">
+        <v>121</v>
+      </c>
+      <c r="I146">
+        <v>1</v>
+      </c>
+      <c r="K146" t="b">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="147" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H147" t="s">
+        <v>124</v>
+      </c>
+      <c r="I147">
+        <v>1</v>
+      </c>
+      <c r="K147" t="b">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="148" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H148" t="s">
+        <v>127</v>
+      </c>
+      <c r="I148">
+        <v>1</v>
+      </c>
+      <c r="K148" t="b">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="149" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H149" t="s">
+        <v>130</v>
+      </c>
+      <c r="I149">
+        <v>1</v>
+      </c>
+      <c r="K149" t="b">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="150" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H150" t="s">
+        <v>133</v>
+      </c>
+      <c r="I150">
+        <v>1</v>
+      </c>
+      <c r="K150" t="b">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="151" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H151" t="s">
+        <v>136</v>
+      </c>
+      <c r="I151">
+        <v>1</v>
+      </c>
+      <c r="K151" t="b">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="152" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H152" t="s">
+        <v>139</v>
+      </c>
+      <c r="I152">
+        <v>1</v>
+      </c>
+      <c r="K152" t="b">
+        <f t="shared" si="5"/>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -12202,16 +13158,19 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T60"/>
+  <dimension ref="A1:T65"/>
   <sheetViews>
-    <sheetView windowProtection="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O35" sqref="O35"/>
+    <sheetView windowProtection="1" topLeftCell="A23" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.28515625"/>
-    <col min="2" max="14" width="10.85546875"/>
+    <col min="2" max="7" width="10.85546875"/>
+    <col min="8" max="8" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="14" width="10.85546875"/>
     <col min="15" max="20" width="10.85546875" style="5"/>
     <col min="21" max="1025" width="10.85546875"/>
   </cols>
@@ -13691,7 +14650,7 @@
         <v>200</v>
       </c>
       <c r="K36">
-        <f t="shared" si="2"/>
+        <f>C36*(I36^F36)</f>
         <v>57457.512220481469</v>
       </c>
       <c r="L36">
@@ -14482,24 +15441,29 @@
         <v>960</v>
       </c>
       <c r="C56">
-        <v>0.2</v>
+        <v>1E-4</v>
       </c>
       <c r="E56" t="s">
         <v>961</v>
       </c>
       <c r="F56">
-        <v>3</v>
+        <v>2.81</v>
       </c>
       <c r="H56">
-        <v>90</v>
+        <f>70*907187</f>
+        <v>63503090</v>
+      </c>
+      <c r="I56">
+        <f>52*0.3048*1000</f>
+        <v>15849.6</v>
       </c>
       <c r="K56">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f>C56*(I56^F56)</f>
+        <v>63394479.542280264</v>
       </c>
       <c r="L56">
         <f t="shared" si="3"/>
-        <v>7.6630943239355291</v>
+        <v>15859.258122628285</v>
       </c>
       <c r="O56" s="5" t="s">
         <v>960</v>
@@ -14663,6 +15627,26 @@
       </c>
       <c r="S60" s="5">
         <v>3.1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="K64">
+        <f>K56-H56</f>
+        <v>-108610.4577197358</v>
+      </c>
+      <c r="L64">
+        <f>L56-I56</f>
+        <v>9.6581226282851276</v>
+      </c>
+    </row>
+    <row r="65" spans="11:12" x14ac:dyDescent="0.25">
+      <c r="K65">
+        <f>K64/K56</f>
+        <v>-1.7132478806344523E-3</v>
+      </c>
+      <c r="L65">
+        <f>L64/L56</f>
+        <v>6.0898956014245954E-4</v>
       </c>
     </row>
   </sheetData>
@@ -14680,10 +15664,10 @@
   <dimension ref="A1:W581"/>
   <sheetViews>
     <sheetView windowProtection="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B183" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B275" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A192" sqref="A1:A1048576"/>
+      <selection pane="bottomRight" activeCell="L214" sqref="L214"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>